<commit_message>
Viaticos_q_Plan de proyecto (actualizacion)
</commit_message>
<xml_diff>
--- a/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/2. Plantillas planeacion/Viaticos_q_Plan_Proyecto.xlsx
+++ b/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/2. Plantillas planeacion/Viaticos_q_Plan_Proyecto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="875" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="875" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Generales" sheetId="23" r:id="rId1"/>
@@ -538,7 +538,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="311">
   <si>
     <t>Nombre</t>
   </si>
@@ -1387,43 +1387,6 @@
     <t>Final del proyecto</t>
   </si>
   <si>
-    <t>Personal capaz de desarrollar plataformas web</t>
-  </si>
-  <si>
-    <t>Personal enfocado en la programacion de plataformas web sin importar el lenguaje que se utilice</t>
-  </si>
-  <si>
-    <t>Personal capacitado para el control y monitoreo de los procesos</t>
-  </si>
-  <si>
-    <t>Contar con los conocimientos suficientes para poder auditar una ejecucion de calidad del proyecto en CMMI DEV nivel 3</t>
-  </si>
-  <si>
-    <t>Puntualidad</t>
-  </si>
-  <si>
-    <t>El personal debera respetar el horario designado al proyecto y cumplir con un total de horas de trabajo</t>
-  </si>
-  <si>
-    <t>Cumplir con las metas diarias propuestas por direccion</t>
-  </si>
-  <si>
-    <t>Ejecutar las metas diarias sin importar el tiempo que este conlleve realizarlas, para si llevar un control del avance del proyecto</t>
-  </si>
-  <si>
-    <t>Informar el avance realizado por dia en el area en la que se encuentran activos en el proyecto, esto con la finalidad de apoyar el control y ejecucion del proyecto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apoyar al personal con el control del avance del proyecto en el area que les pertence
-</t>
-  </si>
-  <si>
-    <t>Respeto</t>
-  </si>
-  <si>
-    <t>Respeto mutuo entre compa~eros de trabajo</t>
-  </si>
-  <si>
     <t>Documento "Manual de requerimientos"</t>
   </si>
   <si>
@@ -1443,6 +1406,75 @@
   </si>
   <si>
     <t>Evaluacion honesta de los productos</t>
+  </si>
+  <si>
+    <t>Disponibilidad de personal</t>
+  </si>
+  <si>
+    <t>Cada empleado de la organizacion puede estar asignado a varios puestos dentro del proyecto y participar en maximo dos proyectos</t>
+  </si>
+  <si>
+    <t>Capacidades del personal</t>
+  </si>
+  <si>
+    <t>Antes de asignar persona a los proyectos, se tiene que analizar el perfil de los empleados verificando asi el perfil adecuado para desarrollar el proyecto</t>
+  </si>
+  <si>
+    <t>Agenda por empleado</t>
+  </si>
+  <si>
+    <t>Cada empleado debe tener asignada una agenda con los horarios que tiene para proyecto en el que se encuentra o area de proceso</t>
+  </si>
+  <si>
+    <t>Trabajo de oficina desde casa</t>
+  </si>
+  <si>
+    <t>Llegar tarde a la oficina (puntualidad)</t>
+  </si>
+  <si>
+    <t>No se podra llegar despues de las 9:15 a.m en caso de que existan juntas con el cliente, juntas de la organizacion o capacitaciones previamente agendadas.</t>
+  </si>
+  <si>
+    <t>Musica sin audifonos</t>
+  </si>
+  <si>
+    <t>No esta permitido escuchar musica a un volumen inapropiado si se encuentra dentro de la jornada laboral</t>
+  </si>
+  <si>
+    <t>Actividades recreativas</t>
+  </si>
+  <si>
+    <t>No se debe de exceder un rango de 10 minutos en actividades recreativas dentro de la oficina durante la jornada laboral o cuando se este utilizando el telefono de la empresa</t>
+  </si>
+  <si>
+    <t>Hora de comida</t>
+  </si>
+  <si>
+    <t>El tiempo maximo para la hora de comida es de 1:30 horas. Esta puede tomarse a la hora que el empleado prefiera</t>
+  </si>
+  <si>
+    <t>Proyectos ajenos a la empresa</t>
+  </si>
+  <si>
+    <t>En jornada laboral no esta permitido realizar actividades de proyecto ajenos a la empresa</t>
+  </si>
+  <si>
+    <t>Vacaciones</t>
+  </si>
+  <si>
+    <t>Las vacaciones deben solicitarse con una semana de anticipacion y solo se dara permiso por 3 dias</t>
+  </si>
+  <si>
+    <t>Salir antes de que termine la jornada laboral</t>
+  </si>
+  <si>
+    <t>Esto puede realizarse solo cuando el proyecto donde este involucrado el personal no se encuentre en fase critica (No se tienen agendas, reuniones de la organizacion, reuniones con el cliente, capacitacion o se requiere de su presencia para actividades de otros en el proyecto)</t>
+  </si>
+  <si>
+    <t>Registro de actividades laborales</t>
+  </si>
+  <si>
+    <t>Se deben registrar las actividades que se realizaron durante la jornada laboral a diario antes de abandonar las instalaciones de la empresa</t>
   </si>
 </sst>
 </file>
@@ -2034,7 +2066,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -2390,21 +2422,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2467,7 +2484,7 @@
     </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="45" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2736,9 +2753,6 @@
     <xf numFmtId="0" fontId="0" fillId="26" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="31" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2786,9 +2800,6 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="27" borderId="28" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="33" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2900,6 +2911,12 @@
     <xf numFmtId="0" fontId="30" fillId="38" borderId="11" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2921,21 +2938,21 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="52" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="25" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="25" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2962,12 +2979,6 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="46" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="56">
@@ -4071,11 +4082,11 @@
   <sheetData>
     <row r="1" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="147"/>
-      <c r="B2" s="146" t="s">
+      <c r="A2" s="145"/>
+      <c r="B2" s="144" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="147"/>
+      <c r="C2" s="145"/>
       <c r="D2" s="77"/>
       <c r="E2" s="77"/>
     </row>
@@ -4102,11 +4113,11 @@
       <c r="E4" s="80"/>
     </row>
     <row r="5" spans="1:7" s="70" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="148"/>
-      <c r="B5" s="147" t="s">
+      <c r="A5" s="146"/>
+      <c r="B5" s="145" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="148"/>
+      <c r="C5" s="146"/>
       <c r="D5" s="78"/>
       <c r="E5" s="78"/>
     </row>
@@ -4126,7 +4137,7 @@
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="163">
+      <c r="C7" s="161">
         <v>42199</v>
       </c>
       <c r="D7" s="178"/>
@@ -4135,11 +4146,11 @@
       <c r="G7" s="70"/>
     </row>
     <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="149"/>
-      <c r="B8" s="146" t="s">
+      <c r="A8" s="147"/>
+      <c r="B8" s="144" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="149"/>
+      <c r="C8" s="147"/>
     </row>
     <row r="9" spans="1:7" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B9" s="65" t="s">
@@ -4148,10 +4159,10 @@
       <c r="C9" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="116" t="s">
+      <c r="E9" s="115" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="116" t="s">
+      <c r="F9" s="115" t="s">
         <v>102</v>
       </c>
     </row>
@@ -4176,11 +4187,11 @@
       <c r="C12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="149"/>
-      <c r="B13" s="146" t="s">
+      <c r="A13" s="147"/>
+      <c r="B13" s="144" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="149"/>
+      <c r="C13" s="147"/>
     </row>
     <row r="14" spans="1:7" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B14" s="61" t="s">
@@ -4269,11 +4280,11 @@
       <c r="C26" s="62"/>
     </row>
     <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="149"/>
-      <c r="B27" s="146" t="s">
+      <c r="A27" s="147"/>
+      <c r="B27" s="144" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="149"/>
+      <c r="C27" s="147"/>
     </row>
     <row r="28" spans="1:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="179" t="s">
@@ -4282,11 +4293,11 @@
       <c r="C28" s="179"/>
     </row>
     <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="149"/>
-      <c r="B29" s="146" t="s">
+      <c r="A29" s="147"/>
+      <c r="B29" s="144" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="149"/>
+      <c r="C29" s="147"/>
     </row>
     <row r="30" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="180" t="s">
@@ -4785,26 +4796,26 @@
   <sheetData>
     <row r="1" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="150"/>
-      <c r="B2" s="151" t="s">
+      <c r="A2" s="148"/>
+      <c r="B2" s="149" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="157"/>
-      <c r="B3" s="158" t="s">
+      <c r="A3" s="155"/>
+      <c r="B3" s="156" t="s">
         <v>185</v>
       </c>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
+      <c r="C3" s="155"/>
+      <c r="D3" s="155"/>
+      <c r="E3" s="155"/>
+      <c r="F3" s="155"/>
+      <c r="G3" s="155"/>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="18" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
@@ -4838,7 +4849,7 @@
       <c r="D5" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="E5" s="164" t="s">
+      <c r="E5" s="162" t="s">
         <v>190</v>
       </c>
       <c r="F5" s="18" t="s">
@@ -4858,118 +4869,118 @@
       <c r="G6" s="23"/>
     </row>
     <row r="7" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A7" s="148"/>
-      <c r="B7" s="152" t="s">
+      <c r="A7" s="146"/>
+      <c r="B7" s="150" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="148"/>
-      <c r="D7" s="148"/>
-      <c r="E7" s="148"/>
-      <c r="F7" s="148"/>
-      <c r="G7" s="148"/>
+      <c r="C7" s="146"/>
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="146"/>
     </row>
     <row r="8" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
       <c r="B8" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="185" t="s">
+      <c r="C8" s="187" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="185"/>
-      <c r="E8" s="186" t="s">
+      <c r="D8" s="187"/>
+      <c r="E8" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="186"/>
+      <c r="F8" s="188"/>
       <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="153"/>
-      <c r="B9" s="154" t="s">
+      <c r="A9" s="151"/>
+      <c r="B9" s="152" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="154"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="154"/>
-      <c r="G9" s="154"/>
+      <c r="C9" s="152"/>
+      <c r="D9" s="152"/>
+      <c r="E9" s="152"/>
+      <c r="F9" s="152"/>
+      <c r="G9" s="152"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="C10" s="184" t="str">
+      <c r="C10" s="185" t="str">
         <f>VLOOKUP(B10,$B$50:$D$66,2,0)</f>
         <v>33 1605 3573</v>
       </c>
-      <c r="D10" s="184"/>
-      <c r="E10" s="184" t="str">
+      <c r="D10" s="185"/>
+      <c r="E10" s="185" t="str">
         <f>VLOOKUP(B10,$B$50:$D$66,3,0)</f>
         <v>felipelozanopadilla@gmail.com</v>
       </c>
-      <c r="F10" s="184"/>
-      <c r="G10" s="165" t="s">
+      <c r="F10" s="185"/>
+      <c r="G10" s="163" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="155"/>
-      <c r="B11" s="156" t="s">
+      <c r="A11" s="153"/>
+      <c r="B11" s="154" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="156"/>
-      <c r="D11" s="156"/>
-      <c r="E11" s="156"/>
-      <c r="F11" s="156"/>
-      <c r="G11" s="156"/>
+      <c r="C11" s="154"/>
+      <c r="D11" s="154"/>
+      <c r="E11" s="154"/>
+      <c r="F11" s="154"/>
+      <c r="G11" s="154"/>
     </row>
     <row r="12" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="C12" s="184" t="str">
+      <c r="C12" s="185" t="str">
         <f>VLOOKUP(B12,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184" t="str">
+      <c r="D12" s="185"/>
+      <c r="E12" s="185" t="str">
         <f>VLOOKUP(B12,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F12" s="184"/>
-      <c r="G12" s="165" t="s">
+      <c r="F12" s="185"/>
+      <c r="G12" s="163" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="155"/>
-      <c r="B13" s="156" t="s">
+      <c r="A13" s="153"/>
+      <c r="B13" s="154" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="156"/>
-      <c r="D13" s="156"/>
-      <c r="E13" s="156"/>
-      <c r="F13" s="156"/>
-      <c r="G13" s="156"/>
+      <c r="C13" s="154"/>
+      <c r="D13" s="154"/>
+      <c r="E13" s="154"/>
+      <c r="F13" s="154"/>
+      <c r="G13" s="154"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="184" t="str">
+      <c r="C14" s="185" t="str">
         <f>VLOOKUP(B14,$B$50:$D$66,2,0)</f>
         <v>33 1862 1719</v>
       </c>
-      <c r="D14" s="184"/>
-      <c r="E14" s="184" t="str">
+      <c r="D14" s="185"/>
+      <c r="E14" s="185" t="str">
         <f>VLOOKUP(B14,$B$50:$D$66,3,0)</f>
         <v>rpulido@qualtop.com</v>
       </c>
-      <c r="F14" s="184"/>
-      <c r="G14" s="165" t="s">
+      <c r="F14" s="185"/>
+      <c r="G14" s="163" t="s">
         <v>205</v>
       </c>
     </row>
@@ -4978,45 +4989,45 @@
       <c r="B15" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="184" t="e">
+      <c r="C15" s="185" t="e">
         <f>VLOOKUP(B15,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D15" s="184"/>
-      <c r="E15" s="184" t="e">
+      <c r="D15" s="185"/>
+      <c r="E15" s="185" t="e">
         <f>VLOOKUP(B15,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F15" s="184"/>
+      <c r="F15" s="185"/>
       <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="155"/>
-      <c r="B16" s="156" t="s">
+      <c r="A16" s="153"/>
+      <c r="B16" s="154" t="s">
         <v>79</v>
       </c>
-      <c r="C16" s="156"/>
-      <c r="D16" s="156"/>
-      <c r="E16" s="156"/>
-      <c r="F16" s="156"/>
-      <c r="G16" s="156"/>
+      <c r="C16" s="154"/>
+      <c r="D16" s="154"/>
+      <c r="E16" s="154"/>
+      <c r="F16" s="154"/>
+      <c r="G16" s="154"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="C17" s="184" t="str">
+      <c r="C17" s="185" t="str">
         <f>VLOOKUP(B17,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D17" s="184"/>
-      <c r="E17" s="184" t="str">
+      <c r="D17" s="185"/>
+      <c r="E17" s="185" t="str">
         <f>VLOOKUP(B17,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F17" s="184"/>
-      <c r="G17" s="165" t="s">
+      <c r="F17" s="185"/>
+      <c r="G17" s="163" t="s">
         <v>205</v>
       </c>
     </row>
@@ -5025,16 +5036,16 @@
       <c r="B18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="184" t="e">
+      <c r="C18" s="185" t="e">
         <f>VLOOKUP(B18,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D18" s="184"/>
-      <c r="E18" s="184" t="e">
+      <c r="D18" s="185"/>
+      <c r="E18" s="185" t="e">
         <f>VLOOKUP(B18,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F18" s="184"/>
+      <c r="F18" s="185"/>
       <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -5042,45 +5053,45 @@
       <c r="B19" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="184" t="e">
+      <c r="C19" s="185" t="e">
         <f>VLOOKUP(B19,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D19" s="184"/>
-      <c r="E19" s="184" t="e">
+      <c r="D19" s="185"/>
+      <c r="E19" s="185" t="e">
         <f>VLOOKUP(B19,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F19" s="184"/>
+      <c r="F19" s="185"/>
       <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="155"/>
-      <c r="B20" s="156" t="s">
+      <c r="A20" s="153"/>
+      <c r="B20" s="154" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="156"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="156"/>
-      <c r="F20" s="156"/>
-      <c r="G20" s="156"/>
+      <c r="C20" s="154"/>
+      <c r="D20" s="154"/>
+      <c r="E20" s="154"/>
+      <c r="F20" s="154"/>
+      <c r="G20" s="154"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="C21" s="184" t="str">
+      <c r="C21" s="185" t="str">
         <f>VLOOKUP(B21,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D21" s="184"/>
-      <c r="E21" s="184" t="str">
+      <c r="D21" s="185"/>
+      <c r="E21" s="185" t="str">
         <f>VLOOKUP(B21,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F21" s="184"/>
-      <c r="G21" s="165" t="s">
+      <c r="F21" s="185"/>
+      <c r="G21" s="163" t="s">
         <v>205</v>
       </c>
     </row>
@@ -5089,285 +5100,285 @@
       <c r="B22" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="184" t="e">
+      <c r="C22" s="185" t="e">
         <f>VLOOKUP(B22,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D22" s="184"/>
-      <c r="E22" s="184" t="e">
+      <c r="D22" s="185"/>
+      <c r="E22" s="185" t="e">
         <f>VLOOKUP(B22,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F22" s="184"/>
+      <c r="F22" s="185"/>
       <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="155"/>
-      <c r="B23" s="156" t="s">
+      <c r="A23" s="153"/>
+      <c r="B23" s="154" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="156"/>
-      <c r="D23" s="156"/>
-      <c r="E23" s="156"/>
-      <c r="F23" s="156"/>
-      <c r="G23" s="156"/>
+      <c r="C23" s="154"/>
+      <c r="D23" s="154"/>
+      <c r="E23" s="154"/>
+      <c r="F23" s="154"/>
+      <c r="G23" s="154"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="C24" s="184" t="str">
+      <c r="C24" s="185" t="str">
         <f>VLOOKUP(B24,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D24" s="184"/>
-      <c r="E24" s="184" t="str">
+      <c r="D24" s="185"/>
+      <c r="E24" s="185" t="str">
         <f>VLOOKUP(B24,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F24" s="184"/>
-      <c r="G24" s="165" t="s">
+      <c r="F24" s="185"/>
+      <c r="G24" s="163" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="155"/>
-      <c r="B25" s="156" t="s">
+      <c r="A25" s="153"/>
+      <c r="B25" s="154" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="156"/>
-      <c r="D25" s="156"/>
-      <c r="E25" s="156"/>
-      <c r="F25" s="156"/>
-      <c r="G25" s="156"/>
+      <c r="C25" s="154"/>
+      <c r="D25" s="154"/>
+      <c r="E25" s="154"/>
+      <c r="F25" s="154"/>
+      <c r="G25" s="154"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="C26" s="184" t="str">
+      <c r="C26" s="185" t="str">
         <f>VLOOKUP(B26,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D26" s="184"/>
-      <c r="E26" s="184" t="str">
+      <c r="D26" s="185"/>
+      <c r="E26" s="185" t="str">
         <f>VLOOKUP(B26,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F26" s="184"/>
-      <c r="G26" s="165" t="s">
+      <c r="F26" s="185"/>
+      <c r="G26" s="163" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="155"/>
-      <c r="B27" s="156" t="s">
+      <c r="A27" s="153"/>
+      <c r="B27" s="154" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="156"/>
-      <c r="D27" s="156"/>
-      <c r="E27" s="156"/>
-      <c r="F27" s="156"/>
-      <c r="G27" s="156"/>
+      <c r="C27" s="154"/>
+      <c r="D27" s="154"/>
+      <c r="E27" s="154"/>
+      <c r="F27" s="154"/>
+      <c r="G27" s="154"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="C28" s="184" t="str">
+      <c r="C28" s="185" t="str">
         <f>VLOOKUP(B28,$B$50:$D$66,2,0)</f>
         <v>33 3807 6830</v>
       </c>
-      <c r="D28" s="184"/>
-      <c r="E28" s="184" t="str">
+      <c r="D28" s="185"/>
+      <c r="E28" s="185" t="str">
         <f>VLOOKUP(B28,$B$50:$D$66,3,0)</f>
         <v>asosa@qualtop.com</v>
       </c>
-      <c r="F28" s="184"/>
-      <c r="G28" s="165" t="s">
+      <c r="F28" s="185"/>
+      <c r="G28" s="163" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="155"/>
-      <c r="B29" s="156" t="s">
+      <c r="A29" s="153"/>
+      <c r="B29" s="154" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="156"/>
-      <c r="D29" s="156"/>
-      <c r="E29" s="156"/>
-      <c r="F29" s="156"/>
-      <c r="G29" s="156"/>
+      <c r="C29" s="154"/>
+      <c r="D29" s="154"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="154"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="C30" s="184" t="str">
+      <c r="C30" s="185" t="str">
         <f>VLOOKUP(B30,$B$50:$D$66,2,0)</f>
         <v>33 3807 6830</v>
       </c>
-      <c r="D30" s="184"/>
-      <c r="E30" s="184" t="str">
+      <c r="D30" s="185"/>
+      <c r="E30" s="185" t="str">
         <f>VLOOKUP(B30,$B$50:$D$66,3,0)</f>
         <v>asosa@qualtop.com</v>
       </c>
-      <c r="F30" s="184"/>
-      <c r="G30" s="165" t="s">
+      <c r="F30" s="185"/>
+      <c r="G30" s="163" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="155"/>
-      <c r="B31" s="156" t="s">
+      <c r="A31" s="153"/>
+      <c r="B31" s="154" t="s">
         <v>118</v>
       </c>
-      <c r="C31" s="156"/>
-      <c r="D31" s="156"/>
-      <c r="E31" s="156"/>
-      <c r="F31" s="156"/>
-      <c r="G31" s="156"/>
+      <c r="C31" s="154"/>
+      <c r="D31" s="154"/>
+      <c r="E31" s="154"/>
+      <c r="F31" s="154"/>
+      <c r="G31" s="154"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="C32" s="184" t="str">
+      <c r="C32" s="185" t="str">
         <f>VLOOKUP(B32,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D32" s="184"/>
-      <c r="E32" s="184" t="str">
+      <c r="D32" s="185"/>
+      <c r="E32" s="185" t="str">
         <f>VLOOKUP(B32,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F32" s="184"/>
-      <c r="G32" s="165" t="s">
+      <c r="F32" s="185"/>
+      <c r="G32" s="163" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="155"/>
-      <c r="B33" s="156" t="s">
+      <c r="A33" s="153"/>
+      <c r="B33" s="154" t="s">
         <v>133</v>
       </c>
-      <c r="C33" s="156"/>
-      <c r="D33" s="156"/>
-      <c r="E33" s="156"/>
-      <c r="F33" s="156"/>
-      <c r="G33" s="156"/>
+      <c r="C33" s="154"/>
+      <c r="D33" s="154"/>
+      <c r="E33" s="154"/>
+      <c r="F33" s="154"/>
+      <c r="G33" s="154"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
       <c r="B34" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="C34" s="187" t="str">
+      <c r="C34" s="186" t="str">
         <f>VLOOKUP(B34,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D34" s="187"/>
-      <c r="E34" s="187" t="str">
+      <c r="D34" s="186"/>
+      <c r="E34" s="186" t="str">
         <f>VLOOKUP(B34,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F34" s="187"/>
-      <c r="G34" s="165" t="s">
+      <c r="F34" s="186"/>
+      <c r="G34" s="163" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="155"/>
-      <c r="B35" s="156" t="s">
+      <c r="A35" s="153"/>
+      <c r="B35" s="154" t="s">
         <v>132</v>
       </c>
-      <c r="C35" s="156"/>
-      <c r="D35" s="156"/>
-      <c r="E35" s="156"/>
-      <c r="F35" s="156"/>
-      <c r="G35" s="156"/>
+      <c r="C35" s="154"/>
+      <c r="D35" s="154"/>
+      <c r="E35" s="154"/>
+      <c r="F35" s="154"/>
+      <c r="G35" s="154"/>
     </row>
     <row r="36" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26"/>
       <c r="B36" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="C36" s="187" t="str">
+      <c r="C36" s="186" t="str">
         <f>VLOOKUP(B36,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D36" s="187"/>
-      <c r="E36" s="187" t="str">
+      <c r="D36" s="186"/>
+      <c r="E36" s="186" t="str">
         <f>VLOOKUP(B36,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F36" s="187"/>
-      <c r="G36" s="165" t="s">
+      <c r="F36" s="186"/>
+      <c r="G36" s="163" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="155"/>
-      <c r="B37" s="156" t="s">
+      <c r="A37" s="153"/>
+      <c r="B37" s="154" t="s">
         <v>119</v>
       </c>
-      <c r="C37" s="156"/>
-      <c r="D37" s="156"/>
-      <c r="E37" s="156"/>
-      <c r="F37" s="156"/>
-      <c r="G37" s="156"/>
+      <c r="C37" s="154"/>
+      <c r="D37" s="154"/>
+      <c r="E37" s="154"/>
+      <c r="F37" s="154"/>
+      <c r="G37" s="154"/>
     </row>
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
       <c r="B38" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="C38" s="184" t="str">
+      <c r="C38" s="185" t="str">
         <f>VLOOKUP(B38,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D38" s="184"/>
-      <c r="E38" s="184" t="str">
+      <c r="D38" s="185"/>
+      <c r="E38" s="185" t="str">
         <f>VLOOKUP(B38,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F38" s="184"/>
-      <c r="G38" s="165" t="s">
+      <c r="F38" s="185"/>
+      <c r="G38" s="163" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="155"/>
-      <c r="B39" s="156" t="s">
+      <c r="A39" s="153"/>
+      <c r="B39" s="154" t="s">
         <v>134</v>
       </c>
-      <c r="C39" s="156"/>
-      <c r="D39" s="156"/>
-      <c r="E39" s="156"/>
-      <c r="F39" s="156"/>
-      <c r="G39" s="156"/>
+      <c r="C39" s="154"/>
+      <c r="D39" s="154"/>
+      <c r="E39" s="154"/>
+      <c r="F39" s="154"/>
+      <c r="G39" s="154"/>
     </row>
     <row r="40" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26"/>
       <c r="B40" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="C40" s="184" t="str">
+      <c r="C40" s="185" t="str">
         <f>VLOOKUP(B40,$B$50:$D$66,2,0)</f>
         <v>33 1862 1719</v>
       </c>
-      <c r="D40" s="184"/>
-      <c r="E40" s="184" t="str">
+      <c r="D40" s="185"/>
+      <c r="E40" s="185" t="str">
         <f>VLOOKUP(B40,$B$50:$D$66,3,0)</f>
         <v>rpulido@qualtop.com</v>
       </c>
-      <c r="F40" s="184"/>
-      <c r="G40" s="165" t="s">
+      <c r="F40" s="185"/>
+      <c r="G40" s="163" t="s">
         <v>205</v>
       </c>
     </row>
@@ -5376,17 +5387,17 @@
       <c r="B41" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="C41" s="184" t="str">
+      <c r="C41" s="185" t="str">
         <f>VLOOKUP(B41,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D41" s="184"/>
-      <c r="E41" s="184" t="str">
+      <c r="D41" s="185"/>
+      <c r="E41" s="185" t="str">
         <f>VLOOKUP(B41,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F41" s="184"/>
-      <c r="G41" s="165" t="s">
+      <c r="F41" s="185"/>
+      <c r="G41" s="163" t="s">
         <v>205</v>
       </c>
     </row>
@@ -5395,46 +5406,46 @@
       <c r="B42" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C42" s="184" t="e">
+      <c r="C42" s="185" t="e">
         <f>VLOOKUP(B42,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D42" s="184"/>
-      <c r="E42" s="184" t="e">
+      <c r="D42" s="185"/>
+      <c r="E42" s="185" t="e">
         <f>VLOOKUP(B42,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F42" s="184"/>
+      <c r="F42" s="185"/>
       <c r="G42" s="23"/>
     </row>
     <row r="43" spans="1:7" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="148"/>
-      <c r="B43" s="147" t="s">
+      <c r="A43" s="146"/>
+      <c r="B43" s="145" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="148"/>
-      <c r="D43" s="148"/>
-      <c r="E43" s="148"/>
-      <c r="F43" s="148"/>
-      <c r="G43" s="148"/>
+      <c r="C43" s="146"/>
+      <c r="D43" s="146"/>
+      <c r="E43" s="146"/>
+      <c r="F43" s="146"/>
+      <c r="G43" s="146"/>
     </row>
     <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
-      <c r="B44" s="188" t="s">
+      <c r="B44" s="184" t="s">
         <v>76</v>
       </c>
-      <c r="C44" s="188"/>
-      <c r="D44" s="188"/>
-      <c r="E44" s="188"/>
-      <c r="F44" s="188"/>
+      <c r="C44" s="184"/>
+      <c r="D44" s="184"/>
+      <c r="E44" s="184"/>
+      <c r="F44" s="184"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="188"/>
-      <c r="C45" s="188"/>
-      <c r="D45" s="188"/>
-      <c r="E45" s="188"/>
-      <c r="F45" s="188"/>
+      <c r="B45" s="184"/>
+      <c r="C45" s="184"/>
+      <c r="D45" s="184"/>
+      <c r="E45" s="184"/>
+      <c r="F45" s="184"/>
       <c r="G45" s="81"/>
     </row>
     <row r="46" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -5571,6 +5582,33 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="43">
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="B44:F45"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
@@ -5587,33 +5625,6 @@
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVM983093:WVM983106 JA50:JA66 SW50:SW66 ACS50:ACS66 AMO50:AMO66 AWK50:AWK66 BGG50:BGG66 BQC50:BQC66 BZY50:BZY66 CJU50:CJU66 CTQ50:CTQ66 DDM50:DDM66 DNI50:DNI66 DXE50:DXE66 EHA50:EHA66 EQW50:EQW66 FAS50:FAS66 FKO50:FKO66 FUK50:FUK66 GEG50:GEG66 GOC50:GOC66 GXY50:GXY66 HHU50:HHU66 HRQ50:HRQ66 IBM50:IBM66 ILI50:ILI66 IVE50:IVE66 JFA50:JFA66 JOW50:JOW66 JYS50:JYS66 KIO50:KIO66 KSK50:KSK66 LCG50:LCG66 LMC50:LMC66 LVY50:LVY66 MFU50:MFU66 MPQ50:MPQ66 MZM50:MZM66 NJI50:NJI66 NTE50:NTE66 ODA50:ODA66 OMW50:OMW66 OWS50:OWS66 PGO50:PGO66 PQK50:PQK66 QAG50:QAG66 QKC50:QKC66 QTY50:QTY66 RDU50:RDU66 RNQ50:RNQ66 RXM50:RXM66 SHI50:SHI66 SRE50:SRE66 TBA50:TBA66 TKW50:TKW66 TUS50:TUS66 UEO50:UEO66 UOK50:UOK66 UYG50:UYG66 VIC50:VIC66 VRY50:VRY66 WBU50:WBU66 WLQ50:WLQ66 WVM50:WVM66 D65570:D65583 JA65589:JA65602 SW65589:SW65602 ACS65589:ACS65602 AMO65589:AMO65602 AWK65589:AWK65602 BGG65589:BGG65602 BQC65589:BQC65602 BZY65589:BZY65602 CJU65589:CJU65602 CTQ65589:CTQ65602 DDM65589:DDM65602 DNI65589:DNI65602 DXE65589:DXE65602 EHA65589:EHA65602 EQW65589:EQW65602 FAS65589:FAS65602 FKO65589:FKO65602 FUK65589:FUK65602 GEG65589:GEG65602 GOC65589:GOC65602 GXY65589:GXY65602 HHU65589:HHU65602 HRQ65589:HRQ65602 IBM65589:IBM65602 ILI65589:ILI65602 IVE65589:IVE65602 JFA65589:JFA65602 JOW65589:JOW65602 JYS65589:JYS65602 KIO65589:KIO65602 KSK65589:KSK65602 LCG65589:LCG65602 LMC65589:LMC65602 LVY65589:LVY65602 MFU65589:MFU65602 MPQ65589:MPQ65602 MZM65589:MZM65602 NJI65589:NJI65602 NTE65589:NTE65602 ODA65589:ODA65602 OMW65589:OMW65602 OWS65589:OWS65602 PGO65589:PGO65602 PQK65589:PQK65602 QAG65589:QAG65602 QKC65589:QKC65602 QTY65589:QTY65602 RDU65589:RDU65602 RNQ65589:RNQ65602 RXM65589:RXM65602 SHI65589:SHI65602 SRE65589:SRE65602 TBA65589:TBA65602 TKW65589:TKW65602 TUS65589:TUS65602 UEO65589:UEO65602 UOK65589:UOK65602 UYG65589:UYG65602 VIC65589:VIC65602 VRY65589:VRY65602 WBU65589:WBU65602 WLQ65589:WLQ65602 WVM65589:WVM65602 D131106:D131119 JA131125:JA131138 SW131125:SW131138 ACS131125:ACS131138 AMO131125:AMO131138 AWK131125:AWK131138 BGG131125:BGG131138 BQC131125:BQC131138 BZY131125:BZY131138 CJU131125:CJU131138 CTQ131125:CTQ131138 DDM131125:DDM131138 DNI131125:DNI131138 DXE131125:DXE131138 EHA131125:EHA131138 EQW131125:EQW131138 FAS131125:FAS131138 FKO131125:FKO131138 FUK131125:FUK131138 GEG131125:GEG131138 GOC131125:GOC131138 GXY131125:GXY131138 HHU131125:HHU131138 HRQ131125:HRQ131138 IBM131125:IBM131138 ILI131125:ILI131138 IVE131125:IVE131138 JFA131125:JFA131138 JOW131125:JOW131138 JYS131125:JYS131138 KIO131125:KIO131138 KSK131125:KSK131138 LCG131125:LCG131138 LMC131125:LMC131138 LVY131125:LVY131138 MFU131125:MFU131138 MPQ131125:MPQ131138 MZM131125:MZM131138 NJI131125:NJI131138 NTE131125:NTE131138 ODA131125:ODA131138 OMW131125:OMW131138 OWS131125:OWS131138 PGO131125:PGO131138 PQK131125:PQK131138 QAG131125:QAG131138 QKC131125:QKC131138 QTY131125:QTY131138 RDU131125:RDU131138 RNQ131125:RNQ131138 RXM131125:RXM131138 SHI131125:SHI131138 SRE131125:SRE131138 TBA131125:TBA131138 TKW131125:TKW131138 TUS131125:TUS131138 UEO131125:UEO131138 UOK131125:UOK131138 UYG131125:UYG131138 VIC131125:VIC131138 VRY131125:VRY131138 WBU131125:WBU131138 WLQ131125:WLQ131138 WVM131125:WVM131138 D196642:D196655 JA196661:JA196674 SW196661:SW196674 ACS196661:ACS196674 AMO196661:AMO196674 AWK196661:AWK196674 BGG196661:BGG196674 BQC196661:BQC196674 BZY196661:BZY196674 CJU196661:CJU196674 CTQ196661:CTQ196674 DDM196661:DDM196674 DNI196661:DNI196674 DXE196661:DXE196674 EHA196661:EHA196674 EQW196661:EQW196674 FAS196661:FAS196674 FKO196661:FKO196674 FUK196661:FUK196674 GEG196661:GEG196674 GOC196661:GOC196674 GXY196661:GXY196674 HHU196661:HHU196674 HRQ196661:HRQ196674 IBM196661:IBM196674 ILI196661:ILI196674 IVE196661:IVE196674 JFA196661:JFA196674 JOW196661:JOW196674 JYS196661:JYS196674 KIO196661:KIO196674 KSK196661:KSK196674 LCG196661:LCG196674 LMC196661:LMC196674 LVY196661:LVY196674 MFU196661:MFU196674 MPQ196661:MPQ196674 MZM196661:MZM196674 NJI196661:NJI196674 NTE196661:NTE196674 ODA196661:ODA196674 OMW196661:OMW196674 OWS196661:OWS196674 PGO196661:PGO196674 PQK196661:PQK196674 QAG196661:QAG196674 QKC196661:QKC196674 QTY196661:QTY196674 RDU196661:RDU196674 RNQ196661:RNQ196674 RXM196661:RXM196674 SHI196661:SHI196674 SRE196661:SRE196674 TBA196661:TBA196674 TKW196661:TKW196674 TUS196661:TUS196674 UEO196661:UEO196674 UOK196661:UOK196674 UYG196661:UYG196674 VIC196661:VIC196674 VRY196661:VRY196674 WBU196661:WBU196674 WLQ196661:WLQ196674 WVM196661:WVM196674 D262178:D262191 JA262197:JA262210 SW262197:SW262210 ACS262197:ACS262210 AMO262197:AMO262210 AWK262197:AWK262210 BGG262197:BGG262210 BQC262197:BQC262210 BZY262197:BZY262210 CJU262197:CJU262210 CTQ262197:CTQ262210 DDM262197:DDM262210 DNI262197:DNI262210 DXE262197:DXE262210 EHA262197:EHA262210 EQW262197:EQW262210 FAS262197:FAS262210 FKO262197:FKO262210 FUK262197:FUK262210 GEG262197:GEG262210 GOC262197:GOC262210 GXY262197:GXY262210 HHU262197:HHU262210 HRQ262197:HRQ262210 IBM262197:IBM262210 ILI262197:ILI262210 IVE262197:IVE262210 JFA262197:JFA262210 JOW262197:JOW262210 JYS262197:JYS262210 KIO262197:KIO262210 KSK262197:KSK262210 LCG262197:LCG262210 LMC262197:LMC262210 LVY262197:LVY262210 MFU262197:MFU262210 MPQ262197:MPQ262210 MZM262197:MZM262210 NJI262197:NJI262210 NTE262197:NTE262210 ODA262197:ODA262210 OMW262197:OMW262210 OWS262197:OWS262210 PGO262197:PGO262210 PQK262197:PQK262210 QAG262197:QAG262210 QKC262197:QKC262210 QTY262197:QTY262210 RDU262197:RDU262210 RNQ262197:RNQ262210 RXM262197:RXM262210 SHI262197:SHI262210 SRE262197:SRE262210 TBA262197:TBA262210 TKW262197:TKW262210 TUS262197:TUS262210 UEO262197:UEO262210 UOK262197:UOK262210 UYG262197:UYG262210 VIC262197:VIC262210 VRY262197:VRY262210 WBU262197:WBU262210 WLQ262197:WLQ262210 WVM262197:WVM262210 D327714:D327727 JA327733:JA327746 SW327733:SW327746 ACS327733:ACS327746 AMO327733:AMO327746 AWK327733:AWK327746 BGG327733:BGG327746 BQC327733:BQC327746 BZY327733:BZY327746 CJU327733:CJU327746 CTQ327733:CTQ327746 DDM327733:DDM327746 DNI327733:DNI327746 DXE327733:DXE327746 EHA327733:EHA327746 EQW327733:EQW327746 FAS327733:FAS327746 FKO327733:FKO327746 FUK327733:FUK327746 GEG327733:GEG327746 GOC327733:GOC327746 GXY327733:GXY327746 HHU327733:HHU327746 HRQ327733:HRQ327746 IBM327733:IBM327746 ILI327733:ILI327746 IVE327733:IVE327746 JFA327733:JFA327746 JOW327733:JOW327746 JYS327733:JYS327746 KIO327733:KIO327746 KSK327733:KSK327746 LCG327733:LCG327746 LMC327733:LMC327746 LVY327733:LVY327746 MFU327733:MFU327746 MPQ327733:MPQ327746 MZM327733:MZM327746 NJI327733:NJI327746 NTE327733:NTE327746 ODA327733:ODA327746 OMW327733:OMW327746 OWS327733:OWS327746 PGO327733:PGO327746 PQK327733:PQK327746 QAG327733:QAG327746 QKC327733:QKC327746 QTY327733:QTY327746 RDU327733:RDU327746 RNQ327733:RNQ327746 RXM327733:RXM327746 SHI327733:SHI327746 SRE327733:SRE327746 TBA327733:TBA327746 TKW327733:TKW327746 TUS327733:TUS327746 UEO327733:UEO327746 UOK327733:UOK327746 UYG327733:UYG327746 VIC327733:VIC327746 VRY327733:VRY327746 WBU327733:WBU327746 WLQ327733:WLQ327746 WVM327733:WVM327746 D393250:D393263 JA393269:JA393282 SW393269:SW393282 ACS393269:ACS393282 AMO393269:AMO393282 AWK393269:AWK393282 BGG393269:BGG393282 BQC393269:BQC393282 BZY393269:BZY393282 CJU393269:CJU393282 CTQ393269:CTQ393282 DDM393269:DDM393282 DNI393269:DNI393282 DXE393269:DXE393282 EHA393269:EHA393282 EQW393269:EQW393282 FAS393269:FAS393282 FKO393269:FKO393282 FUK393269:FUK393282 GEG393269:GEG393282 GOC393269:GOC393282 GXY393269:GXY393282 HHU393269:HHU393282 HRQ393269:HRQ393282 IBM393269:IBM393282 ILI393269:ILI393282 IVE393269:IVE393282 JFA393269:JFA393282 JOW393269:JOW393282 JYS393269:JYS393282 KIO393269:KIO393282 KSK393269:KSK393282 LCG393269:LCG393282 LMC393269:LMC393282 LVY393269:LVY393282 MFU393269:MFU393282 MPQ393269:MPQ393282 MZM393269:MZM393282 NJI393269:NJI393282 NTE393269:NTE393282 ODA393269:ODA393282 OMW393269:OMW393282 OWS393269:OWS393282 PGO393269:PGO393282 PQK393269:PQK393282 QAG393269:QAG393282 QKC393269:QKC393282 QTY393269:QTY393282 RDU393269:RDU393282 RNQ393269:RNQ393282 RXM393269:RXM393282 SHI393269:SHI393282 SRE393269:SRE393282 TBA393269:TBA393282 TKW393269:TKW393282 TUS393269:TUS393282 UEO393269:UEO393282 UOK393269:UOK393282 UYG393269:UYG393282 VIC393269:VIC393282 VRY393269:VRY393282 WBU393269:WBU393282 WLQ393269:WLQ393282 WVM393269:WVM393282 D458786:D458799 JA458805:JA458818 SW458805:SW458818 ACS458805:ACS458818 AMO458805:AMO458818 AWK458805:AWK458818 BGG458805:BGG458818 BQC458805:BQC458818 BZY458805:BZY458818 CJU458805:CJU458818 CTQ458805:CTQ458818 DDM458805:DDM458818 DNI458805:DNI458818 DXE458805:DXE458818 EHA458805:EHA458818 EQW458805:EQW458818 FAS458805:FAS458818 FKO458805:FKO458818 FUK458805:FUK458818 GEG458805:GEG458818 GOC458805:GOC458818 GXY458805:GXY458818 HHU458805:HHU458818 HRQ458805:HRQ458818 IBM458805:IBM458818 ILI458805:ILI458818 IVE458805:IVE458818 JFA458805:JFA458818 JOW458805:JOW458818 JYS458805:JYS458818 KIO458805:KIO458818 KSK458805:KSK458818 LCG458805:LCG458818 LMC458805:LMC458818 LVY458805:LVY458818 MFU458805:MFU458818 MPQ458805:MPQ458818 MZM458805:MZM458818 NJI458805:NJI458818 NTE458805:NTE458818 ODA458805:ODA458818 OMW458805:OMW458818 OWS458805:OWS458818 PGO458805:PGO458818 PQK458805:PQK458818 QAG458805:QAG458818 QKC458805:QKC458818 QTY458805:QTY458818 RDU458805:RDU458818 RNQ458805:RNQ458818 RXM458805:RXM458818 SHI458805:SHI458818 SRE458805:SRE458818 TBA458805:TBA458818 TKW458805:TKW458818 TUS458805:TUS458818 UEO458805:UEO458818 UOK458805:UOK458818 UYG458805:UYG458818 VIC458805:VIC458818 VRY458805:VRY458818 WBU458805:WBU458818 WLQ458805:WLQ458818 WVM458805:WVM458818 D524322:D524335 JA524341:JA524354 SW524341:SW524354 ACS524341:ACS524354 AMO524341:AMO524354 AWK524341:AWK524354 BGG524341:BGG524354 BQC524341:BQC524354 BZY524341:BZY524354 CJU524341:CJU524354 CTQ524341:CTQ524354 DDM524341:DDM524354 DNI524341:DNI524354 DXE524341:DXE524354 EHA524341:EHA524354 EQW524341:EQW524354 FAS524341:FAS524354 FKO524341:FKO524354 FUK524341:FUK524354 GEG524341:GEG524354 GOC524341:GOC524354 GXY524341:GXY524354 HHU524341:HHU524354 HRQ524341:HRQ524354 IBM524341:IBM524354 ILI524341:ILI524354 IVE524341:IVE524354 JFA524341:JFA524354 JOW524341:JOW524354 JYS524341:JYS524354 KIO524341:KIO524354 KSK524341:KSK524354 LCG524341:LCG524354 LMC524341:LMC524354 LVY524341:LVY524354 MFU524341:MFU524354 MPQ524341:MPQ524354 MZM524341:MZM524354 NJI524341:NJI524354 NTE524341:NTE524354 ODA524341:ODA524354 OMW524341:OMW524354 OWS524341:OWS524354 PGO524341:PGO524354 PQK524341:PQK524354 QAG524341:QAG524354 QKC524341:QKC524354 QTY524341:QTY524354 RDU524341:RDU524354 RNQ524341:RNQ524354 RXM524341:RXM524354 SHI524341:SHI524354 SRE524341:SRE524354 TBA524341:TBA524354 TKW524341:TKW524354 TUS524341:TUS524354 UEO524341:UEO524354 UOK524341:UOK524354 UYG524341:UYG524354 VIC524341:VIC524354 VRY524341:VRY524354 WBU524341:WBU524354 WLQ524341:WLQ524354 WVM524341:WVM524354 D589858:D589871 JA589877:JA589890 SW589877:SW589890 ACS589877:ACS589890 AMO589877:AMO589890 AWK589877:AWK589890 BGG589877:BGG589890 BQC589877:BQC589890 BZY589877:BZY589890 CJU589877:CJU589890 CTQ589877:CTQ589890 DDM589877:DDM589890 DNI589877:DNI589890 DXE589877:DXE589890 EHA589877:EHA589890 EQW589877:EQW589890 FAS589877:FAS589890 FKO589877:FKO589890 FUK589877:FUK589890 GEG589877:GEG589890 GOC589877:GOC589890 GXY589877:GXY589890 HHU589877:HHU589890 HRQ589877:HRQ589890 IBM589877:IBM589890 ILI589877:ILI589890 IVE589877:IVE589890 JFA589877:JFA589890 JOW589877:JOW589890 JYS589877:JYS589890 KIO589877:KIO589890 KSK589877:KSK589890 LCG589877:LCG589890 LMC589877:LMC589890 LVY589877:LVY589890 MFU589877:MFU589890 MPQ589877:MPQ589890 MZM589877:MZM589890 NJI589877:NJI589890 NTE589877:NTE589890 ODA589877:ODA589890 OMW589877:OMW589890 OWS589877:OWS589890 PGO589877:PGO589890 PQK589877:PQK589890 QAG589877:QAG589890 QKC589877:QKC589890 QTY589877:QTY589890 RDU589877:RDU589890 RNQ589877:RNQ589890 RXM589877:RXM589890 SHI589877:SHI589890 SRE589877:SRE589890 TBA589877:TBA589890 TKW589877:TKW589890 TUS589877:TUS589890 UEO589877:UEO589890 UOK589877:UOK589890 UYG589877:UYG589890 VIC589877:VIC589890 VRY589877:VRY589890 WBU589877:WBU589890 WLQ589877:WLQ589890 WVM589877:WVM589890 D655394:D655407 JA655413:JA655426 SW655413:SW655426 ACS655413:ACS655426 AMO655413:AMO655426 AWK655413:AWK655426 BGG655413:BGG655426 BQC655413:BQC655426 BZY655413:BZY655426 CJU655413:CJU655426 CTQ655413:CTQ655426 DDM655413:DDM655426 DNI655413:DNI655426 DXE655413:DXE655426 EHA655413:EHA655426 EQW655413:EQW655426 FAS655413:FAS655426 FKO655413:FKO655426 FUK655413:FUK655426 GEG655413:GEG655426 GOC655413:GOC655426 GXY655413:GXY655426 HHU655413:HHU655426 HRQ655413:HRQ655426 IBM655413:IBM655426 ILI655413:ILI655426 IVE655413:IVE655426 JFA655413:JFA655426 JOW655413:JOW655426 JYS655413:JYS655426 KIO655413:KIO655426 KSK655413:KSK655426 LCG655413:LCG655426 LMC655413:LMC655426 LVY655413:LVY655426 MFU655413:MFU655426 MPQ655413:MPQ655426 MZM655413:MZM655426 NJI655413:NJI655426 NTE655413:NTE655426 ODA655413:ODA655426 OMW655413:OMW655426 OWS655413:OWS655426 PGO655413:PGO655426 PQK655413:PQK655426 QAG655413:QAG655426 QKC655413:QKC655426 QTY655413:QTY655426 RDU655413:RDU655426 RNQ655413:RNQ655426 RXM655413:RXM655426 SHI655413:SHI655426 SRE655413:SRE655426 TBA655413:TBA655426 TKW655413:TKW655426 TUS655413:TUS655426 UEO655413:UEO655426 UOK655413:UOK655426 UYG655413:UYG655426 VIC655413:VIC655426 VRY655413:VRY655426 WBU655413:WBU655426 WLQ655413:WLQ655426 WVM655413:WVM655426 D720930:D720943 JA720949:JA720962 SW720949:SW720962 ACS720949:ACS720962 AMO720949:AMO720962 AWK720949:AWK720962 BGG720949:BGG720962 BQC720949:BQC720962 BZY720949:BZY720962 CJU720949:CJU720962 CTQ720949:CTQ720962 DDM720949:DDM720962 DNI720949:DNI720962 DXE720949:DXE720962 EHA720949:EHA720962 EQW720949:EQW720962 FAS720949:FAS720962 FKO720949:FKO720962 FUK720949:FUK720962 GEG720949:GEG720962 GOC720949:GOC720962 GXY720949:GXY720962 HHU720949:HHU720962 HRQ720949:HRQ720962 IBM720949:IBM720962 ILI720949:ILI720962 IVE720949:IVE720962 JFA720949:JFA720962 JOW720949:JOW720962 JYS720949:JYS720962 KIO720949:KIO720962 KSK720949:KSK720962 LCG720949:LCG720962 LMC720949:LMC720962 LVY720949:LVY720962 MFU720949:MFU720962 MPQ720949:MPQ720962 MZM720949:MZM720962 NJI720949:NJI720962 NTE720949:NTE720962 ODA720949:ODA720962 OMW720949:OMW720962 OWS720949:OWS720962 PGO720949:PGO720962 PQK720949:PQK720962 QAG720949:QAG720962 QKC720949:QKC720962 QTY720949:QTY720962 RDU720949:RDU720962 RNQ720949:RNQ720962 RXM720949:RXM720962 SHI720949:SHI720962 SRE720949:SRE720962 TBA720949:TBA720962 TKW720949:TKW720962 TUS720949:TUS720962 UEO720949:UEO720962 UOK720949:UOK720962 UYG720949:UYG720962 VIC720949:VIC720962 VRY720949:VRY720962 WBU720949:WBU720962 WLQ720949:WLQ720962 WVM720949:WVM720962 D786466:D786479 JA786485:JA786498 SW786485:SW786498 ACS786485:ACS786498 AMO786485:AMO786498 AWK786485:AWK786498 BGG786485:BGG786498 BQC786485:BQC786498 BZY786485:BZY786498 CJU786485:CJU786498 CTQ786485:CTQ786498 DDM786485:DDM786498 DNI786485:DNI786498 DXE786485:DXE786498 EHA786485:EHA786498 EQW786485:EQW786498 FAS786485:FAS786498 FKO786485:FKO786498 FUK786485:FUK786498 GEG786485:GEG786498 GOC786485:GOC786498 GXY786485:GXY786498 HHU786485:HHU786498 HRQ786485:HRQ786498 IBM786485:IBM786498 ILI786485:ILI786498 IVE786485:IVE786498 JFA786485:JFA786498 JOW786485:JOW786498 JYS786485:JYS786498 KIO786485:KIO786498 KSK786485:KSK786498 LCG786485:LCG786498 LMC786485:LMC786498 LVY786485:LVY786498 MFU786485:MFU786498 MPQ786485:MPQ786498 MZM786485:MZM786498 NJI786485:NJI786498 NTE786485:NTE786498 ODA786485:ODA786498 OMW786485:OMW786498 OWS786485:OWS786498 PGO786485:PGO786498 PQK786485:PQK786498 QAG786485:QAG786498 QKC786485:QKC786498 QTY786485:QTY786498 RDU786485:RDU786498 RNQ786485:RNQ786498 RXM786485:RXM786498 SHI786485:SHI786498 SRE786485:SRE786498 TBA786485:TBA786498 TKW786485:TKW786498 TUS786485:TUS786498 UEO786485:UEO786498 UOK786485:UOK786498 UYG786485:UYG786498 VIC786485:VIC786498 VRY786485:VRY786498 WBU786485:WBU786498 WLQ786485:WLQ786498 WVM786485:WVM786498 D852002:D852015 JA852021:JA852034 SW852021:SW852034 ACS852021:ACS852034 AMO852021:AMO852034 AWK852021:AWK852034 BGG852021:BGG852034 BQC852021:BQC852034 BZY852021:BZY852034 CJU852021:CJU852034 CTQ852021:CTQ852034 DDM852021:DDM852034 DNI852021:DNI852034 DXE852021:DXE852034 EHA852021:EHA852034 EQW852021:EQW852034 FAS852021:FAS852034 FKO852021:FKO852034 FUK852021:FUK852034 GEG852021:GEG852034 GOC852021:GOC852034 GXY852021:GXY852034 HHU852021:HHU852034 HRQ852021:HRQ852034 IBM852021:IBM852034 ILI852021:ILI852034 IVE852021:IVE852034 JFA852021:JFA852034 JOW852021:JOW852034 JYS852021:JYS852034 KIO852021:KIO852034 KSK852021:KSK852034 LCG852021:LCG852034 LMC852021:LMC852034 LVY852021:LVY852034 MFU852021:MFU852034 MPQ852021:MPQ852034 MZM852021:MZM852034 NJI852021:NJI852034 NTE852021:NTE852034 ODA852021:ODA852034 OMW852021:OMW852034 OWS852021:OWS852034 PGO852021:PGO852034 PQK852021:PQK852034 QAG852021:QAG852034 QKC852021:QKC852034 QTY852021:QTY852034 RDU852021:RDU852034 RNQ852021:RNQ852034 RXM852021:RXM852034 SHI852021:SHI852034 SRE852021:SRE852034 TBA852021:TBA852034 TKW852021:TKW852034 TUS852021:TUS852034 UEO852021:UEO852034 UOK852021:UOK852034 UYG852021:UYG852034 VIC852021:VIC852034 VRY852021:VRY852034 WBU852021:WBU852034 WLQ852021:WLQ852034 WVM852021:WVM852034 D917538:D917551 JA917557:JA917570 SW917557:SW917570 ACS917557:ACS917570 AMO917557:AMO917570 AWK917557:AWK917570 BGG917557:BGG917570 BQC917557:BQC917570 BZY917557:BZY917570 CJU917557:CJU917570 CTQ917557:CTQ917570 DDM917557:DDM917570 DNI917557:DNI917570 DXE917557:DXE917570 EHA917557:EHA917570 EQW917557:EQW917570 FAS917557:FAS917570 FKO917557:FKO917570 FUK917557:FUK917570 GEG917557:GEG917570 GOC917557:GOC917570 GXY917557:GXY917570 HHU917557:HHU917570 HRQ917557:HRQ917570 IBM917557:IBM917570 ILI917557:ILI917570 IVE917557:IVE917570 JFA917557:JFA917570 JOW917557:JOW917570 JYS917557:JYS917570 KIO917557:KIO917570 KSK917557:KSK917570 LCG917557:LCG917570 LMC917557:LMC917570 LVY917557:LVY917570 MFU917557:MFU917570 MPQ917557:MPQ917570 MZM917557:MZM917570 NJI917557:NJI917570 NTE917557:NTE917570 ODA917557:ODA917570 OMW917557:OMW917570 OWS917557:OWS917570 PGO917557:PGO917570 PQK917557:PQK917570 QAG917557:QAG917570 QKC917557:QKC917570 QTY917557:QTY917570 RDU917557:RDU917570 RNQ917557:RNQ917570 RXM917557:RXM917570 SHI917557:SHI917570 SRE917557:SRE917570 TBA917557:TBA917570 TKW917557:TKW917570 TUS917557:TUS917570 UEO917557:UEO917570 UOK917557:UOK917570 UYG917557:UYG917570 VIC917557:VIC917570 VRY917557:VRY917570 WBU917557:WBU917570 WLQ917557:WLQ917570 WVM917557:WVM917570 D983074:D983087 JA983093:JA983106 SW983093:SW983106 ACS983093:ACS983106 AMO983093:AMO983106 AWK983093:AWK983106 BGG983093:BGG983106 BQC983093:BQC983106 BZY983093:BZY983106 CJU983093:CJU983106 CTQ983093:CTQ983106 DDM983093:DDM983106 DNI983093:DNI983106 DXE983093:DXE983106 EHA983093:EHA983106 EQW983093:EQW983106 FAS983093:FAS983106 FKO983093:FKO983106 FUK983093:FUK983106 GEG983093:GEG983106 GOC983093:GOC983106 GXY983093:GXY983106 HHU983093:HHU983106 HRQ983093:HRQ983106 IBM983093:IBM983106 ILI983093:ILI983106 IVE983093:IVE983106 JFA983093:JFA983106 JOW983093:JOW983106 JYS983093:JYS983106 KIO983093:KIO983106 KSK983093:KSK983106 LCG983093:LCG983106 LMC983093:LMC983106 LVY983093:LVY983106 MFU983093:MFU983106 MPQ983093:MPQ983106 MZM983093:MZM983106 NJI983093:NJI983106 NTE983093:NTE983106 ODA983093:ODA983106 OMW983093:OMW983106 OWS983093:OWS983106 PGO983093:PGO983106 PQK983093:PQK983106 QAG983093:QAG983106 QKC983093:QKC983106 QTY983093:QTY983106 RDU983093:RDU983106 RNQ983093:RNQ983106 RXM983093:RXM983106 SHI983093:SHI983106 SRE983093:SRE983106 TBA983093:TBA983106 TKW983093:TKW983106 TUS983093:TUS983106 UEO983093:UEO983106 UOK983093:UOK983106 UYG983093:UYG983106 VIC983093:VIC983106 VRY983093:VRY983106 WBU983093:WBU983106 WLQ983093:WLQ983106">
@@ -6447,15 +6458,15 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="150"/>
-      <c r="B2" s="151" t="s">
+      <c r="A2" s="148"/>
+      <c r="B2" s="149" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="E2" s="150"/>
-      <c r="F2" s="150"/>
-      <c r="G2" s="150"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
@@ -7597,48 +7608,48 @@
   <sheetData>
     <row r="1" spans="1:269" ht="57" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:269" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="134"/>
-      <c r="B2" s="135" t="s">
+      <c r="A2" s="132"/>
+      <c r="B2" s="133" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="136"/>
-      <c r="L2" s="137"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="134"/>
-      <c r="O2" s="134"/>
-      <c r="P2" s="134"/>
-      <c r="Q2" s="134"/>
-      <c r="R2" s="134"/>
+      <c r="C2" s="133"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="132"/>
+      <c r="F2" s="132"/>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="135"/>
+      <c r="M2" s="136"/>
+      <c r="N2" s="132"/>
+      <c r="O2" s="132"/>
+      <c r="P2" s="132"/>
+      <c r="Q2" s="132"/>
+      <c r="R2" s="132"/>
       <c r="S2" s="189" t="s">
         <v>48</v>
       </c>
-      <c r="JB2" s="162" t="s">
+      <c r="JB2" s="160" t="s">
         <v>163</v>
       </c>
       <c r="JC2" s="27">
         <v>5</v>
       </c>
-      <c r="JD2" s="108">
+      <c r="JD2" s="107">
         <v>5</v>
       </c>
-      <c r="JE2" s="108">
+      <c r="JE2" s="107">
         <v>10</v>
       </c>
-      <c r="JF2" s="107">
+      <c r="JF2" s="106">
         <v>15</v>
       </c>
-      <c r="JG2" s="107">
+      <c r="JG2" s="106">
         <v>20</v>
       </c>
-      <c r="JH2" s="107">
+      <c r="JH2" s="106">
         <v>25</v>
       </c>
       <c r="JI2" s="32"/>
@@ -7697,70 +7708,70 @@
         <v>11</v>
       </c>
       <c r="S3" s="189"/>
-      <c r="JB3" s="162" t="s">
+      <c r="JB3" s="160" t="s">
         <v>164</v>
       </c>
       <c r="JC3" s="27">
         <v>4</v>
       </c>
-      <c r="JD3" s="106">
+      <c r="JD3" s="105">
         <v>4</v>
       </c>
-      <c r="JE3" s="108">
+      <c r="JE3" s="107">
         <v>8</v>
       </c>
-      <c r="JF3" s="107">
+      <c r="JF3" s="106">
         <v>12</v>
       </c>
-      <c r="JG3" s="107">
+      <c r="JG3" s="106">
         <v>16</v>
       </c>
-      <c r="JH3" s="107">
+      <c r="JH3" s="106">
         <v>20</v>
       </c>
       <c r="JI3" s="32"/>
     </row>
     <row r="4" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="167"/>
-      <c r="B4" s="166" t="s">
+      <c r="A4" s="165"/>
+      <c r="B4" s="164" t="s">
         <v>220</v>
       </c>
-      <c r="C4" s="166"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="167"/>
-      <c r="F4" s="167"/>
-      <c r="G4" s="167"/>
-      <c r="H4" s="168"/>
-      <c r="I4" s="167"/>
-      <c r="J4" s="169"/>
-      <c r="K4" s="170"/>
-      <c r="L4" s="166"/>
-      <c r="M4" s="171"/>
-      <c r="N4" s="166"/>
-      <c r="O4" s="172"/>
-      <c r="P4" s="172"/>
-      <c r="Q4" s="172"/>
-      <c r="R4" s="171"/>
+      <c r="C4" s="164"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="165"/>
+      <c r="F4" s="165"/>
+      <c r="G4" s="165"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="165"/>
+      <c r="J4" s="167"/>
+      <c r="K4" s="168"/>
+      <c r="L4" s="164"/>
+      <c r="M4" s="169"/>
+      <c r="N4" s="164"/>
+      <c r="O4" s="170"/>
+      <c r="P4" s="170"/>
+      <c r="Q4" s="170"/>
+      <c r="R4" s="169"/>
       <c r="S4" s="189"/>
-      <c r="JB4" s="162" t="s">
+      <c r="JB4" s="160" t="s">
         <v>165</v>
       </c>
       <c r="JC4" s="27">
         <v>3</v>
       </c>
-      <c r="JD4" s="106">
+      <c r="JD4" s="105">
         <v>3</v>
       </c>
-      <c r="JE4" s="108">
+      <c r="JE4" s="107">
         <v>6</v>
       </c>
-      <c r="JF4" s="108">
+      <c r="JF4" s="107">
         <v>9</v>
       </c>
-      <c r="JG4" s="107">
+      <c r="JG4" s="106">
         <v>12</v>
       </c>
-      <c r="JH4" s="107">
+      <c r="JH4" s="106">
         <v>15</v>
       </c>
       <c r="JI4" s="32"/>
@@ -7784,26 +7795,26 @@
       <c r="F5" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="143">
+      <c r="G5" s="141">
         <v>1</v>
       </c>
-      <c r="H5" s="142">
+      <c r="H5" s="140">
         <v>3</v>
       </c>
-      <c r="I5" s="140" t="s">
+      <c r="I5" s="138" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="139" t="s">
+      <c r="J5" s="137" t="s">
         <v>40</v>
       </c>
       <c r="K5" s="35"/>
       <c r="L5" s="54" t="s">
         <v>237</v>
       </c>
-      <c r="M5" s="198" t="s">
+      <c r="M5" s="175" t="s">
         <v>238</v>
       </c>
-      <c r="N5" s="198" t="s">
+      <c r="N5" s="175" t="s">
         <v>239</v>
       </c>
       <c r="O5" s="52" t="s">
@@ -7817,12 +7828,12 @@
       </c>
       <c r="R5" s="42"/>
       <c r="S5" s="189"/>
-      <c r="JB5" s="162"/>
-      <c r="JD5" s="106"/>
-      <c r="JE5" s="108"/>
-      <c r="JF5" s="108"/>
-      <c r="JG5" s="107"/>
-      <c r="JH5" s="107"/>
+      <c r="JB5" s="160"/>
+      <c r="JD5" s="105"/>
+      <c r="JE5" s="107"/>
+      <c r="JF5" s="107"/>
+      <c r="JG5" s="106"/>
+      <c r="JH5" s="106"/>
       <c r="JI5" s="32"/>
     </row>
     <row r="6" spans="1:269" ht="25.5" x14ac:dyDescent="0.2">
@@ -7844,26 +7855,26 @@
       <c r="F6" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="G6" s="143">
+      <c r="G6" s="141">
         <v>2</v>
       </c>
-      <c r="H6" s="142">
+      <c r="H6" s="140">
         <v>1</v>
       </c>
-      <c r="I6" s="141" t="s">
+      <c r="I6" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="139" t="s">
+      <c r="J6" s="137" t="s">
         <v>236</v>
       </c>
       <c r="K6" s="35"/>
       <c r="L6" s="53" t="s">
         <v>242</v>
       </c>
-      <c r="M6" s="198" t="s">
+      <c r="M6" s="175" t="s">
         <v>243</v>
       </c>
-      <c r="N6" s="198" t="s">
+      <c r="N6" s="175" t="s">
         <v>245</v>
       </c>
       <c r="O6" s="52" t="s">
@@ -7877,25 +7888,25 @@
       </c>
       <c r="R6" s="59"/>
       <c r="S6" s="189"/>
-      <c r="JB6" s="162" t="s">
+      <c r="JB6" s="160" t="s">
         <v>166</v>
       </c>
       <c r="JC6" s="27">
         <v>2</v>
       </c>
-      <c r="JD6" s="106">
+      <c r="JD6" s="105">
         <v>2</v>
       </c>
-      <c r="JE6" s="106">
+      <c r="JE6" s="105">
         <v>4</v>
       </c>
-      <c r="JF6" s="108">
+      <c r="JF6" s="107">
         <v>6</v>
       </c>
-      <c r="JG6" s="108">
+      <c r="JG6" s="107">
         <v>8</v>
       </c>
-      <c r="JH6" s="108">
+      <c r="JH6" s="107">
         <v>10</v>
       </c>
       <c r="JI6" s="32"/>
@@ -7919,26 +7930,26 @@
       <c r="F7" s="56" t="s">
         <v>235</v>
       </c>
-      <c r="G7" s="143">
+      <c r="G7" s="141">
         <v>2</v>
       </c>
-      <c r="H7" s="142">
+      <c r="H7" s="140">
         <v>1</v>
       </c>
-      <c r="I7" s="140" t="s">
+      <c r="I7" s="138" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="139" t="s">
+      <c r="J7" s="137" t="s">
         <v>40</v>
       </c>
       <c r="K7" s="35"/>
       <c r="L7" s="53" t="s">
         <v>248</v>
       </c>
-      <c r="M7" s="198" t="s">
+      <c r="M7" s="175" t="s">
         <v>249</v>
       </c>
-      <c r="N7" s="198" t="s">
+      <c r="N7" s="175" t="s">
         <v>250</v>
       </c>
       <c r="O7" s="52" t="s">
@@ -7952,25 +7963,25 @@
       </c>
       <c r="R7" s="59"/>
       <c r="S7" s="189"/>
-      <c r="JB7" s="162" t="s">
+      <c r="JB7" s="160" t="s">
         <v>165</v>
       </c>
       <c r="JC7" s="27">
         <v>1</v>
       </c>
-      <c r="JD7" s="106">
+      <c r="JD7" s="105">
         <v>1</v>
       </c>
-      <c r="JE7" s="106">
+      <c r="JE7" s="105">
         <v>2</v>
       </c>
-      <c r="JF7" s="106">
+      <c r="JF7" s="105">
         <v>3</v>
       </c>
-      <c r="JG7" s="106">
+      <c r="JG7" s="105">
         <v>4</v>
       </c>
-      <c r="JH7" s="108">
+      <c r="JH7" s="107">
         <v>5</v>
       </c>
       <c r="JI7" s="32"/>
@@ -7994,26 +8005,26 @@
       <c r="F8" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="G8" s="143">
+      <c r="G8" s="141">
         <v>1</v>
       </c>
-      <c r="H8" s="142">
+      <c r="H8" s="140">
         <v>1</v>
       </c>
-      <c r="I8" s="141" t="s">
+      <c r="I8" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="139" t="s">
+      <c r="J8" s="137" t="s">
         <v>38</v>
       </c>
       <c r="K8" s="35"/>
       <c r="L8" s="53" t="s">
         <v>254</v>
       </c>
-      <c r="M8" s="198" t="s">
+      <c r="M8" s="175" t="s">
         <v>255</v>
       </c>
-      <c r="N8" s="198" t="s">
+      <c r="N8" s="175" t="s">
         <v>256</v>
       </c>
       <c r="O8" s="52" t="s">
@@ -8045,40 +8056,40 @@
       <c r="JI8" s="32"/>
     </row>
     <row r="9" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="173"/>
-      <c r="B9" s="174" t="s">
+      <c r="A9" s="171"/>
+      <c r="B9" s="172" t="s">
         <v>221</v>
       </c>
-      <c r="C9" s="166"/>
-      <c r="D9" s="168"/>
-      <c r="E9" s="167"/>
-      <c r="F9" s="167"/>
-      <c r="G9" s="167"/>
-      <c r="H9" s="168"/>
-      <c r="I9" s="167"/>
-      <c r="J9" s="169"/>
-      <c r="K9" s="170"/>
-      <c r="L9" s="175"/>
-      <c r="M9" s="174"/>
-      <c r="N9" s="174"/>
-      <c r="O9" s="172"/>
-      <c r="P9" s="172"/>
-      <c r="Q9" s="172"/>
-      <c r="R9" s="176"/>
+      <c r="C9" s="164"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="165"/>
+      <c r="F9" s="165"/>
+      <c r="G9" s="165"/>
+      <c r="H9" s="166"/>
+      <c r="I9" s="165"/>
+      <c r="J9" s="167"/>
+      <c r="K9" s="168"/>
+      <c r="L9" s="173"/>
+      <c r="M9" s="172"/>
+      <c r="N9" s="172"/>
+      <c r="O9" s="170"/>
+      <c r="P9" s="170"/>
+      <c r="Q9" s="170"/>
+      <c r="R9" s="174"/>
       <c r="JC9" s="32"/>
-      <c r="JD9" s="162" t="s">
+      <c r="JD9" s="160" t="s">
         <v>165</v>
       </c>
-      <c r="JE9" s="162" t="s">
+      <c r="JE9" s="160" t="s">
         <v>166</v>
       </c>
-      <c r="JF9" s="162" t="s">
+      <c r="JF9" s="160" t="s">
         <v>167</v>
       </c>
-      <c r="JG9" s="162" t="s">
+      <c r="JG9" s="160" t="s">
         <v>164</v>
       </c>
-      <c r="JH9" s="162" t="s">
+      <c r="JH9" s="160" t="s">
         <v>163</v>
       </c>
       <c r="JI9" s="32"/>
@@ -8102,23 +8113,23 @@
       <c r="F10" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="G10" s="143">
+      <c r="G10" s="141">
         <v>1</v>
       </c>
-      <c r="H10" s="142">
+      <c r="H10" s="140">
         <v>1</v>
       </c>
-      <c r="I10" s="141" t="s">
+      <c r="I10" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="139" t="s">
+      <c r="J10" s="137" t="s">
         <v>39</v>
       </c>
       <c r="K10" s="35"/>
       <c r="L10" s="53" t="s">
         <v>259</v>
       </c>
-      <c r="M10" s="198" t="s">
+      <c r="M10" s="175" t="s">
         <v>260</v>
       </c>
       <c r="N10" s="36" t="s">
@@ -8136,7 +8147,7 @@
       <c r="R10" s="59"/>
       <c r="JC10" s="32"/>
       <c r="JD10" s="32"/>
-      <c r="JE10" s="162" t="s">
+      <c r="JE10" s="160" t="s">
         <v>55</v>
       </c>
       <c r="JF10" s="34"/>
@@ -8163,26 +8174,26 @@
       <c r="F11" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="G11" s="143">
+      <c r="G11" s="141">
         <v>2</v>
       </c>
-      <c r="H11" s="142">
+      <c r="H11" s="140">
         <v>1</v>
       </c>
-      <c r="I11" s="140" t="s">
+      <c r="I11" s="138" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="139" t="s">
+      <c r="J11" s="137" t="s">
         <v>40</v>
       </c>
       <c r="K11" s="35"/>
       <c r="L11" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="M11" s="198" t="s">
+      <c r="M11" s="175" t="s">
         <v>264</v>
       </c>
-      <c r="N11" s="198" t="s">
+      <c r="N11" s="175" t="s">
         <v>244</v>
       </c>
       <c r="O11" s="52" t="s">
@@ -8222,26 +8233,26 @@
       <c r="F12" s="56" t="s">
         <v>235</v>
       </c>
-      <c r="G12" s="143">
+      <c r="G12" s="141">
         <v>3</v>
       </c>
-      <c r="H12" s="142">
+      <c r="H12" s="140">
         <v>1</v>
       </c>
-      <c r="I12" s="141" t="s">
+      <c r="I12" s="139" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="139" t="s">
+      <c r="J12" s="137" t="s">
         <v>236</v>
       </c>
       <c r="K12" s="35"/>
       <c r="L12" s="53" t="s">
         <v>266</v>
       </c>
-      <c r="M12" s="198" t="s">
+      <c r="M12" s="175" t="s">
         <v>267</v>
       </c>
-      <c r="N12" s="198" t="s">
+      <c r="N12" s="175" t="s">
         <v>268</v>
       </c>
       <c r="O12" s="52" t="s">
@@ -8254,13 +8265,13 @@
         <v>143</v>
       </c>
       <c r="R12" s="59"/>
-      <c r="JC12" s="144"/>
-      <c r="JD12" s="145" t="s">
+      <c r="JC12" s="142"/>
+      <c r="JD12" s="143" t="s">
         <v>56</v>
       </c>
-      <c r="JE12" s="131"/>
-      <c r="JF12" s="131"/>
-      <c r="JG12" s="131"/>
+      <c r="JE12" s="129"/>
+      <c r="JF12" s="129"/>
+      <c r="JG12" s="129"/>
       <c r="JH12" s="32"/>
       <c r="JI12" s="32"/>
     </row>
@@ -8283,26 +8294,26 @@
       <c r="F13" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="G13" s="143">
+      <c r="G13" s="141">
         <v>1</v>
       </c>
-      <c r="H13" s="142">
+      <c r="H13" s="140">
         <v>3</v>
       </c>
-      <c r="I13" s="141" t="s">
+      <c r="I13" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="J13" s="139" t="s">
+      <c r="J13" s="137" t="s">
         <v>39</v>
       </c>
       <c r="K13" s="35"/>
       <c r="L13" s="53" t="s">
         <v>270</v>
       </c>
-      <c r="M13" s="198" t="s">
+      <c r="M13" s="175" t="s">
         <v>271</v>
       </c>
-      <c r="N13" s="198" t="s">
+      <c r="N13" s="175" t="s">
         <v>272</v>
       </c>
       <c r="O13" s="52" t="s">
@@ -8321,9 +8332,9 @@
       <c r="JD13" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="JE13" s="131"/>
-      <c r="JF13" s="132"/>
-      <c r="JG13" s="132"/>
+      <c r="JE13" s="129"/>
+      <c r="JF13" s="130"/>
+      <c r="JG13" s="130"/>
       <c r="JH13" s="32"/>
       <c r="JI13" s="32"/>
     </row>
@@ -8336,10 +8347,10 @@
       <c r="D14" s="73"/>
       <c r="E14" s="56"/>
       <c r="F14" s="56"/>
-      <c r="G14" s="143"/>
-      <c r="H14" s="142"/>
-      <c r="I14" s="141"/>
-      <c r="J14" s="139"/>
+      <c r="G14" s="141"/>
+      <c r="H14" s="140"/>
+      <c r="I14" s="139"/>
+      <c r="J14" s="137"/>
       <c r="K14" s="35"/>
       <c r="L14" s="55"/>
       <c r="M14" s="59"/>
@@ -8354,12 +8365,12 @@
       <c r="JD14" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="JE14" s="131"/>
-      <c r="JF14" s="132" t="s">
+      <c r="JE14" s="129"/>
+      <c r="JF14" s="130" t="s">
         <v>143</v>
       </c>
-      <c r="JG14" s="132"/>
-      <c r="JH14" s="130"/>
+      <c r="JG14" s="130"/>
+      <c r="JH14" s="128"/>
       <c r="JI14" s="32"/>
     </row>
     <row r="15" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
@@ -8371,10 +8382,10 @@
       <c r="D15" s="73"/>
       <c r="E15" s="56"/>
       <c r="F15" s="56"/>
-      <c r="G15" s="143"/>
-      <c r="H15" s="142"/>
-      <c r="I15" s="140"/>
-      <c r="J15" s="139"/>
+      <c r="G15" s="141"/>
+      <c r="H15" s="140"/>
+      <c r="I15" s="138"/>
+      <c r="J15" s="137"/>
       <c r="K15" s="35"/>
       <c r="L15" s="53"/>
       <c r="M15" s="53"/>
@@ -8389,12 +8400,12 @@
       <c r="JD15" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="JE15" s="132"/>
-      <c r="JF15" s="132" t="s">
+      <c r="JE15" s="130"/>
+      <c r="JF15" s="130" t="s">
         <v>144</v>
       </c>
-      <c r="JG15" s="132"/>
-      <c r="JH15" s="129"/>
+      <c r="JG15" s="130"/>
+      <c r="JH15" s="127"/>
       <c r="JI15" s="28"/>
     </row>
     <row r="16" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
@@ -8404,10 +8415,10 @@
       <c r="D16" s="73"/>
       <c r="E16" s="56"/>
       <c r="F16" s="56"/>
-      <c r="G16" s="143"/>
-      <c r="H16" s="142"/>
-      <c r="I16" s="141"/>
-      <c r="J16" s="139"/>
+      <c r="G16" s="141"/>
+      <c r="H16" s="140"/>
+      <c r="I16" s="139"/>
+      <c r="J16" s="137"/>
       <c r="K16" s="35"/>
       <c r="L16" s="53"/>
       <c r="M16" s="53"/>
@@ -8422,12 +8433,12 @@
       <c r="JD16" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="JE16" s="132"/>
-      <c r="JF16" s="133" t="s">
+      <c r="JE16" s="130"/>
+      <c r="JF16" s="131" t="s">
         <v>145</v>
       </c>
-      <c r="JG16" s="131"/>
-      <c r="JH16" s="129"/>
+      <c r="JG16" s="129"/>
+      <c r="JH16" s="127"/>
       <c r="JI16" s="32"/>
     </row>
     <row r="17" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
@@ -8437,10 +8448,10 @@
       <c r="D17" s="73"/>
       <c r="E17" s="56"/>
       <c r="F17" s="56"/>
-      <c r="G17" s="143"/>
-      <c r="H17" s="142"/>
-      <c r="I17" s="140"/>
-      <c r="J17" s="139"/>
+      <c r="G17" s="141"/>
+      <c r="H17" s="140"/>
+      <c r="I17" s="138"/>
+      <c r="J17" s="137"/>
       <c r="K17" s="35"/>
       <c r="L17" s="55"/>
       <c r="M17" s="53"/>
@@ -8455,12 +8466,12 @@
       <c r="JD17" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="JE17" s="132"/>
-      <c r="JF17" s="133" t="s">
+      <c r="JE17" s="130"/>
+      <c r="JF17" s="131" t="s">
         <v>146</v>
       </c>
-      <c r="JG17" s="131"/>
-      <c r="JH17" s="129"/>
+      <c r="JG17" s="129"/>
+      <c r="JH17" s="127"/>
       <c r="JI17" s="32"/>
     </row>
     <row r="18" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
@@ -8470,10 +8481,10 @@
       <c r="D18" s="73"/>
       <c r="E18" s="56"/>
       <c r="F18" s="56"/>
-      <c r="G18" s="143"/>
-      <c r="H18" s="142"/>
-      <c r="I18" s="141"/>
-      <c r="J18" s="139"/>
+      <c r="G18" s="141"/>
+      <c r="H18" s="140"/>
+      <c r="I18" s="139"/>
+      <c r="J18" s="137"/>
       <c r="K18" s="35"/>
       <c r="L18" s="53"/>
       <c r="M18" s="53"/>
@@ -8488,12 +8499,12 @@
       <c r="JD18" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="JE18" s="131"/>
-      <c r="JF18" s="133" t="s">
+      <c r="JE18" s="129"/>
+      <c r="JF18" s="131" t="s">
         <v>147</v>
       </c>
-      <c r="JG18" s="131"/>
-      <c r="JH18" s="130"/>
+      <c r="JG18" s="129"/>
+      <c r="JH18" s="128"/>
       <c r="JI18" s="32"/>
     </row>
     <row r="19" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
@@ -8503,10 +8514,10 @@
       <c r="D19" s="73"/>
       <c r="E19" s="56"/>
       <c r="F19" s="56"/>
-      <c r="G19" s="143"/>
-      <c r="H19" s="142"/>
-      <c r="I19" s="141"/>
-      <c r="J19" s="139"/>
+      <c r="G19" s="141"/>
+      <c r="H19" s="140"/>
+      <c r="I19" s="139"/>
+      <c r="J19" s="137"/>
       <c r="K19" s="35"/>
       <c r="L19" s="53"/>
       <c r="M19" s="59"/>
@@ -8521,12 +8532,12 @@
       <c r="JD19" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="JE19" s="131"/>
-      <c r="JF19" s="132" t="s">
+      <c r="JE19" s="129"/>
+      <c r="JF19" s="130" t="s">
         <v>148</v>
       </c>
-      <c r="JG19" s="132"/>
-      <c r="JH19" s="130"/>
+      <c r="JG19" s="130"/>
+      <c r="JH19" s="128"/>
       <c r="JI19" s="32"/>
     </row>
     <row r="20" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
@@ -8536,10 +8547,10 @@
       <c r="D20" s="73"/>
       <c r="E20" s="56"/>
       <c r="F20" s="56"/>
-      <c r="G20" s="143"/>
-      <c r="H20" s="142"/>
-      <c r="I20" s="140"/>
-      <c r="J20" s="139"/>
+      <c r="G20" s="141"/>
+      <c r="H20" s="140"/>
+      <c r="I20" s="138"/>
+      <c r="J20" s="137"/>
       <c r="K20" s="35"/>
       <c r="L20" s="55"/>
       <c r="M20" s="59"/>
@@ -8554,12 +8565,12 @@
       <c r="JD20" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="JE20" s="131"/>
-      <c r="JF20" s="132" t="s">
+      <c r="JE20" s="129"/>
+      <c r="JF20" s="130" t="s">
         <v>149</v>
       </c>
-      <c r="JG20" s="132"/>
-      <c r="JH20" s="130"/>
+      <c r="JG20" s="130"/>
+      <c r="JH20" s="128"/>
       <c r="JI20" s="32"/>
     </row>
     <row r="21" spans="1:269" s="39" customFormat="1" ht="35.25" x14ac:dyDescent="0.3">
@@ -8569,10 +8580,10 @@
       <c r="D21" s="73"/>
       <c r="E21" s="56"/>
       <c r="F21" s="56"/>
-      <c r="G21" s="143"/>
-      <c r="H21" s="142"/>
-      <c r="I21" s="141"/>
-      <c r="J21" s="139"/>
+      <c r="G21" s="141"/>
+      <c r="H21" s="140"/>
+      <c r="I21" s="139"/>
+      <c r="J21" s="137"/>
       <c r="K21" s="35"/>
       <c r="L21" s="53"/>
       <c r="M21" s="59"/>
@@ -8588,10 +8599,10 @@
       <c r="JD21" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="JE21" s="132"/>
-      <c r="JF21" s="132"/>
-      <c r="JG21" s="132"/>
-      <c r="JH21" s="129"/>
+      <c r="JE21" s="130"/>
+      <c r="JF21" s="130"/>
+      <c r="JG21" s="130"/>
+      <c r="JH21" s="127"/>
       <c r="JI21" s="32"/>
     </row>
     <row r="22" spans="1:269" s="37" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8601,10 +8612,10 @@
       <c r="D22" s="73"/>
       <c r="E22" s="56"/>
       <c r="F22" s="56"/>
-      <c r="G22" s="143"/>
-      <c r="H22" s="142"/>
-      <c r="I22" s="140"/>
-      <c r="J22" s="139"/>
+      <c r="G22" s="141"/>
+      <c r="H22" s="140"/>
+      <c r="I22" s="138"/>
+      <c r="J22" s="137"/>
       <c r="K22" s="35"/>
       <c r="L22" s="53"/>
       <c r="M22" s="59"/>
@@ -8625,10 +8636,10 @@
       <c r="JD22" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="JE22" s="132"/>
-      <c r="JF22" s="132"/>
-      <c r="JG22" s="132"/>
-      <c r="JH22" s="129"/>
+      <c r="JE22" s="130"/>
+      <c r="JF22" s="130"/>
+      <c r="JG22" s="130"/>
+      <c r="JH22" s="127"/>
       <c r="JI22" s="32"/>
     </row>
     <row r="23" spans="1:269" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8656,9 +8667,9 @@
       <c r="JD23" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="JE23" s="132"/>
-      <c r="JF23" s="131"/>
-      <c r="JG23" s="131"/>
+      <c r="JE23" s="130"/>
+      <c r="JF23" s="129"/>
+      <c r="JG23" s="129"/>
       <c r="JH23" s="34"/>
       <c r="JI23" s="32"/>
     </row>
@@ -8781,13 +8792,13 @@
       <c r="JD30" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="JE30" s="122" t="s">
+      <c r="JE30" s="121" t="s">
         <v>58</v>
       </c>
-      <c r="JF30" s="122" t="s">
+      <c r="JF30" s="121" t="s">
         <v>57</v>
       </c>
-      <c r="JG30" s="122" t="s">
+      <c r="JG30" s="121" t="s">
         <v>106</v>
       </c>
       <c r="JH30" s="32"/>
@@ -8798,17 +8809,17 @@
       <c r="J31" s="32"/>
       <c r="K31" s="31"/>
       <c r="L31" s="33"/>
-      <c r="JC31" s="109"/>
-      <c r="JD31" s="112" t="s">
+      <c r="JC31" s="108"/>
+      <c r="JD31" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="JE31" s="124" t="s">
+      <c r="JE31" s="123" t="s">
         <v>85</v>
       </c>
-      <c r="JF31" s="125" t="s">
+      <c r="JF31" s="124" t="s">
         <v>138</v>
       </c>
-      <c r="JG31" s="125" t="s">
+      <c r="JG31" s="124" t="s">
         <v>139</v>
       </c>
       <c r="JH31" s="32"/>
@@ -8819,17 +8830,17 @@
       <c r="J32" s="32"/>
       <c r="K32" s="31"/>
       <c r="L32" s="33"/>
-      <c r="JC32" s="110"/>
-      <c r="JD32" s="112" t="s">
+      <c r="JC32" s="109"/>
+      <c r="JD32" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="JE32" s="124" t="s">
+      <c r="JE32" s="123" t="s">
         <v>86</v>
       </c>
-      <c r="JF32" s="124" t="s">
+      <c r="JF32" s="123" t="s">
         <v>137</v>
       </c>
-      <c r="JG32" s="125" t="s">
+      <c r="JG32" s="124" t="s">
         <v>140</v>
       </c>
       <c r="JH32" s="32"/>
@@ -8840,17 +8851,17 @@
       <c r="J33" s="32"/>
       <c r="K33" s="31"/>
       <c r="L33" s="33"/>
-      <c r="JC33" s="111"/>
-      <c r="JD33" s="112" t="s">
+      <c r="JC33" s="110"/>
+      <c r="JD33" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="JE33" s="124" t="s">
+      <c r="JE33" s="123" t="s">
         <v>87</v>
       </c>
-      <c r="JF33" s="125" t="s">
+      <c r="JF33" s="124" t="s">
         <v>135</v>
       </c>
-      <c r="JG33" s="125" t="s">
+      <c r="JG33" s="124" t="s">
         <v>141</v>
       </c>
       <c r="JH33" s="32"/>
@@ -9122,8 +9133,8 @@
     </row>
     <row r="63" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A63" s="32"/>
-      <c r="B63" s="123"/>
-      <c r="C63" s="123"/>
+      <c r="B63" s="122"/>
+      <c r="C63" s="122"/>
       <c r="D63" s="32"/>
       <c r="E63" s="32"/>
       <c r="F63" s="32"/>
@@ -9138,10 +9149,10 @@
     </row>
     <row r="64" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A64" s="32"/>
-      <c r="B64" s="123" t="s">
+      <c r="B64" s="122" t="s">
         <v>83</v>
       </c>
-      <c r="C64" s="123" t="s">
+      <c r="C64" s="122" t="s">
         <v>85</v>
       </c>
       <c r="D64" s="32"/>
@@ -9158,10 +9169,10 @@
     </row>
     <row r="65" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A65" s="32"/>
-      <c r="B65" s="123" t="s">
+      <c r="B65" s="122" t="s">
         <v>84</v>
       </c>
-      <c r="C65" s="123" t="s">
+      <c r="C65" s="122" t="s">
         <v>86</v>
       </c>
       <c r="D65" s="32"/>
@@ -9178,10 +9189,10 @@
     </row>
     <row r="66" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A66" s="32"/>
-      <c r="B66" s="123" t="s">
+      <c r="B66" s="122" t="s">
         <v>136</v>
       </c>
-      <c r="C66" s="123" t="s">
+      <c r="C66" s="122" t="s">
         <v>87</v>
       </c>
       <c r="D66" s="32"/>
@@ -9198,8 +9209,8 @@
     </row>
     <row r="67" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A67" s="32"/>
-      <c r="B67" s="123"/>
-      <c r="C67" s="123"/>
+      <c r="B67" s="122"/>
+      <c r="C67" s="122"/>
       <c r="D67" s="32"/>
       <c r="E67" s="32"/>
       <c r="F67" s="32"/>
@@ -9214,8 +9225,8 @@
     </row>
     <row r="68" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A68" s="32"/>
-      <c r="B68" s="123"/>
-      <c r="C68" s="123"/>
+      <c r="B68" s="122"/>
+      <c r="C68" s="122"/>
       <c r="D68" s="32"/>
       <c r="E68" s="32"/>
       <c r="F68" s="32"/>
@@ -9230,8 +9241,8 @@
     </row>
     <row r="69" spans="1:17" s="31" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="32"/>
-      <c r="B69" s="123"/>
-      <c r="C69" s="123"/>
+      <c r="B69" s="122"/>
+      <c r="C69" s="122"/>
       <c r="D69" s="32"/>
       <c r="E69" s="28"/>
       <c r="F69" s="28"/>
@@ -10141,10 +10152,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="157" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="159" t="s">
+      <c r="B3" s="157" t="s">
         <v>90</v>
       </c>
     </row>
@@ -10584,39 +10595,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="62.85546875" style="92" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" style="92" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" style="92" customWidth="1"/>
     <col min="3" max="3" width="36" style="92" customWidth="1"/>
     <col min="4" max="16384" width="11.42578125" style="92"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="113"/>
+      <c r="C2" s="112"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="157" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="160" t="s">
+      <c r="B3" s="158" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="114"/>
-    </row>
-    <row r="4" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="127" t="s">
-        <v>281</v>
-      </c>
-      <c r="B4" s="115" t="s">
-        <v>282</v>
-      </c>
-      <c r="C4" s="114"/>
+      <c r="C3" s="113"/>
+    </row>
+    <row r="4" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="125" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4" s="114" t="s">
+        <v>289</v>
+      </c>
+      <c r="C4" s="113"/>
       <c r="D4" s="100"/>
       <c r="E4" s="100"/>
       <c r="F4" s="100"/>
@@ -10626,13 +10637,13 @@
       <c r="H4" s="100"/>
     </row>
     <row r="5" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="128" t="s">
-        <v>283</v>
-      </c>
-      <c r="B5" s="115" t="s">
-        <v>284</v>
-      </c>
-      <c r="C5" s="114"/>
+      <c r="A5" s="126" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="114" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="113"/>
       <c r="D5" s="100"/>
       <c r="E5" s="100"/>
       <c r="F5" s="100"/>
@@ -10641,10 +10652,14 @@
       </c>
       <c r="H5" s="100"/>
     </row>
-    <row r="6" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="128"/>
-      <c r="B6" s="115"/>
-      <c r="C6" s="114"/>
+    <row r="6" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="126" t="s">
+        <v>292</v>
+      </c>
+      <c r="B6" s="114" t="s">
+        <v>293</v>
+      </c>
+      <c r="C6" s="113"/>
       <c r="D6" s="100"/>
       <c r="E6" s="100"/>
       <c r="F6" s="100"/>
@@ -10656,22 +10671,22 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="159" t="s">
+      <c r="A7" s="157" t="s">
         <v>105</v>
       </c>
-      <c r="B7" s="159" t="s">
+      <c r="B7" s="157" t="s">
         <v>106</v>
       </c>
-      <c r="C7" s="161" t="s">
+      <c r="C7" s="159" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="127" t="s">
-        <v>285</v>
+    <row r="8" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="125" t="s">
+        <v>294</v>
       </c>
       <c r="B8" s="101" t="s">
-        <v>286</v>
+        <v>308</v>
       </c>
       <c r="C8" s="94" t="s">
         <v>108</v>
@@ -10690,11 +10705,11 @@
       <c r="J8" s="100"/>
     </row>
     <row r="9" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="128" t="s">
-        <v>287</v>
+      <c r="A9" s="126" t="s">
+        <v>295</v>
       </c>
       <c r="B9" s="102" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="C9" s="94" t="s">
         <v>108</v>
@@ -10707,13 +10722,13 @@
       <c r="J9" s="100"/>
     </row>
     <row r="10" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="199" t="s">
-        <v>290</v>
+      <c r="A10" s="176" t="s">
+        <v>297</v>
       </c>
       <c r="B10" s="103" t="s">
-        <v>289</v>
-      </c>
-      <c r="C10" s="126" t="s">
+        <v>298</v>
+      </c>
+      <c r="C10" s="94" t="s">
         <v>108</v>
       </c>
       <c r="E10" s="100"/>
@@ -10721,12 +10736,12 @@
       <c r="G10" s="100"/>
       <c r="H10" s="100"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="128" t="s">
-        <v>291</v>
+    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="126" t="s">
+        <v>299</v>
       </c>
       <c r="B11" s="102" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="C11" s="94" t="s">
         <v>108</v>
@@ -10737,9 +10752,15 @@
       <c r="H11" s="100"/>
     </row>
     <row r="12" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="128"/>
-      <c r="B12" s="102"/>
-      <c r="C12" s="126"/>
+      <c r="A12" s="126" t="s">
+        <v>301</v>
+      </c>
+      <c r="B12" s="102" t="s">
+        <v>302</v>
+      </c>
+      <c r="C12" s="94" t="s">
+        <v>108</v>
+      </c>
       <c r="D12" s="100"/>
       <c r="E12" s="100"/>
       <c r="F12" s="100"/>
@@ -10747,9 +10768,15 @@
       <c r="H12" s="100"/>
     </row>
     <row r="13" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="128"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="126"/>
+      <c r="A13" s="126" t="s">
+        <v>303</v>
+      </c>
+      <c r="B13" s="104" t="s">
+        <v>304</v>
+      </c>
+      <c r="C13" s="94" t="s">
+        <v>108</v>
+      </c>
       <c r="D13" s="100"/>
       <c r="E13" s="100"/>
       <c r="F13" s="100"/>
@@ -10757,9 +10784,15 @@
       <c r="H13" s="100"/>
     </row>
     <row r="14" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="128"/>
-      <c r="B14" s="104"/>
-      <c r="C14" s="94"/>
+      <c r="A14" s="126" t="s">
+        <v>305</v>
+      </c>
+      <c r="B14" s="104" t="s">
+        <v>306</v>
+      </c>
+      <c r="C14" s="94" t="s">
+        <v>109</v>
+      </c>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
       <c r="F14" s="100"/>
@@ -10767,9 +10800,15 @@
       <c r="H14" s="100"/>
     </row>
     <row r="15" spans="1:10" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="128"/>
-      <c r="B15" s="105"/>
-      <c r="C15" s="94"/>
+      <c r="A15" s="126" t="s">
+        <v>307</v>
+      </c>
+      <c r="B15" s="101" t="s">
+        <v>308</v>
+      </c>
+      <c r="C15" s="94" t="s">
+        <v>108</v>
+      </c>
       <c r="D15" s="100"/>
       <c r="E15" s="100"/>
       <c r="F15" s="100"/>
@@ -10777,9 +10816,15 @@
       <c r="H15" s="100"/>
     </row>
     <row r="16" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="128"/>
-      <c r="B16" s="102"/>
-      <c r="C16" s="126"/>
+      <c r="A16" s="126" t="s">
+        <v>309</v>
+      </c>
+      <c r="B16" s="102" t="s">
+        <v>310</v>
+      </c>
+      <c r="C16" s="94" t="s">
+        <v>108</v>
+      </c>
       <c r="D16" s="100"/>
       <c r="E16" s="100"/>
       <c r="F16" s="100"/>
@@ -10921,7 +10966,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C9 C11 C14:C15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C16">
       <formula1>$F$8:$G$8</formula1>
     </dataValidation>
   </dataValidations>
@@ -11714,15 +11759,15 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="150"/>
-      <c r="B2" s="151" t="s">
+      <c r="A2" s="148"/>
+      <c r="B2" s="149" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="121"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="120"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
@@ -11735,18 +11780,18 @@
       <c r="D3" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117" t="s">
+      <c r="G3" s="116"/>
+      <c r="H3" s="116" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="117" t="s">
+      <c r="I3" s="116" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="67" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>114</v>
@@ -11754,11 +11799,11 @@
       <c r="D4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="117"/>
-      <c r="H4" s="117" t="s">
+      <c r="G4" s="116"/>
+      <c r="H4" s="116" t="s">
         <v>114</v>
       </c>
-      <c r="I4" s="117" t="s">
+      <c r="I4" s="116" t="s">
         <v>9</v>
       </c>
     </row>
@@ -11773,13 +11818,13 @@
       <c r="D5" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="G5" s="117"/>
-      <c r="H5" s="117"/>
-      <c r="I5" s="117"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="116"/>
     </row>
     <row r="6" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="62" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>114</v>
@@ -11787,9 +11832,9 @@
       <c r="D6" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="117" t="s">
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="116" t="s">
         <v>116</v>
       </c>
     </row>
@@ -11803,9 +11848,9 @@
       <c r="D7" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="118"/>
-      <c r="H7" s="118"/>
-      <c r="I7" s="117" t="s">
+      <c r="G7" s="117"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="116" t="s">
         <v>117</v>
       </c>
     </row>
@@ -11819,15 +11864,15 @@
       <c r="D8" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G8" s="118"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="119" t="s">
+      <c r="G8" s="117"/>
+      <c r="H8" s="117"/>
+      <c r="I8" s="118" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="62" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>113</v>
@@ -11835,9 +11880,9 @@
       <c r="D9" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="119" t="s">
+      <c r="G9" s="117"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="118" t="s">
         <v>121</v>
       </c>
     </row>
@@ -11851,9 +11896,9 @@
       <c r="D10" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="G10" s="118"/>
-      <c r="H10" s="118"/>
-      <c r="I10" s="119" t="s">
+      <c r="G10" s="117"/>
+      <c r="H10" s="117"/>
+      <c r="I10" s="118" t="s">
         <v>130</v>
       </c>
     </row>
@@ -11867,9 +11912,9 @@
       <c r="D11" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="119" t="s">
+      <c r="G11" s="117"/>
+      <c r="H11" s="117"/>
+      <c r="I11" s="118" t="s">
         <v>131</v>
       </c>
     </row>
@@ -11883,9 +11928,9 @@
       <c r="D12" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="119"/>
+      <c r="G12" s="117"/>
+      <c r="H12" s="117"/>
+      <c r="I12" s="118"/>
     </row>
     <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
@@ -11897,19 +11942,19 @@
       <c r="D13" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="G13" s="117"/>
-      <c r="H13" s="117"/>
-      <c r="I13" s="117"/>
+      <c r="G13" s="116"/>
+      <c r="H13" s="116"/>
+      <c r="I13" s="116"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G14" s="117"/>
-      <c r="H14" s="117"/>
-      <c r="I14" s="120"/>
+      <c r="G14" s="116"/>
+      <c r="H14" s="116"/>
+      <c r="I14" s="119"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="119"/>
+      <c r="G15" s="117"/>
+      <c r="H15" s="117"/>
+      <c r="I15" s="118"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I16" s="83"/>
@@ -11940,7 +11985,7 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:D5"/>
     </sheetView>
   </sheetViews>
@@ -12717,15 +12762,15 @@
       <c r="A1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="150"/>
-      <c r="B2" s="151" t="s">
+      <c r="A2" s="148"/>
+      <c r="B2" s="149" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="150"/>
-      <c r="D2" s="150"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
@@ -12734,38 +12779,38 @@
       </c>
       <c r="C3" s="197"/>
       <c r="D3" s="197"/>
-      <c r="G3" s="117"/>
-      <c r="H3" s="117" t="s">
+      <c r="G3" s="116"/>
+      <c r="H3" s="116" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="117" t="s">
+      <c r="I3" s="116" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="196" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="C4" s="196"/>
       <c r="D4" s="196"/>
-      <c r="G4" s="117"/>
-      <c r="H4" s="117" t="s">
+      <c r="G4" s="116"/>
+      <c r="H4" s="116" t="s">
         <v>114</v>
       </c>
-      <c r="I4" s="117" t="s">
+      <c r="I4" s="116" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="196" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="C5" s="196"/>
       <c r="D5" s="196"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="117" t="s">
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="116" t="s">
         <v>117</v>
       </c>
     </row>
@@ -12775,9 +12820,9 @@
       </c>
       <c r="C6" s="196"/>
       <c r="D6" s="196"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="119"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="196" t="s">
@@ -12785,9 +12830,9 @@
       </c>
       <c r="C7" s="196"/>
       <c r="D7" s="196"/>
-      <c r="G7" s="118"/>
-      <c r="H7" s="118"/>
-      <c r="I7" s="119"/>
+      <c r="G7" s="117"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="118"/>
     </row>
     <row r="8" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="196" t="s">
@@ -12795,9 +12840,9 @@
       </c>
       <c r="C8" s="196"/>
       <c r="D8" s="196"/>
-      <c r="G8" s="118"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="119"/>
+      <c r="G8" s="117"/>
+      <c r="H8" s="117"/>
+      <c r="I8" s="118"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="196" t="s">
@@ -12805,30 +12850,30 @@
       </c>
       <c r="C9" s="196"/>
       <c r="D9" s="196"/>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="119"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="117"/>
+      <c r="I9" s="118"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G10" s="117"/>
-      <c r="H10" s="117"/>
-      <c r="I10" s="117"/>
+      <c r="G10" s="116"/>
+      <c r="H10" s="116"/>
+      <c r="I10" s="116"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="G11" s="117"/>
-      <c r="H11" s="117"/>
-      <c r="I11" s="120"/>
+      <c r="G11" s="116"/>
+      <c r="H11" s="116"/>
+      <c r="I11" s="119"/>
     </row>
     <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="150"/>
-      <c r="B12" s="151" t="s">
+      <c r="A12" s="148"/>
+      <c r="B12" s="149" t="s">
         <v>124</v>
       </c>
-      <c r="C12" s="150"/>
-      <c r="D12" s="150"/>
-      <c r="G12" s="117"/>
-      <c r="H12" s="117"/>
-      <c r="I12" s="117"/>
+      <c r="C12" s="148"/>
+      <c r="D12" s="148"/>
+      <c r="G12" s="116"/>
+      <c r="H12" s="116"/>
+      <c r="I12" s="116"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
@@ -12837,11 +12882,11 @@
       </c>
       <c r="C13" s="197"/>
       <c r="D13" s="197"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="117" t="s">
+      <c r="G13" s="116"/>
+      <c r="H13" s="116" t="s">
         <v>113</v>
       </c>
-      <c r="I13" s="117" t="s">
+      <c r="I13" s="116" t="s">
         <v>115</v>
       </c>
     </row>
@@ -12852,11 +12897,11 @@
       </c>
       <c r="C14" s="196"/>
       <c r="D14" s="196"/>
-      <c r="G14" s="117"/>
-      <c r="H14" s="117" t="s">
+      <c r="G14" s="116"/>
+      <c r="H14" s="116" t="s">
         <v>114</v>
       </c>
-      <c r="I14" s="117" t="s">
+      <c r="I14" s="116" t="s">
         <v>9</v>
       </c>
     </row>
@@ -12866,31 +12911,31 @@
       </c>
       <c r="C15" s="196"/>
       <c r="D15" s="196"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="117" t="s">
+      <c r="G15" s="117"/>
+      <c r="H15" s="117"/>
+      <c r="I15" s="116" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="196" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="C16" s="196"/>
       <c r="D16" s="196"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="119"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="117"/>
+      <c r="I16" s="118"/>
     </row>
     <row r="17" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="196" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="C17" s="196"/>
       <c r="D17" s="196"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="119"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="117"/>
+      <c r="I17" s="118"/>
     </row>
     <row r="18" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="196" t="s">
@@ -12898,9 +12943,9 @@
       </c>
       <c r="C18" s="196"/>
       <c r="D18" s="196"/>
-      <c r="G18" s="118"/>
-      <c r="H18" s="118"/>
-      <c r="I18" s="119"/>
+      <c r="G18" s="117"/>
+      <c r="H18" s="117"/>
+      <c r="I18" s="118"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="196" t="s">
@@ -12908,12 +12953,19 @@
       </c>
       <c r="C19" s="196"/>
       <c r="D19" s="196"/>
-      <c r="G19" s="118"/>
-      <c r="H19" s="118"/>
-      <c r="I19" s="119"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B3:D3"/>
@@ -12921,13 +12973,6 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="IS65533:IS65542 SO65533:SO65542 ACK65533:ACK65542 AMG65533:AMG65542 AWC65533:AWC65542 BFY65533:BFY65542 BPU65533:BPU65542 BZQ65533:BZQ65542 CJM65533:CJM65542 CTI65533:CTI65542 DDE65533:DDE65542 DNA65533:DNA65542 DWW65533:DWW65542 EGS65533:EGS65542 EQO65533:EQO65542 FAK65533:FAK65542 FKG65533:FKG65542 FUC65533:FUC65542 GDY65533:GDY65542 GNU65533:GNU65542 GXQ65533:GXQ65542 HHM65533:HHM65542 HRI65533:HRI65542 IBE65533:IBE65542 ILA65533:ILA65542 IUW65533:IUW65542 JES65533:JES65542 JOO65533:JOO65542 JYK65533:JYK65542 KIG65533:KIG65542 KSC65533:KSC65542 LBY65533:LBY65542 LLU65533:LLU65542 LVQ65533:LVQ65542 MFM65533:MFM65542 MPI65533:MPI65542 MZE65533:MZE65542 NJA65533:NJA65542 NSW65533:NSW65542 OCS65533:OCS65542 OMO65533:OMO65542 OWK65533:OWK65542 PGG65533:PGG65542 PQC65533:PQC65542 PZY65533:PZY65542 QJU65533:QJU65542 QTQ65533:QTQ65542 RDM65533:RDM65542 RNI65533:RNI65542 RXE65533:RXE65542 SHA65533:SHA65542 SQW65533:SQW65542 TAS65533:TAS65542 TKO65533:TKO65542 TUK65533:TUK65542 UEG65533:UEG65542 UOC65533:UOC65542 UXY65533:UXY65542 VHU65533:VHU65542 VRQ65533:VRQ65542 WBM65533:WBM65542 WLI65533:WLI65542 WVE65533:WVE65542 IS131069:IS131078 SO131069:SO131078 ACK131069:ACK131078 AMG131069:AMG131078 AWC131069:AWC131078 BFY131069:BFY131078 BPU131069:BPU131078 BZQ131069:BZQ131078 CJM131069:CJM131078 CTI131069:CTI131078 DDE131069:DDE131078 DNA131069:DNA131078 DWW131069:DWW131078 EGS131069:EGS131078 EQO131069:EQO131078 FAK131069:FAK131078 FKG131069:FKG131078 FUC131069:FUC131078 GDY131069:GDY131078 GNU131069:GNU131078 GXQ131069:GXQ131078 HHM131069:HHM131078 HRI131069:HRI131078 IBE131069:IBE131078 ILA131069:ILA131078 IUW131069:IUW131078 JES131069:JES131078 JOO131069:JOO131078 JYK131069:JYK131078 KIG131069:KIG131078 KSC131069:KSC131078 LBY131069:LBY131078 LLU131069:LLU131078 LVQ131069:LVQ131078 MFM131069:MFM131078 MPI131069:MPI131078 MZE131069:MZE131078 NJA131069:NJA131078 NSW131069:NSW131078 OCS131069:OCS131078 OMO131069:OMO131078 OWK131069:OWK131078 PGG131069:PGG131078 PQC131069:PQC131078 PZY131069:PZY131078 QJU131069:QJU131078 QTQ131069:QTQ131078 RDM131069:RDM131078 RNI131069:RNI131078 RXE131069:RXE131078 SHA131069:SHA131078 SQW131069:SQW131078 TAS131069:TAS131078 TKO131069:TKO131078 TUK131069:TUK131078 UEG131069:UEG131078 UOC131069:UOC131078 UXY131069:UXY131078 VHU131069:VHU131078 VRQ131069:VRQ131078 WBM131069:WBM131078 WLI131069:WLI131078 WVE131069:WVE131078 IS196605:IS196614 SO196605:SO196614 ACK196605:ACK196614 AMG196605:AMG196614 AWC196605:AWC196614 BFY196605:BFY196614 BPU196605:BPU196614 BZQ196605:BZQ196614 CJM196605:CJM196614 CTI196605:CTI196614 DDE196605:DDE196614 DNA196605:DNA196614 DWW196605:DWW196614 EGS196605:EGS196614 EQO196605:EQO196614 FAK196605:FAK196614 FKG196605:FKG196614 FUC196605:FUC196614 GDY196605:GDY196614 GNU196605:GNU196614 GXQ196605:GXQ196614 HHM196605:HHM196614 HRI196605:HRI196614 IBE196605:IBE196614 ILA196605:ILA196614 IUW196605:IUW196614 JES196605:JES196614 JOO196605:JOO196614 JYK196605:JYK196614 KIG196605:KIG196614 KSC196605:KSC196614 LBY196605:LBY196614 LLU196605:LLU196614 LVQ196605:LVQ196614 MFM196605:MFM196614 MPI196605:MPI196614 MZE196605:MZE196614 NJA196605:NJA196614 NSW196605:NSW196614 OCS196605:OCS196614 OMO196605:OMO196614 OWK196605:OWK196614 PGG196605:PGG196614 PQC196605:PQC196614 PZY196605:PZY196614 QJU196605:QJU196614 QTQ196605:QTQ196614 RDM196605:RDM196614 RNI196605:RNI196614 RXE196605:RXE196614 SHA196605:SHA196614 SQW196605:SQW196614 TAS196605:TAS196614 TKO196605:TKO196614 TUK196605:TUK196614 UEG196605:UEG196614 UOC196605:UOC196614 UXY196605:UXY196614 VHU196605:VHU196614 VRQ196605:VRQ196614 WBM196605:WBM196614 WLI196605:WLI196614 WVE196605:WVE196614 IS262141:IS262150 SO262141:SO262150 ACK262141:ACK262150 AMG262141:AMG262150 AWC262141:AWC262150 BFY262141:BFY262150 BPU262141:BPU262150 BZQ262141:BZQ262150 CJM262141:CJM262150 CTI262141:CTI262150 DDE262141:DDE262150 DNA262141:DNA262150 DWW262141:DWW262150 EGS262141:EGS262150 EQO262141:EQO262150 FAK262141:FAK262150 FKG262141:FKG262150 FUC262141:FUC262150 GDY262141:GDY262150 GNU262141:GNU262150 GXQ262141:GXQ262150 HHM262141:HHM262150 HRI262141:HRI262150 IBE262141:IBE262150 ILA262141:ILA262150 IUW262141:IUW262150 JES262141:JES262150 JOO262141:JOO262150 JYK262141:JYK262150 KIG262141:KIG262150 KSC262141:KSC262150 LBY262141:LBY262150 LLU262141:LLU262150 LVQ262141:LVQ262150 MFM262141:MFM262150 MPI262141:MPI262150 MZE262141:MZE262150 NJA262141:NJA262150 NSW262141:NSW262150 OCS262141:OCS262150 OMO262141:OMO262150 OWK262141:OWK262150 PGG262141:PGG262150 PQC262141:PQC262150 PZY262141:PZY262150 QJU262141:QJU262150 QTQ262141:QTQ262150 RDM262141:RDM262150 RNI262141:RNI262150 RXE262141:RXE262150 SHA262141:SHA262150 SQW262141:SQW262150 TAS262141:TAS262150 TKO262141:TKO262150 TUK262141:TUK262150 UEG262141:UEG262150 UOC262141:UOC262150 UXY262141:UXY262150 VHU262141:VHU262150 VRQ262141:VRQ262150 WBM262141:WBM262150 WLI262141:WLI262150 WVE262141:WVE262150 IS327677:IS327686 SO327677:SO327686 ACK327677:ACK327686 AMG327677:AMG327686 AWC327677:AWC327686 BFY327677:BFY327686 BPU327677:BPU327686 BZQ327677:BZQ327686 CJM327677:CJM327686 CTI327677:CTI327686 DDE327677:DDE327686 DNA327677:DNA327686 DWW327677:DWW327686 EGS327677:EGS327686 EQO327677:EQO327686 FAK327677:FAK327686 FKG327677:FKG327686 FUC327677:FUC327686 GDY327677:GDY327686 GNU327677:GNU327686 GXQ327677:GXQ327686 HHM327677:HHM327686 HRI327677:HRI327686 IBE327677:IBE327686 ILA327677:ILA327686 IUW327677:IUW327686 JES327677:JES327686 JOO327677:JOO327686 JYK327677:JYK327686 KIG327677:KIG327686 KSC327677:KSC327686 LBY327677:LBY327686 LLU327677:LLU327686 LVQ327677:LVQ327686 MFM327677:MFM327686 MPI327677:MPI327686 MZE327677:MZE327686 NJA327677:NJA327686 NSW327677:NSW327686 OCS327677:OCS327686 OMO327677:OMO327686 OWK327677:OWK327686 PGG327677:PGG327686 PQC327677:PQC327686 PZY327677:PZY327686 QJU327677:QJU327686 QTQ327677:QTQ327686 RDM327677:RDM327686 RNI327677:RNI327686 RXE327677:RXE327686 SHA327677:SHA327686 SQW327677:SQW327686 TAS327677:TAS327686 TKO327677:TKO327686 TUK327677:TUK327686 UEG327677:UEG327686 UOC327677:UOC327686 UXY327677:UXY327686 VHU327677:VHU327686 VRQ327677:VRQ327686 WBM327677:WBM327686 WLI327677:WLI327686 WVE327677:WVE327686 IS393213:IS393222 SO393213:SO393222 ACK393213:ACK393222 AMG393213:AMG393222 AWC393213:AWC393222 BFY393213:BFY393222 BPU393213:BPU393222 BZQ393213:BZQ393222 CJM393213:CJM393222 CTI393213:CTI393222 DDE393213:DDE393222 DNA393213:DNA393222 DWW393213:DWW393222 EGS393213:EGS393222 EQO393213:EQO393222 FAK393213:FAK393222 FKG393213:FKG393222 FUC393213:FUC393222 GDY393213:GDY393222 GNU393213:GNU393222 GXQ393213:GXQ393222 HHM393213:HHM393222 HRI393213:HRI393222 IBE393213:IBE393222 ILA393213:ILA393222 IUW393213:IUW393222 JES393213:JES393222 JOO393213:JOO393222 JYK393213:JYK393222 KIG393213:KIG393222 KSC393213:KSC393222 LBY393213:LBY393222 LLU393213:LLU393222 LVQ393213:LVQ393222 MFM393213:MFM393222 MPI393213:MPI393222 MZE393213:MZE393222 NJA393213:NJA393222 NSW393213:NSW393222 OCS393213:OCS393222 OMO393213:OMO393222 OWK393213:OWK393222 PGG393213:PGG393222 PQC393213:PQC393222 PZY393213:PZY393222 QJU393213:QJU393222 QTQ393213:QTQ393222 RDM393213:RDM393222 RNI393213:RNI393222 RXE393213:RXE393222 SHA393213:SHA393222 SQW393213:SQW393222 TAS393213:TAS393222 TKO393213:TKO393222 TUK393213:TUK393222 UEG393213:UEG393222 UOC393213:UOC393222 UXY393213:UXY393222 VHU393213:VHU393222 VRQ393213:VRQ393222 WBM393213:WBM393222 WLI393213:WLI393222 WVE393213:WVE393222 IS458749:IS458758 SO458749:SO458758 ACK458749:ACK458758 AMG458749:AMG458758 AWC458749:AWC458758 BFY458749:BFY458758 BPU458749:BPU458758 BZQ458749:BZQ458758 CJM458749:CJM458758 CTI458749:CTI458758 DDE458749:DDE458758 DNA458749:DNA458758 DWW458749:DWW458758 EGS458749:EGS458758 EQO458749:EQO458758 FAK458749:FAK458758 FKG458749:FKG458758 FUC458749:FUC458758 GDY458749:GDY458758 GNU458749:GNU458758 GXQ458749:GXQ458758 HHM458749:HHM458758 HRI458749:HRI458758 IBE458749:IBE458758 ILA458749:ILA458758 IUW458749:IUW458758 JES458749:JES458758 JOO458749:JOO458758 JYK458749:JYK458758 KIG458749:KIG458758 KSC458749:KSC458758 LBY458749:LBY458758 LLU458749:LLU458758 LVQ458749:LVQ458758 MFM458749:MFM458758 MPI458749:MPI458758 MZE458749:MZE458758 NJA458749:NJA458758 NSW458749:NSW458758 OCS458749:OCS458758 OMO458749:OMO458758 OWK458749:OWK458758 PGG458749:PGG458758 PQC458749:PQC458758 PZY458749:PZY458758 QJU458749:QJU458758 QTQ458749:QTQ458758 RDM458749:RDM458758 RNI458749:RNI458758 RXE458749:RXE458758 SHA458749:SHA458758 SQW458749:SQW458758 TAS458749:TAS458758 TKO458749:TKO458758 TUK458749:TUK458758 UEG458749:UEG458758 UOC458749:UOC458758 UXY458749:UXY458758 VHU458749:VHU458758 VRQ458749:VRQ458758 WBM458749:WBM458758 WLI458749:WLI458758 WVE458749:WVE458758 IS524285:IS524294 SO524285:SO524294 ACK524285:ACK524294 AMG524285:AMG524294 AWC524285:AWC524294 BFY524285:BFY524294 BPU524285:BPU524294 BZQ524285:BZQ524294 CJM524285:CJM524294 CTI524285:CTI524294 DDE524285:DDE524294 DNA524285:DNA524294 DWW524285:DWW524294 EGS524285:EGS524294 EQO524285:EQO524294 FAK524285:FAK524294 FKG524285:FKG524294 FUC524285:FUC524294 GDY524285:GDY524294 GNU524285:GNU524294 GXQ524285:GXQ524294 HHM524285:HHM524294 HRI524285:HRI524294 IBE524285:IBE524294 ILA524285:ILA524294 IUW524285:IUW524294 JES524285:JES524294 JOO524285:JOO524294 JYK524285:JYK524294 KIG524285:KIG524294 KSC524285:KSC524294 LBY524285:LBY524294 LLU524285:LLU524294 LVQ524285:LVQ524294 MFM524285:MFM524294 MPI524285:MPI524294 MZE524285:MZE524294 NJA524285:NJA524294 NSW524285:NSW524294 OCS524285:OCS524294 OMO524285:OMO524294 OWK524285:OWK524294 PGG524285:PGG524294 PQC524285:PQC524294 PZY524285:PZY524294 QJU524285:QJU524294 QTQ524285:QTQ524294 RDM524285:RDM524294 RNI524285:RNI524294 RXE524285:RXE524294 SHA524285:SHA524294 SQW524285:SQW524294 TAS524285:TAS524294 TKO524285:TKO524294 TUK524285:TUK524294 UEG524285:UEG524294 UOC524285:UOC524294 UXY524285:UXY524294 VHU524285:VHU524294 VRQ524285:VRQ524294 WBM524285:WBM524294 WLI524285:WLI524294 WVE524285:WVE524294 IS589821:IS589830 SO589821:SO589830 ACK589821:ACK589830 AMG589821:AMG589830 AWC589821:AWC589830 BFY589821:BFY589830 BPU589821:BPU589830 BZQ589821:BZQ589830 CJM589821:CJM589830 CTI589821:CTI589830 DDE589821:DDE589830 DNA589821:DNA589830 DWW589821:DWW589830 EGS589821:EGS589830 EQO589821:EQO589830 FAK589821:FAK589830 FKG589821:FKG589830 FUC589821:FUC589830 GDY589821:GDY589830 GNU589821:GNU589830 GXQ589821:GXQ589830 HHM589821:HHM589830 HRI589821:HRI589830 IBE589821:IBE589830 ILA589821:ILA589830 IUW589821:IUW589830 JES589821:JES589830 JOO589821:JOO589830 JYK589821:JYK589830 KIG589821:KIG589830 KSC589821:KSC589830 LBY589821:LBY589830 LLU589821:LLU589830 LVQ589821:LVQ589830 MFM589821:MFM589830 MPI589821:MPI589830 MZE589821:MZE589830 NJA589821:NJA589830 NSW589821:NSW589830 OCS589821:OCS589830 OMO589821:OMO589830 OWK589821:OWK589830 PGG589821:PGG589830 PQC589821:PQC589830 PZY589821:PZY589830 QJU589821:QJU589830 QTQ589821:QTQ589830 RDM589821:RDM589830 RNI589821:RNI589830 RXE589821:RXE589830 SHA589821:SHA589830 SQW589821:SQW589830 TAS589821:TAS589830 TKO589821:TKO589830 TUK589821:TUK589830 UEG589821:UEG589830 UOC589821:UOC589830 UXY589821:UXY589830 VHU589821:VHU589830 VRQ589821:VRQ589830 WBM589821:WBM589830 WLI589821:WLI589830 WVE589821:WVE589830 IS655357:IS655366 SO655357:SO655366 ACK655357:ACK655366 AMG655357:AMG655366 AWC655357:AWC655366 BFY655357:BFY655366 BPU655357:BPU655366 BZQ655357:BZQ655366 CJM655357:CJM655366 CTI655357:CTI655366 DDE655357:DDE655366 DNA655357:DNA655366 DWW655357:DWW655366 EGS655357:EGS655366 EQO655357:EQO655366 FAK655357:FAK655366 FKG655357:FKG655366 FUC655357:FUC655366 GDY655357:GDY655366 GNU655357:GNU655366 GXQ655357:GXQ655366 HHM655357:HHM655366 HRI655357:HRI655366 IBE655357:IBE655366 ILA655357:ILA655366 IUW655357:IUW655366 JES655357:JES655366 JOO655357:JOO655366 JYK655357:JYK655366 KIG655357:KIG655366 KSC655357:KSC655366 LBY655357:LBY655366 LLU655357:LLU655366 LVQ655357:LVQ655366 MFM655357:MFM655366 MPI655357:MPI655366 MZE655357:MZE655366 NJA655357:NJA655366 NSW655357:NSW655366 OCS655357:OCS655366 OMO655357:OMO655366 OWK655357:OWK655366 PGG655357:PGG655366 PQC655357:PQC655366 PZY655357:PZY655366 QJU655357:QJU655366 QTQ655357:QTQ655366 RDM655357:RDM655366 RNI655357:RNI655366 RXE655357:RXE655366 SHA655357:SHA655366 SQW655357:SQW655366 TAS655357:TAS655366 TKO655357:TKO655366 TUK655357:TUK655366 UEG655357:UEG655366 UOC655357:UOC655366 UXY655357:UXY655366 VHU655357:VHU655366 VRQ655357:VRQ655366 WBM655357:WBM655366 WLI655357:WLI655366 WVE655357:WVE655366 IS720893:IS720902 SO720893:SO720902 ACK720893:ACK720902 AMG720893:AMG720902 AWC720893:AWC720902 BFY720893:BFY720902 BPU720893:BPU720902 BZQ720893:BZQ720902 CJM720893:CJM720902 CTI720893:CTI720902 DDE720893:DDE720902 DNA720893:DNA720902 DWW720893:DWW720902 EGS720893:EGS720902 EQO720893:EQO720902 FAK720893:FAK720902 FKG720893:FKG720902 FUC720893:FUC720902 GDY720893:GDY720902 GNU720893:GNU720902 GXQ720893:GXQ720902 HHM720893:HHM720902 HRI720893:HRI720902 IBE720893:IBE720902 ILA720893:ILA720902 IUW720893:IUW720902 JES720893:JES720902 JOO720893:JOO720902 JYK720893:JYK720902 KIG720893:KIG720902 KSC720893:KSC720902 LBY720893:LBY720902 LLU720893:LLU720902 LVQ720893:LVQ720902 MFM720893:MFM720902 MPI720893:MPI720902 MZE720893:MZE720902 NJA720893:NJA720902 NSW720893:NSW720902 OCS720893:OCS720902 OMO720893:OMO720902 OWK720893:OWK720902 PGG720893:PGG720902 PQC720893:PQC720902 PZY720893:PZY720902 QJU720893:QJU720902 QTQ720893:QTQ720902 RDM720893:RDM720902 RNI720893:RNI720902 RXE720893:RXE720902 SHA720893:SHA720902 SQW720893:SQW720902 TAS720893:TAS720902 TKO720893:TKO720902 TUK720893:TUK720902 UEG720893:UEG720902 UOC720893:UOC720902 UXY720893:UXY720902 VHU720893:VHU720902 VRQ720893:VRQ720902 WBM720893:WBM720902 WLI720893:WLI720902 WVE720893:WVE720902 IS786429:IS786438 SO786429:SO786438 ACK786429:ACK786438 AMG786429:AMG786438 AWC786429:AWC786438 BFY786429:BFY786438 BPU786429:BPU786438 BZQ786429:BZQ786438 CJM786429:CJM786438 CTI786429:CTI786438 DDE786429:DDE786438 DNA786429:DNA786438 DWW786429:DWW786438 EGS786429:EGS786438 EQO786429:EQO786438 FAK786429:FAK786438 FKG786429:FKG786438 FUC786429:FUC786438 GDY786429:GDY786438 GNU786429:GNU786438 GXQ786429:GXQ786438 HHM786429:HHM786438 HRI786429:HRI786438 IBE786429:IBE786438 ILA786429:ILA786438 IUW786429:IUW786438 JES786429:JES786438 JOO786429:JOO786438 JYK786429:JYK786438 KIG786429:KIG786438 KSC786429:KSC786438 LBY786429:LBY786438 LLU786429:LLU786438 LVQ786429:LVQ786438 MFM786429:MFM786438 MPI786429:MPI786438 MZE786429:MZE786438 NJA786429:NJA786438 NSW786429:NSW786438 OCS786429:OCS786438 OMO786429:OMO786438 OWK786429:OWK786438 PGG786429:PGG786438 PQC786429:PQC786438 PZY786429:PZY786438 QJU786429:QJU786438 QTQ786429:QTQ786438 RDM786429:RDM786438 RNI786429:RNI786438 RXE786429:RXE786438 SHA786429:SHA786438 SQW786429:SQW786438 TAS786429:TAS786438 TKO786429:TKO786438 TUK786429:TUK786438 UEG786429:UEG786438 UOC786429:UOC786438 UXY786429:UXY786438 VHU786429:VHU786438 VRQ786429:VRQ786438 WBM786429:WBM786438 WLI786429:WLI786438 WVE786429:WVE786438 IS851965:IS851974 SO851965:SO851974 ACK851965:ACK851974 AMG851965:AMG851974 AWC851965:AWC851974 BFY851965:BFY851974 BPU851965:BPU851974 BZQ851965:BZQ851974 CJM851965:CJM851974 CTI851965:CTI851974 DDE851965:DDE851974 DNA851965:DNA851974 DWW851965:DWW851974 EGS851965:EGS851974 EQO851965:EQO851974 FAK851965:FAK851974 FKG851965:FKG851974 FUC851965:FUC851974 GDY851965:GDY851974 GNU851965:GNU851974 GXQ851965:GXQ851974 HHM851965:HHM851974 HRI851965:HRI851974 IBE851965:IBE851974 ILA851965:ILA851974 IUW851965:IUW851974 JES851965:JES851974 JOO851965:JOO851974 JYK851965:JYK851974 KIG851965:KIG851974 KSC851965:KSC851974 LBY851965:LBY851974 LLU851965:LLU851974 LVQ851965:LVQ851974 MFM851965:MFM851974 MPI851965:MPI851974 MZE851965:MZE851974 NJA851965:NJA851974 NSW851965:NSW851974 OCS851965:OCS851974 OMO851965:OMO851974 OWK851965:OWK851974 PGG851965:PGG851974 PQC851965:PQC851974 PZY851965:PZY851974 QJU851965:QJU851974 QTQ851965:QTQ851974 RDM851965:RDM851974 RNI851965:RNI851974 RXE851965:RXE851974 SHA851965:SHA851974 SQW851965:SQW851974 TAS851965:TAS851974 TKO851965:TKO851974 TUK851965:TUK851974 UEG851965:UEG851974 UOC851965:UOC851974 UXY851965:UXY851974 VHU851965:VHU851974 VRQ851965:VRQ851974 WBM851965:WBM851974 WLI851965:WLI851974 WVE851965:WVE851974 IS917501:IS917510 SO917501:SO917510 ACK917501:ACK917510 AMG917501:AMG917510 AWC917501:AWC917510 BFY917501:BFY917510 BPU917501:BPU917510 BZQ917501:BZQ917510 CJM917501:CJM917510 CTI917501:CTI917510 DDE917501:DDE917510 DNA917501:DNA917510 DWW917501:DWW917510 EGS917501:EGS917510 EQO917501:EQO917510 FAK917501:FAK917510 FKG917501:FKG917510 FUC917501:FUC917510 GDY917501:GDY917510 GNU917501:GNU917510 GXQ917501:GXQ917510 HHM917501:HHM917510 HRI917501:HRI917510 IBE917501:IBE917510 ILA917501:ILA917510 IUW917501:IUW917510 JES917501:JES917510 JOO917501:JOO917510 JYK917501:JYK917510 KIG917501:KIG917510 KSC917501:KSC917510 LBY917501:LBY917510 LLU917501:LLU917510 LVQ917501:LVQ917510 MFM917501:MFM917510 MPI917501:MPI917510 MZE917501:MZE917510 NJA917501:NJA917510 NSW917501:NSW917510 OCS917501:OCS917510 OMO917501:OMO917510 OWK917501:OWK917510 PGG917501:PGG917510 PQC917501:PQC917510 PZY917501:PZY917510 QJU917501:QJU917510 QTQ917501:QTQ917510 RDM917501:RDM917510 RNI917501:RNI917510 RXE917501:RXE917510 SHA917501:SHA917510 SQW917501:SQW917510 TAS917501:TAS917510 TKO917501:TKO917510 TUK917501:TUK917510 UEG917501:UEG917510 UOC917501:UOC917510 UXY917501:UXY917510 VHU917501:VHU917510 VRQ917501:VRQ917510 WBM917501:WBM917510 WLI917501:WLI917510 WVE917501:WVE917510 IS983037:IS983046 SO983037:SO983046 ACK983037:ACK983046 AMG983037:AMG983046 AWC983037:AWC983046 BFY983037:BFY983046 BPU983037:BPU983046 BZQ983037:BZQ983046 CJM983037:CJM983046 CTI983037:CTI983046 DDE983037:DDE983046 DNA983037:DNA983046 DWW983037:DWW983046 EGS983037:EGS983046 EQO983037:EQO983046 FAK983037:FAK983046 FKG983037:FKG983046 FUC983037:FUC983046 GDY983037:GDY983046 GNU983037:GNU983046 GXQ983037:GXQ983046 HHM983037:HHM983046 HRI983037:HRI983046 IBE983037:IBE983046 ILA983037:ILA983046 IUW983037:IUW983046 JES983037:JES983046 JOO983037:JOO983046 JYK983037:JYK983046 KIG983037:KIG983046 KSC983037:KSC983046 LBY983037:LBY983046 LLU983037:LLU983046 LVQ983037:LVQ983046 MFM983037:MFM983046 MPI983037:MPI983046 MZE983037:MZE983046 NJA983037:NJA983046 NSW983037:NSW983046 OCS983037:OCS983046 OMO983037:OMO983046 OWK983037:OWK983046 PGG983037:PGG983046 PQC983037:PQC983046 PZY983037:PZY983046 QJU983037:QJU983046 QTQ983037:QTQ983046 RDM983037:RDM983046 RNI983037:RNI983046 RXE983037:RXE983046 SHA983037:SHA983046 SQW983037:SQW983046 TAS983037:TAS983046 TKO983037:TKO983046 TUK983037:TUK983046 UEG983037:UEG983046 UOC983037:UOC983046 UXY983037:UXY983046 VHU983037:VHU983046 VRQ983037:VRQ983046 WBM983037:WBM983046 WLI983037:WLI983046 WVE983037:WVE983046 SO5:SO8 ACK5:ACK8 AMG5:AMG8 AWC5:AWC8 BFY5:BFY8 BPU5:BPU8 BZQ5:BZQ8 CJM5:CJM8 CTI5:CTI8 DDE5:DDE8 DNA5:DNA8 DWW5:DWW8 EGS5:EGS8 EQO5:EQO8 FAK5:FAK8 FKG5:FKG8 FUC5:FUC8 GDY5:GDY8 GNU5:GNU8 GXQ5:GXQ8 HHM5:HHM8 HRI5:HRI8 IBE5:IBE8 ILA5:ILA8 IUW5:IUW8 JES5:JES8 JOO5:JOO8 JYK5:JYK8 KIG5:KIG8 KSC5:KSC8 LBY5:LBY8 LLU5:LLU8 LVQ5:LVQ8 MFM5:MFM8 MPI5:MPI8 MZE5:MZE8 NJA5:NJA8 NSW5:NSW8 OCS5:OCS8 OMO5:OMO8 OWK5:OWK8 PGG5:PGG8 PQC5:PQC8 PZY5:PZY8 QJU5:QJU8 QTQ5:QTQ8 RDM5:RDM8 RNI5:RNI8 RXE5:RXE8 SHA5:SHA8 SQW5:SQW8 TAS5:TAS8 TKO5:TKO8 TUK5:TUK8 UEG5:UEG8 UOC5:UOC8 UXY5:UXY8 VHU5:VHU8 VRQ5:VRQ8 WBM5:WBM8 WLI5:WLI8 WVE5:WVE8 IS5:IS8 SO15:SO18 ACK15:ACK18 AMG15:AMG18 AWC15:AWC18 BFY15:BFY18 BPU15:BPU18 BZQ15:BZQ18 CJM15:CJM18 CTI15:CTI18 DDE15:DDE18 DNA15:DNA18 DWW15:DWW18 EGS15:EGS18 EQO15:EQO18 FAK15:FAK18 FKG15:FKG18 FUC15:FUC18 GDY15:GDY18 GNU15:GNU18 GXQ15:GXQ18 HHM15:HHM18 HRI15:HRI18 IBE15:IBE18 ILA15:ILA18 IUW15:IUW18 JES15:JES18 JOO15:JOO18 JYK15:JYK18 KIG15:KIG18 KSC15:KSC18 LBY15:LBY18 LLU15:LLU18 LVQ15:LVQ18 MFM15:MFM18 MPI15:MPI18 MZE15:MZE18 NJA15:NJA18 NSW15:NSW18 OCS15:OCS18 OMO15:OMO18 OWK15:OWK18 PGG15:PGG18 PQC15:PQC18 PZY15:PZY18 QJU15:QJU18 QTQ15:QTQ18 RDM15:RDM18 RNI15:RNI18 RXE15:RXE18 SHA15:SHA18 SQW15:SQW18 TAS15:TAS18 TKO15:TKO18 TUK15:TUK18 UEG15:UEG18 UOC15:UOC18 UXY15:UXY18 VHU15:VHU18 VRQ15:VRQ18 WBM15:WBM18 WLI15:WLI18 WVE15:WVE18 IS15:IS18">

</xml_diff>

<commit_message>
coreccion ortrografica propuesta comercial
</commit_message>
<xml_diff>
--- a/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/2. Plantillas planeacion/Viaticos_q_Plan_Proyecto.xlsx
+++ b/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/2. Plantillas planeacion/Viaticos_q_Plan_Proyecto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="875" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Generales" sheetId="23" r:id="rId1"/>
@@ -202,8 +202,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Es el encargado de estructurar las diferentes partes hechas por los integrantes del grupo de desarrollo dentro de la etapa de implementacion, esto es importante para realizar  las primeras pruebas de integridad del software como unidad y no como objetos, librerias, componentes, etc.
-Es el encargdo de realizar el ejecutable del sistema y las líneas base de desarrollo.</t>
+          <t>Es el encargado de estructurar las diferentes partes hechas por los integrantes del grupo de desarrollo dentro de la etapa de implementación, esto es importante para realizar  las primeras pruebas de integridad del software como unidad y no como objetos, librerías, componentes, etc.
+Es el encargado de realizar el ejecutable del sistema y las líneas base de desarrollo.</t>
         </r>
       </text>
     </comment>
@@ -246,7 +246,7 @@
             <family val="2"/>
           </rPr>
           <t>El arquitecto de software tiene tres variables principales sobre cuales moverse: tiempo, satisfacción del cliente y, principalmente, costo de los desarrollos.
-Actividades del rquitecto: Concepción del proyecto, Requerimientos, Diseño del sistema, Construcción y pruebas del sistema y Liberación.</t>
+Actividades del arquitecto: Concepción del proyecto, Requerimientos, Diseño del sistema, Construcción y pruebas del sistema y Liberación.</t>
         </r>
       </text>
     </comment>
@@ -270,7 +270,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Personas con el conocimiento requerido par tomar decisiones en conjunto para analizar lo mejor para un proyecto bajo los criterios que se establecierón previamente</t>
+Personas con el conocimiento requerido par tomar decisiones en conjunto para analizar lo mejor para un proyecto bajo los criterios que se establecieron previamente</t>
         </r>
       </text>
     </comment>
@@ -293,7 +293,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Colocar aquí el nombre del elemento de comunicación. Ej:
+          <t>Colocar aquí el nombre del elemento de comunicación. Ej.:
 "Kick Off,  Plan de Proyecto, Reuniones de Equipo"</t>
         </r>
       </text>
@@ -454,7 +454,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Colocar aquí el nombre del elemento de comunicación. Ej:
+          <t>Colocar aquí el nombre del elemento de comunicación. Ej.:
 "Kick Off,  Plan de Proyecto, Reuniones de Equipo"</t>
         </r>
       </text>
@@ -514,7 +514,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Colocar aquí el nombre del elemento de comunicación. Ej:
+          <t>Colocar aquí el nombre del elemento de comunicación. Ej.:
 "Kick Off,  Plan de Proyecto, Reuniones de Equipo"</t>
         </r>
       </text>
@@ -528,7 +528,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Colocar aquí el nombre del elemento de comunicación. Ej:
+          <t>Colocar aquí el nombre del elemento de comunicación. Ej.:
 "Kick Off,  Plan de Proyecto, Reuniones de Equipo"</t>
         </r>
       </text>
@@ -538,7 +538,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="308">
   <si>
     <t>Nombre</t>
   </si>
@@ -637,9 +637,6 @@
   </si>
   <si>
     <t>Capacitaciones Necesarias para el Equipo de Proyecto</t>
-  </si>
-  <si>
-    <t>Plan de Comunicacción</t>
   </si>
   <si>
     <t>b</t>
@@ -691,9 +688,6 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>Muy alto:Perdida del proyecto</t>
-  </si>
-  <si>
     <t>Alto: Se paro el proyecto</t>
   </si>
   <si>
@@ -719,9 +713,6 @@
     <t>Estrategia de Comunicación</t>
   </si>
   <si>
-    <t>Plan de contigencia</t>
-  </si>
-  <si>
     <t>Plan de mitigación</t>
   </si>
   <si>
@@ -761,9 +752,6 @@
     <t>Tester</t>
   </si>
   <si>
-    <t>Estimacion del Proyecto</t>
-  </si>
-  <si>
     <t>Calendario del Proyecto</t>
   </si>
   <si>
@@ -896,12 +884,6 @@
     <t>Integrador</t>
   </si>
   <si>
-    <t>Arquitecto ó Líder técnico</t>
-  </si>
-  <si>
-    <t>Pruebas de recuperacoòn</t>
-  </si>
-  <si>
     <t>Pruebas de rendimiento(Volumen y Performance)</t>
   </si>
   <si>
@@ -941,9 +923,6 @@
     <t>Implementador</t>
   </si>
   <si>
-    <t>Comité de desiciones</t>
-  </si>
-  <si>
     <t>Solo equipo</t>
   </si>
   <si>
@@ -953,21 +932,12 @@
     <t>Equipo y dirección</t>
   </si>
   <si>
-    <t>Equipo,Dirección y Cliente</t>
-  </si>
-  <si>
-    <t>En  caso de que el riesgo sea demasiado alto se debe agendar una reunicón con dirección, equipo de trabajo y cliente para buscar una solución para mitigar el riego</t>
-  </si>
-  <si>
     <t>Si el riesgo no tiene una severidad alta pero esta latente, se realiza la junta con dirección y equipo de trabajo</t>
   </si>
   <si>
     <t>Si la severidad del riesgo es muy baja solo se requiere una junta con el equipo de trabajo</t>
   </si>
   <si>
-    <t>Categoria</t>
-  </si>
-  <si>
     <t>General</t>
   </si>
   <si>
@@ -980,36 +950,21 @@
     <t xml:space="preserve">Proyecto Interno </t>
   </si>
   <si>
-    <t>Proyecto ecterno</t>
-  </si>
-  <si>
     <t>Proyecto de  12 o menos semanas</t>
   </si>
   <si>
     <t>Proyecto de 13 o más semanas</t>
   </si>
   <si>
-    <t xml:space="preserve">Validacion de requerimientos </t>
-  </si>
-  <si>
     <t>Requerimientos</t>
   </si>
   <si>
     <t>Verificación de casos de uso</t>
   </si>
   <si>
-    <t>Ejecucion</t>
-  </si>
-  <si>
     <t>Entrega</t>
   </si>
   <si>
-    <t>Realizar la verificacion de analisis y diseño</t>
-  </si>
-  <si>
-    <t>Realizar validacn del producto</t>
-  </si>
-  <si>
     <t>Capacitación</t>
   </si>
   <si>
@@ -1064,36 +1019,21 @@
     <t>Documento "Plan de proyecto"</t>
   </si>
   <si>
-    <t>Documento "Anallisis y dise~o"</t>
-  </si>
-  <si>
-    <t>Carpeta con el codigo del proyecto</t>
-  </si>
-  <si>
     <t>Documento "Reporte de pruebas"</t>
   </si>
   <si>
     <t>Documento "Manual de usuario"</t>
   </si>
   <si>
-    <t>Documento "Manual tecnico"</t>
-  </si>
-  <si>
     <t>Documento "Reporte de defectos encontrados"</t>
   </si>
   <si>
     <t>Documento "Cierre del proyecto"</t>
   </si>
   <si>
-    <t>Estimacion y planeacion</t>
-  </si>
-  <si>
     <t>Cierre de proyecto</t>
   </si>
   <si>
-    <t xml:space="preserve">Viaticos_q/2. Estimacion y planeacion/ 1. Plantillas estimacion/Estimacion Esfuerzo </t>
-  </si>
-  <si>
     <t>Roles Equipo de Qualtop</t>
   </si>
   <si>
@@ -1106,11 +1046,6 @@
     <t>****</t>
   </si>
   <si>
-    <t>Validacion de requerimientos
-Aprobacion de la propuesta comercial
-Validacion del producto</t>
-  </si>
-  <si>
     <t>rpulido@qualtop.com</t>
   </si>
   <si>
@@ -1156,39 +1091,15 @@
     <t>felipelozanopadilla@gmail.com</t>
   </si>
   <si>
-    <t>Vease en matriz de roles</t>
-  </si>
-  <si>
     <t>Kick off</t>
   </si>
   <si>
     <t>Reuniones de equipo</t>
   </si>
   <si>
-    <t>Lider de proyecto</t>
-  </si>
-  <si>
     <t>Informar el status del proyecto</t>
   </si>
   <si>
-    <t>Cada 15 dias</t>
-  </si>
-  <si>
-    <t>Cada 7 dias</t>
-  </si>
-  <si>
-    <t>Informar el plan de ejecucion del proyecto y avance</t>
-  </si>
-  <si>
-    <t>Tiempo de ejecucion del proyecto</t>
-  </si>
-  <si>
-    <t>No se cumpla la planificacion</t>
-  </si>
-  <si>
-    <t>Falta de ejecucion de un area especifica</t>
-  </si>
-  <si>
     <t>Financiamiento</t>
   </si>
   <si>
@@ -1216,18 +1127,9 @@
     <t>Desarrollo del proyecto (Complejidad alta y fiabilidad)</t>
   </si>
   <si>
-    <t>Falla tecnologica (Falla de un instrumento que contenga informacion unica)</t>
-  </si>
-  <si>
     <t>Cliente no satisfecho con la idea</t>
   </si>
   <si>
-    <t>Problemas administrativos y tecnicos</t>
-  </si>
-  <si>
-    <t>Comunicacion (cada integrante activo en el proyecto trabaje por su lado, sin estar informado de los ya ejecutado)</t>
-  </si>
-  <si>
     <t>Se duplique trabajo ya realizado o se ejecute un proceso de manera incorrecta</t>
   </si>
   <si>
@@ -1252,12 +1154,6 @@
     <t>Critico</t>
   </si>
   <si>
-    <t>Factores que afecten la ejecucion del proyecto</t>
-  </si>
-  <si>
-    <t>Llevar control de auditoria cada 3er dia</t>
-  </si>
-  <si>
     <t>Aumentar el numero de actividades por meta no cumplida en fecha establecida</t>
   </si>
   <si>
@@ -1270,111 +1166,51 @@
     <t>Falta de personal capaz de participar activamente en el proyecto</t>
   </si>
   <si>
-    <t>Administrar de manera uniforme los recursos paras las areas requeridas en el desarrollo del proyecto</t>
-  </si>
-  <si>
     <t>Contratar personal capaz de realizar lo requerido en el proyecto</t>
   </si>
   <si>
-    <t>Contratar personal capaz de llevar a cabo el puesto requerido en el proyecto y/o realizar capacitacion</t>
-  </si>
-  <si>
     <t>Auditoria de esfuerzos</t>
   </si>
   <si>
     <t>Monitorear trabajo diario</t>
   </si>
   <si>
-    <t>Falla en estimacion y mal administracion de los recursos</t>
-  </si>
-  <si>
-    <t>Llevar auditoria de gastos dia a dia que requiere el desarrollo del proyecto</t>
-  </si>
-  <si>
-    <t>Encontrar estrategias para disminuir los gastos en el desarrollo del proyecto, de no ser asi, cotizar una nueva estimacion del desarrollo del proyecto</t>
-  </si>
-  <si>
-    <t>Informe de costos semanal a direccion</t>
-  </si>
-  <si>
     <t xml:space="preserve">Llevar el control de los gastos generados </t>
   </si>
   <si>
     <t>Revisión a distancia</t>
   </si>
   <si>
-    <t>Falta de mobilirario e infraestructura adecuada para el desarrollo del proyecto</t>
-  </si>
-  <si>
-    <t>Tener un lugar definido para el desarrollo del proyecto, asi como el mobiliario adecuado</t>
-  </si>
-  <si>
     <t>Adquirir mobiliario adecuado. Adquirir un lugar adecuado para el desarrollo del proyecto</t>
   </si>
   <si>
-    <t>Informar a direccion los recursos necesarios para el desarrollo del proyecto</t>
-  </si>
-  <si>
     <t>Checklist de mobiliario e infraestructura necesarios</t>
   </si>
   <si>
-    <t>Termino de vida util de una herramienta tecnologica</t>
-  </si>
-  <si>
-    <t>Tener respaldos de informacion en diferentes herramientas tecnologicas (CPU)</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>Informe a direccion de falla cuando suceda</t>
-  </si>
-  <si>
     <t>Falta de capacidad en personal</t>
   </si>
   <si>
     <t>Evaluar la capacidad del personal involucrado en el proyecto</t>
   </si>
   <si>
-    <t>Informar cualidades del personal que labora en el proyecto a direccion</t>
-  </si>
-  <si>
-    <t>Falla en la ejecucion del proyecto</t>
-  </si>
-  <si>
     <t>Asegurar por contrato el desarrollo del proyecto con el cliente e involucrar riesgos</t>
   </si>
   <si>
-    <t>Busqueda de nuevo cliente</t>
-  </si>
-  <si>
     <t>Informe semanal del avance del proyecto</t>
   </si>
   <si>
-    <t>Falta de comunicacion entre personal</t>
-  </si>
-  <si>
-    <t>Estar en constante comunicacion por el medio que se adecue a cada uno</t>
-  </si>
-  <si>
     <t>Corregir errores cometidos a tiempo, informando el error inmediatamente al auditar el proyecto</t>
   </si>
   <si>
     <t>Junta de equipo semanal, informe por medio emal</t>
   </si>
   <si>
-    <t>Asegurar la comunicacion entre participantes del proyecto</t>
-  </si>
-  <si>
     <t>Entrega de proyecto</t>
   </si>
   <si>
-    <t>Líder de proyecto, Respresentante de proyecto</t>
-  </si>
-  <si>
-    <t>Líder de proyecto, analista, arquitecto, Desarrollador, tester, aseguramiento de la calidad, lider de procesos, director general, director operativo, administrador de la configuración</t>
-  </si>
-  <si>
     <t>Director operativo, Líder de proyecto, aseguramiento de la calidad, Líder de procesos</t>
   </si>
   <si>
@@ -1390,66 +1226,33 @@
     <t>Documento "Propuesta comercial"</t>
   </si>
   <si>
-    <t>Codigo</t>
-  </si>
-  <si>
     <t>Seguimiento plan de proyecto</t>
   </si>
   <si>
     <t>Informes (auditorias y control)</t>
   </si>
   <si>
-    <t>Ejecucion del plan de pruebas</t>
-  </si>
-  <si>
-    <t>Evaluacion honesta de los productos</t>
-  </si>
-  <si>
     <t>Disponibilidad de personal</t>
   </si>
   <si>
-    <t>Cada empleado de la organizacion puede estar asignado a varios puestos dentro del proyecto y participar en maximo dos proyectos</t>
-  </si>
-  <si>
     <t>Capacidades del personal</t>
   </si>
   <si>
-    <t>Antes de asignar persona a los proyectos, se tiene que analizar el perfil de los empleados verificando asi el perfil adecuado para desarrollar el proyecto</t>
-  </si>
-  <si>
     <t>Agenda por empleado</t>
   </si>
   <si>
-    <t>Cada empleado debe tener asignada una agenda con los horarios que tiene para proyecto en el que se encuentra o area de proceso</t>
-  </si>
-  <si>
     <t>Trabajo de oficina desde casa</t>
   </si>
   <si>
     <t>Llegar tarde a la oficina (puntualidad)</t>
   </si>
   <si>
-    <t>No se podra llegar despues de las 9:15 a.m en caso de que existan juntas con el cliente, juntas de la organizacion o capacitaciones previamente agendadas.</t>
-  </si>
-  <si>
-    <t>Musica sin audifonos</t>
-  </si>
-  <si>
-    <t>No esta permitido escuchar musica a un volumen inapropiado si se encuentra dentro de la jornada laboral</t>
-  </si>
-  <si>
     <t>Actividades recreativas</t>
   </si>
   <si>
-    <t>No se debe de exceder un rango de 10 minutos en actividades recreativas dentro de la oficina durante la jornada laboral o cuando se este utilizando el telefono de la empresa</t>
-  </si>
-  <si>
     <t>Hora de comida</t>
   </si>
   <si>
-    <t>El tiempo maximo para la hora de comida es de 1:30 horas. Esta puede tomarse a la hora que el empleado prefiera</t>
-  </si>
-  <si>
     <t>Proyectos ajenos a la empresa</t>
   </si>
   <si>
@@ -1459,15 +1262,9 @@
     <t>Vacaciones</t>
   </si>
   <si>
-    <t>Las vacaciones deben solicitarse con una semana de anticipacion y solo se dara permiso por 3 dias</t>
-  </si>
-  <si>
     <t>Salir antes de que termine la jornada laboral</t>
   </si>
   <si>
-    <t>Esto puede realizarse solo cuando el proyecto donde este involucrado el personal no se encuentre en fase critica (No se tienen agendas, reuniones de la organizacion, reuniones con el cliente, capacitacion o se requiere de su presencia para actividades de otros en el proyecto)</t>
-  </si>
-  <si>
     <t>Registro de actividades laborales</t>
   </si>
   <si>
@@ -1475,6 +1272,200 @@
   </si>
   <si>
     <t>http://www.iwm.mx/cmmi/index.php?m=projects&amp;a=view&amp;project_id=19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viaticos_q/2. Estimación y planeación/ 1. Plantillas estimación/Estimación Esfuerzo </t>
+  </si>
+  <si>
+    <t>Estimación y planeación</t>
+  </si>
+  <si>
+    <t>Ejecución</t>
+  </si>
+  <si>
+    <t>Documento "Análisis y diseño"</t>
+  </si>
+  <si>
+    <t>Carpeta con el código del proyecto</t>
+  </si>
+  <si>
+    <t>Documento "Manual técnico"</t>
+  </si>
+  <si>
+    <t>Estimación del Proyecto</t>
+  </si>
+  <si>
+    <t>Véase en matriz de roles</t>
+  </si>
+  <si>
+    <t>Arquitecto o Líder técnico</t>
+  </si>
+  <si>
+    <t>Comité de decisiones</t>
+  </si>
+  <si>
+    <t>Validación de requerimientos
+Aprobación de la propuesta comercial
+Validación del producto</t>
+  </si>
+  <si>
+    <t>Líder de proyecto</t>
+  </si>
+  <si>
+    <t>Líder de proyecto, analista, arquitecto, Desarrollador, tester, aseguramiento de la calidad, líder de procesos, director general, director operativo, administrador de la configuración</t>
+  </si>
+  <si>
+    <t>Informar el plan de ejecución del proyecto y avance</t>
+  </si>
+  <si>
+    <t>Cada 15 días</t>
+  </si>
+  <si>
+    <t>Cada 7 días</t>
+  </si>
+  <si>
+    <t>Líder de proyecto, Representante de proyecto</t>
+  </si>
+  <si>
+    <t>Muy alto: Perdida del proyecto</t>
+  </si>
+  <si>
+    <t>Proyecto externo</t>
+  </si>
+  <si>
+    <t>En  caso de que el riesgo sea demasiado alto se debe agendar una reunión con dirección, equipo de trabajo y cliente para buscar una solución para mitigar el riego</t>
+  </si>
+  <si>
+    <t>Plan de contingencia</t>
+  </si>
+  <si>
+    <t>Tiempo de ejecución del proyecto</t>
+  </si>
+  <si>
+    <t>No se cumpla la planificación</t>
+  </si>
+  <si>
+    <t>Factores que afecten la ejecución del proyecto</t>
+  </si>
+  <si>
+    <t>Llevar control de auditoria cada 3er día</t>
+  </si>
+  <si>
+    <t>Falta de ejecución de un área especifica</t>
+  </si>
+  <si>
+    <t>Administrar de manera uniforme los recursos paras las áreas requeridas en el desarrollo del proyecto</t>
+  </si>
+  <si>
+    <t>Contratar personal capaz de llevar a cabo el puesto requerido en el proyecto y/o realizar capacitación</t>
+  </si>
+  <si>
+    <t>Falla en estimación y mal administración de los recursos</t>
+  </si>
+  <si>
+    <t>Llevar auditoria de gastos día a día que requiere el desarrollo del proyecto</t>
+  </si>
+  <si>
+    <t>Encontrar estrategias para disminuir los gastos en el desarrollo del proyecto, de no ser así, cotizar una nueva estimación del desarrollo del proyecto</t>
+  </si>
+  <si>
+    <t>Informe de costos semanal a dirección</t>
+  </si>
+  <si>
+    <t>Falta de mobiliario e infraestructura adecuada para el desarrollo del proyecto</t>
+  </si>
+  <si>
+    <t>Tener un lugar definido para el desarrollo del proyecto, así como el mobiliario adecuado</t>
+  </si>
+  <si>
+    <t>Informar a dirección los recursos necesarios para el desarrollo del proyecto</t>
+  </si>
+  <si>
+    <t>Falla tecnológica (Falla de un instrumento que contenga información única)</t>
+  </si>
+  <si>
+    <t>Termino de vida útil de una herramienta tecnológica</t>
+  </si>
+  <si>
+    <t>Tener respaldos de información en diferentes herramientas tecnológicas (CPU)</t>
+  </si>
+  <si>
+    <t>Informe a dirección de falla cuando suceda</t>
+  </si>
+  <si>
+    <t>Informar cualidades del personal que labora en el proyecto a dirección</t>
+  </si>
+  <si>
+    <t>Problemas administrativos y técnicos</t>
+  </si>
+  <si>
+    <t>Falla en la ejecución del proyecto</t>
+  </si>
+  <si>
+    <t>Búsqueda de nuevo cliente</t>
+  </si>
+  <si>
+    <t>Comunicación (cada integrante activo en el proyecto trabaje por su lado, sin estar informado de los ya ejecutado)</t>
+  </si>
+  <si>
+    <t>Falta de comunicación entre personal</t>
+  </si>
+  <si>
+    <t>Estar en constante comunicación por el medio que se adecue a cada uno</t>
+  </si>
+  <si>
+    <t>Asegurar la comunicación entre participantes del proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validación de requerimientos </t>
+  </si>
+  <si>
+    <t>Realizar la verificación de análisis y diseño</t>
+  </si>
+  <si>
+    <t>Realizar validación del producto</t>
+  </si>
+  <si>
+    <t>Cada empleado de la organización puede estar asignado a varios puestos dentro del proyecto y participar en máximo dos proyectos</t>
+  </si>
+  <si>
+    <t>Antes de asignar persona a los proyectos, se tiene que analizar el perfil de los empleados verificando así el perfil adecuado para desarrollar el proyecto</t>
+  </si>
+  <si>
+    <t>Cada empleado debe tener asignada una agenda con los horarios que tiene para proyecto en el que se encuentra o área de proceso</t>
+  </si>
+  <si>
+    <t>Esto puede realizarse solo cuando el proyecto donde este involucrado el personal no se encuentre en fase critica (No se tienen agendas, reuniones de la organización, reuniones con el cliente, capacitación o se requiere de su presencia para actividades de otros en el proyecto)</t>
+  </si>
+  <si>
+    <t>No se podrá llegar después de las 9:15 a.m. en caso de que existan juntas con el cliente, juntas de la organización o capacitaciones previamente agendadas.</t>
+  </si>
+  <si>
+    <t>Música sin audífonos</t>
+  </si>
+  <si>
+    <t>No esta permitido escuchar música a un volumen inapropiado si se encuentra dentro de la jornada laboral</t>
+  </si>
+  <si>
+    <t>No se debe de exceder un rango de 10 minutos en actividades recreativas dentro de la oficina durante la jornada laboral o cuando se este utilizando el teléfono de la empresa</t>
+  </si>
+  <si>
+    <t>El tiempo máximo para la hora de comida es de 1:30 horas. Esta puede tomarse a la hora que el empleado prefiera</t>
+  </si>
+  <si>
+    <t>Las vacaciones deben solicitarse con una semana de anticipación y solo se dará permiso por 3 días</t>
+  </si>
+  <si>
+    <t>Pruebas de recuperación</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Evaluación honesta de los productos</t>
+  </si>
+  <si>
+    <t>Ejecución del plan de pruebas</t>
   </si>
 </sst>
 </file>
@@ -2923,12 +2914,12 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="54" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="52" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="54" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="52" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2938,19 +2929,19 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="52" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="25" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="25" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3816,8 +3807,8 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -4107,7 +4098,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="D4" s="80"/>
       <c r="E4" s="80"/>
@@ -4127,7 +4118,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D6" s="76"/>
       <c r="E6" s="76"/>
@@ -4157,13 +4148,13 @@
         <v>22</v>
       </c>
       <c r="C9" s="98" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F9" s="115" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4179,7 +4170,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -4203,76 +4194,76 @@
     </row>
     <row r="15" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B15" s="181" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B16" s="182"/>
       <c r="C16" s="67" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B17" s="183" t="s">
-        <v>181</v>
+        <v>245</v>
       </c>
       <c r="C17" s="62" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B18" s="182"/>
       <c r="C18" s="62" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B19" s="183" t="s">
-        <v>152</v>
+        <v>246</v>
       </c>
       <c r="C19" s="62" t="s">
-        <v>174</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B20" s="181"/>
       <c r="C20" s="62" t="s">
-        <v>175</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B21" s="181"/>
       <c r="C21" s="62" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B22" s="181"/>
       <c r="C22" s="62" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B23" s="182"/>
       <c r="C23" s="62" t="s">
-        <v>178</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B24" s="183" t="s">
-        <v>182</v>
+        <v>163</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B25" s="182"/>
       <c r="C25" s="62" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4282,28 +4273,28 @@
     <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="147"/>
       <c r="B27" s="144" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C27" s="147"/>
     </row>
     <row r="28" spans="1:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="180" t="s">
-        <v>310</v>
-      </c>
-      <c r="C28" s="179"/>
+      <c r="B28" s="179" t="s">
+        <v>243</v>
+      </c>
+      <c r="C28" s="180"/>
     </row>
     <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="147"/>
       <c r="B29" s="144" t="s">
-        <v>73</v>
+        <v>250</v>
       </c>
       <c r="C29" s="147"/>
     </row>
     <row r="30" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="180" t="s">
-        <v>183</v>
-      </c>
-      <c r="C30" s="180"/>
+      <c r="B30" s="179" t="s">
+        <v>244</v>
+      </c>
+      <c r="C30" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4339,8 +4330,8 @@
   </sheetPr>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D28" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -4799,7 +4790,7 @@
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -4810,7 +4801,7 @@
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="155"/>
       <c r="B3" s="156" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="C3" s="155"/>
       <c r="D3" s="155"/>
@@ -4833,7 +4824,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G4" s="25" t="s">
         <v>29</v>
@@ -4842,22 +4833,22 @@
     <row r="5" spans="1:7" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
       <c r="B5" s="16" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="E5" s="162" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>188</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4885,20 +4876,20 @@
       <c r="B8" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="185" t="s">
+      <c r="C8" s="187" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="185"/>
-      <c r="E8" s="186" t="s">
+      <c r="D8" s="187"/>
+      <c r="E8" s="188" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="186"/>
+      <c r="F8" s="188"/>
       <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A9" s="151"/>
       <c r="B9" s="152" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C9" s="152"/>
       <c r="D9" s="152"/>
@@ -4909,26 +4900,26 @@
     <row r="10" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="C10" s="184" t="str">
+        <v>180</v>
+      </c>
+      <c r="C10" s="185" t="str">
         <f>VLOOKUP(B10,$B$50:$D$66,2,0)</f>
         <v>33 1605 3573</v>
       </c>
-      <c r="D10" s="184"/>
-      <c r="E10" s="184" t="str">
+      <c r="D10" s="185"/>
+      <c r="E10" s="185" t="str">
         <f>VLOOKUP(B10,$B$50:$D$66,3,0)</f>
         <v>felipelozanopadilla@gmail.com</v>
       </c>
-      <c r="F10" s="184"/>
+      <c r="F10" s="185"/>
       <c r="G10" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="153"/>
       <c r="B11" s="154" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C11" s="154"/>
       <c r="D11" s="154"/>
@@ -4939,26 +4930,26 @@
     <row r="12" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="C12" s="184" t="str">
+        <v>170</v>
+      </c>
+      <c r="C12" s="185" t="str">
         <f>VLOOKUP(B12,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D12" s="184"/>
-      <c r="E12" s="184" t="str">
+      <c r="D12" s="185"/>
+      <c r="E12" s="185" t="str">
         <f>VLOOKUP(B12,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F12" s="184"/>
+      <c r="F12" s="185"/>
       <c r="G12" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="153"/>
       <c r="B13" s="154" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C13" s="154"/>
       <c r="D13" s="154"/>
@@ -4969,43 +4960,43 @@
     <row r="14" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="C14" s="184" t="str">
+        <v>165</v>
+      </c>
+      <c r="C14" s="185" t="str">
         <f>VLOOKUP(B14,$B$50:$D$66,2,0)</f>
         <v>33 1862 1719</v>
       </c>
-      <c r="D14" s="184"/>
-      <c r="E14" s="184" t="str">
+      <c r="D14" s="185"/>
+      <c r="E14" s="185" t="str">
         <f>VLOOKUP(B14,$B$50:$D$66,3,0)</f>
         <v>rpulido@qualtop.com</v>
       </c>
-      <c r="F14" s="184"/>
+      <c r="F14" s="185"/>
       <c r="G14" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="184" t="e">
+        <v>76</v>
+      </c>
+      <c r="C15" s="185" t="e">
         <f>VLOOKUP(B15,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D15" s="184"/>
-      <c r="E15" s="184" t="e">
+      <c r="D15" s="185"/>
+      <c r="E15" s="185" t="e">
         <f>VLOOKUP(B15,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F15" s="184"/>
+      <c r="F15" s="185"/>
       <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="153"/>
       <c r="B16" s="154" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C16" s="154"/>
       <c r="D16" s="154"/>
@@ -5016,60 +5007,60 @@
     <row r="17" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C17" s="184" t="str">
+        <v>172</v>
+      </c>
+      <c r="C17" s="185" t="str">
         <f>VLOOKUP(B17,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D17" s="184"/>
-      <c r="E17" s="184" t="str">
+      <c r="D17" s="185"/>
+      <c r="E17" s="185" t="str">
         <f>VLOOKUP(B17,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F17" s="184"/>
+      <c r="F17" s="185"/>
       <c r="G17" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="184" t="e">
+        <v>76</v>
+      </c>
+      <c r="C18" s="185" t="e">
         <f>VLOOKUP(B18,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D18" s="184"/>
-      <c r="E18" s="184" t="e">
+      <c r="D18" s="185"/>
+      <c r="E18" s="185" t="e">
         <f>VLOOKUP(B18,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F18" s="184"/>
+      <c r="F18" s="185"/>
       <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="184" t="e">
+        <v>76</v>
+      </c>
+      <c r="C19" s="185" t="e">
         <f>VLOOKUP(B19,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D19" s="184"/>
-      <c r="E19" s="184" t="e">
+      <c r="D19" s="185"/>
+      <c r="E19" s="185" t="e">
         <f>VLOOKUP(B19,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F19" s="184"/>
+      <c r="F19" s="185"/>
       <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="153"/>
       <c r="B20" s="154" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C20" s="154"/>
       <c r="D20" s="154"/>
@@ -5080,37 +5071,37 @@
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="C21" s="184" t="str">
+        <v>170</v>
+      </c>
+      <c r="C21" s="185" t="str">
         <f>VLOOKUP(B21,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D21" s="184"/>
-      <c r="E21" s="184" t="str">
+      <c r="D21" s="185"/>
+      <c r="E21" s="185" t="str">
         <f>VLOOKUP(B21,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F21" s="184"/>
+      <c r="F21" s="185"/>
       <c r="G21" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C22" s="184" t="e">
+        <v>76</v>
+      </c>
+      <c r="C22" s="185" t="e">
         <f>VLOOKUP(B22,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D22" s="184"/>
-      <c r="E22" s="184" t="e">
+      <c r="D22" s="185"/>
+      <c r="E22" s="185" t="e">
         <f>VLOOKUP(B22,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F22" s="184"/>
+      <c r="F22" s="185"/>
       <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -5127,20 +5118,20 @@
     <row r="24" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C24" s="184" t="str">
+        <v>172</v>
+      </c>
+      <c r="C24" s="185" t="str">
         <f>VLOOKUP(B24,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D24" s="184"/>
-      <c r="E24" s="184" t="str">
+      <c r="D24" s="185"/>
+      <c r="E24" s="185" t="str">
         <f>VLOOKUP(B24,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F24" s="184"/>
+      <c r="F24" s="185"/>
       <c r="G24" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -5157,26 +5148,26 @@
     <row r="26" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C26" s="184" t="str">
+        <v>172</v>
+      </c>
+      <c r="C26" s="185" t="str">
         <f>VLOOKUP(B26,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D26" s="184"/>
-      <c r="E26" s="184" t="str">
+      <c r="D26" s="185"/>
+      <c r="E26" s="185" t="str">
         <f>VLOOKUP(B26,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F26" s="184"/>
+      <c r="F26" s="185"/>
       <c r="G26" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="153"/>
       <c r="B27" s="154" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C27" s="154"/>
       <c r="D27" s="154"/>
@@ -5187,26 +5178,26 @@
     <row r="28" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="C28" s="184" t="str">
+        <v>173</v>
+      </c>
+      <c r="C28" s="185" t="str">
         <f>VLOOKUP(B28,$B$50:$D$66,2,0)</f>
         <v>33 3807 6830</v>
       </c>
-      <c r="D28" s="184"/>
-      <c r="E28" s="184" t="str">
+      <c r="D28" s="185"/>
+      <c r="E28" s="185" t="str">
         <f>VLOOKUP(B28,$B$50:$D$66,3,0)</f>
         <v>asosa@qualtop.com</v>
       </c>
-      <c r="F28" s="184"/>
+      <c r="F28" s="185"/>
       <c r="G28" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="153"/>
       <c r="B29" s="154" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C29" s="154"/>
       <c r="D29" s="154"/>
@@ -5217,26 +5208,26 @@
     <row r="30" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="C30" s="184" t="str">
+        <v>173</v>
+      </c>
+      <c r="C30" s="185" t="str">
         <f>VLOOKUP(B30,$B$50:$D$66,2,0)</f>
         <v>33 3807 6830</v>
       </c>
-      <c r="D30" s="184"/>
-      <c r="E30" s="184" t="str">
+      <c r="D30" s="185"/>
+      <c r="E30" s="185" t="str">
         <f>VLOOKUP(B30,$B$50:$D$66,3,0)</f>
         <v>asosa@qualtop.com</v>
       </c>
-      <c r="F30" s="184"/>
+      <c r="F30" s="185"/>
       <c r="G30" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="153"/>
       <c r="B31" s="154" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C31" s="154"/>
       <c r="D31" s="154"/>
@@ -5247,26 +5238,26 @@
     <row r="32" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="C32" s="184" t="str">
+        <v>170</v>
+      </c>
+      <c r="C32" s="185" t="str">
         <f>VLOOKUP(B32,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D32" s="184"/>
-      <c r="E32" s="184" t="str">
+      <c r="D32" s="185"/>
+      <c r="E32" s="185" t="str">
         <f>VLOOKUP(B32,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F32" s="184"/>
+      <c r="F32" s="185"/>
       <c r="G32" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="153"/>
       <c r="B33" s="154" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C33" s="154"/>
       <c r="D33" s="154"/>
@@ -5277,26 +5268,26 @@
     <row r="34" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
       <c r="B34" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C34" s="187" t="str">
+        <v>172</v>
+      </c>
+      <c r="C34" s="186" t="str">
         <f>VLOOKUP(B34,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D34" s="187"/>
-      <c r="E34" s="187" t="str">
+      <c r="D34" s="186"/>
+      <c r="E34" s="186" t="str">
         <f>VLOOKUP(B34,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F34" s="187"/>
+      <c r="F34" s="186"/>
       <c r="G34" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="153"/>
       <c r="B35" s="154" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C35" s="154"/>
       <c r="D35" s="154"/>
@@ -5307,26 +5298,26 @@
     <row r="36" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26"/>
       <c r="B36" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="C36" s="187" t="str">
+        <v>170</v>
+      </c>
+      <c r="C36" s="186" t="str">
         <f>VLOOKUP(B36,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D36" s="187"/>
-      <c r="E36" s="187" t="str">
+      <c r="D36" s="186"/>
+      <c r="E36" s="186" t="str">
         <f>VLOOKUP(B36,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F36" s="187"/>
+      <c r="F36" s="186"/>
       <c r="G36" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="153"/>
       <c r="B37" s="154" t="s">
-        <v>118</v>
+        <v>252</v>
       </c>
       <c r="C37" s="154"/>
       <c r="D37" s="154"/>
@@ -5337,26 +5328,26 @@
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
       <c r="B38" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C38" s="184" t="str">
+        <v>172</v>
+      </c>
+      <c r="C38" s="185" t="str">
         <f>VLOOKUP(B38,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D38" s="184"/>
-      <c r="E38" s="184" t="str">
+      <c r="D38" s="185"/>
+      <c r="E38" s="185" t="str">
         <f>VLOOKUP(B38,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F38" s="184"/>
+      <c r="F38" s="185"/>
       <c r="G38" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="153"/>
       <c r="B39" s="154" t="s">
-        <v>133</v>
+        <v>253</v>
       </c>
       <c r="C39" s="154"/>
       <c r="D39" s="154"/>
@@ -5367,56 +5358,56 @@
     <row r="40" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26"/>
       <c r="B40" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="C40" s="184" t="str">
+        <v>165</v>
+      </c>
+      <c r="C40" s="185" t="str">
         <f>VLOOKUP(B40,$B$50:$D$66,2,0)</f>
         <v>33 1862 1719</v>
       </c>
-      <c r="D40" s="184"/>
-      <c r="E40" s="184" t="str">
+      <c r="D40" s="185"/>
+      <c r="E40" s="185" t="str">
         <f>VLOOKUP(B40,$B$50:$D$66,3,0)</f>
         <v>rpulido@qualtop.com</v>
       </c>
-      <c r="F40" s="184"/>
+      <c r="F40" s="185"/>
       <c r="G40" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
       <c r="B41" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="C41" s="184" t="str">
+        <v>170</v>
+      </c>
+      <c r="C41" s="185" t="str">
         <f>VLOOKUP(B41,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D41" s="184"/>
-      <c r="E41" s="184" t="str">
+      <c r="D41" s="185"/>
+      <c r="E41" s="185" t="str">
         <f>VLOOKUP(B41,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F41" s="184"/>
+      <c r="F41" s="185"/>
       <c r="G41" s="163" t="s">
-        <v>204</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26"/>
       <c r="B42" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="184" t="e">
+        <v>76</v>
+      </c>
+      <c r="C42" s="185" t="e">
         <f>VLOOKUP(B42,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D42" s="184"/>
-      <c r="E42" s="184" t="e">
+      <c r="D42" s="185"/>
+      <c r="E42" s="185" t="e">
         <f>VLOOKUP(B42,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F42" s="184"/>
+      <c r="F42" s="185"/>
       <c r="G42" s="23"/>
     </row>
     <row r="43" spans="1:7" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5432,21 +5423,21 @@
     </row>
     <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
-      <c r="B44" s="188" t="s">
-        <v>75</v>
-      </c>
-      <c r="C44" s="188"/>
-      <c r="D44" s="188"/>
-      <c r="E44" s="188"/>
-      <c r="F44" s="188"/>
+      <c r="B44" s="184" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="184"/>
+      <c r="D44" s="184"/>
+      <c r="E44" s="184"/>
+      <c r="F44" s="184"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="188"/>
-      <c r="C45" s="188"/>
-      <c r="D45" s="188"/>
-      <c r="E45" s="188"/>
-      <c r="F45" s="188"/>
+      <c r="B45" s="184"/>
+      <c r="C45" s="184"/>
+      <c r="D45" s="184"/>
+      <c r="E45" s="184"/>
+      <c r="F45" s="184"/>
       <c r="G45" s="81"/>
     </row>
     <row r="46" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -5467,57 +5458,57 @@
     </row>
     <row r="50" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B50" s="84" t="s">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="C50" s="85" t="s">
-        <v>196</v>
+        <v>175</v>
       </c>
       <c r="D50" s="82" t="s">
-        <v>192</v>
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B51" s="84" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="C51" s="85" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
       <c r="D51" s="82" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B52" s="84" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C52" s="85" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
       <c r="D52" s="82" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B53" s="84" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="C53" s="85" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="D53" s="82" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B54" s="84" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="C54" s="85" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="D54" s="82" t="s">
-        <v>203</v>
+        <v>182</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -5583,6 +5574,33 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="43">
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="B44:F45"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E21:F21"/>
@@ -5599,33 +5617,6 @@
     <mergeCell ref="C41:D41"/>
     <mergeCell ref="E41:F41"/>
     <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E14:F14"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVM983093:WVM983106 JA50:JA66 SW50:SW66 ACS50:ACS66 AMO50:AMO66 AWK50:AWK66 BGG50:BGG66 BQC50:BQC66 BZY50:BZY66 CJU50:CJU66 CTQ50:CTQ66 DDM50:DDM66 DNI50:DNI66 DXE50:DXE66 EHA50:EHA66 EQW50:EQW66 FAS50:FAS66 FKO50:FKO66 FUK50:FUK66 GEG50:GEG66 GOC50:GOC66 GXY50:GXY66 HHU50:HHU66 HRQ50:HRQ66 IBM50:IBM66 ILI50:ILI66 IVE50:IVE66 JFA50:JFA66 JOW50:JOW66 JYS50:JYS66 KIO50:KIO66 KSK50:KSK66 LCG50:LCG66 LMC50:LMC66 LVY50:LVY66 MFU50:MFU66 MPQ50:MPQ66 MZM50:MZM66 NJI50:NJI66 NTE50:NTE66 ODA50:ODA66 OMW50:OMW66 OWS50:OWS66 PGO50:PGO66 PQK50:PQK66 QAG50:QAG66 QKC50:QKC66 QTY50:QTY66 RDU50:RDU66 RNQ50:RNQ66 RXM50:RXM66 SHI50:SHI66 SRE50:SRE66 TBA50:TBA66 TKW50:TKW66 TUS50:TUS66 UEO50:UEO66 UOK50:UOK66 UYG50:UYG66 VIC50:VIC66 VRY50:VRY66 WBU50:WBU66 WLQ50:WLQ66 WVM50:WVM66 D65570:D65583 JA65589:JA65602 SW65589:SW65602 ACS65589:ACS65602 AMO65589:AMO65602 AWK65589:AWK65602 BGG65589:BGG65602 BQC65589:BQC65602 BZY65589:BZY65602 CJU65589:CJU65602 CTQ65589:CTQ65602 DDM65589:DDM65602 DNI65589:DNI65602 DXE65589:DXE65602 EHA65589:EHA65602 EQW65589:EQW65602 FAS65589:FAS65602 FKO65589:FKO65602 FUK65589:FUK65602 GEG65589:GEG65602 GOC65589:GOC65602 GXY65589:GXY65602 HHU65589:HHU65602 HRQ65589:HRQ65602 IBM65589:IBM65602 ILI65589:ILI65602 IVE65589:IVE65602 JFA65589:JFA65602 JOW65589:JOW65602 JYS65589:JYS65602 KIO65589:KIO65602 KSK65589:KSK65602 LCG65589:LCG65602 LMC65589:LMC65602 LVY65589:LVY65602 MFU65589:MFU65602 MPQ65589:MPQ65602 MZM65589:MZM65602 NJI65589:NJI65602 NTE65589:NTE65602 ODA65589:ODA65602 OMW65589:OMW65602 OWS65589:OWS65602 PGO65589:PGO65602 PQK65589:PQK65602 QAG65589:QAG65602 QKC65589:QKC65602 QTY65589:QTY65602 RDU65589:RDU65602 RNQ65589:RNQ65602 RXM65589:RXM65602 SHI65589:SHI65602 SRE65589:SRE65602 TBA65589:TBA65602 TKW65589:TKW65602 TUS65589:TUS65602 UEO65589:UEO65602 UOK65589:UOK65602 UYG65589:UYG65602 VIC65589:VIC65602 VRY65589:VRY65602 WBU65589:WBU65602 WLQ65589:WLQ65602 WVM65589:WVM65602 D131106:D131119 JA131125:JA131138 SW131125:SW131138 ACS131125:ACS131138 AMO131125:AMO131138 AWK131125:AWK131138 BGG131125:BGG131138 BQC131125:BQC131138 BZY131125:BZY131138 CJU131125:CJU131138 CTQ131125:CTQ131138 DDM131125:DDM131138 DNI131125:DNI131138 DXE131125:DXE131138 EHA131125:EHA131138 EQW131125:EQW131138 FAS131125:FAS131138 FKO131125:FKO131138 FUK131125:FUK131138 GEG131125:GEG131138 GOC131125:GOC131138 GXY131125:GXY131138 HHU131125:HHU131138 HRQ131125:HRQ131138 IBM131125:IBM131138 ILI131125:ILI131138 IVE131125:IVE131138 JFA131125:JFA131138 JOW131125:JOW131138 JYS131125:JYS131138 KIO131125:KIO131138 KSK131125:KSK131138 LCG131125:LCG131138 LMC131125:LMC131138 LVY131125:LVY131138 MFU131125:MFU131138 MPQ131125:MPQ131138 MZM131125:MZM131138 NJI131125:NJI131138 NTE131125:NTE131138 ODA131125:ODA131138 OMW131125:OMW131138 OWS131125:OWS131138 PGO131125:PGO131138 PQK131125:PQK131138 QAG131125:QAG131138 QKC131125:QKC131138 QTY131125:QTY131138 RDU131125:RDU131138 RNQ131125:RNQ131138 RXM131125:RXM131138 SHI131125:SHI131138 SRE131125:SRE131138 TBA131125:TBA131138 TKW131125:TKW131138 TUS131125:TUS131138 UEO131125:UEO131138 UOK131125:UOK131138 UYG131125:UYG131138 VIC131125:VIC131138 VRY131125:VRY131138 WBU131125:WBU131138 WLQ131125:WLQ131138 WVM131125:WVM131138 D196642:D196655 JA196661:JA196674 SW196661:SW196674 ACS196661:ACS196674 AMO196661:AMO196674 AWK196661:AWK196674 BGG196661:BGG196674 BQC196661:BQC196674 BZY196661:BZY196674 CJU196661:CJU196674 CTQ196661:CTQ196674 DDM196661:DDM196674 DNI196661:DNI196674 DXE196661:DXE196674 EHA196661:EHA196674 EQW196661:EQW196674 FAS196661:FAS196674 FKO196661:FKO196674 FUK196661:FUK196674 GEG196661:GEG196674 GOC196661:GOC196674 GXY196661:GXY196674 HHU196661:HHU196674 HRQ196661:HRQ196674 IBM196661:IBM196674 ILI196661:ILI196674 IVE196661:IVE196674 JFA196661:JFA196674 JOW196661:JOW196674 JYS196661:JYS196674 KIO196661:KIO196674 KSK196661:KSK196674 LCG196661:LCG196674 LMC196661:LMC196674 LVY196661:LVY196674 MFU196661:MFU196674 MPQ196661:MPQ196674 MZM196661:MZM196674 NJI196661:NJI196674 NTE196661:NTE196674 ODA196661:ODA196674 OMW196661:OMW196674 OWS196661:OWS196674 PGO196661:PGO196674 PQK196661:PQK196674 QAG196661:QAG196674 QKC196661:QKC196674 QTY196661:QTY196674 RDU196661:RDU196674 RNQ196661:RNQ196674 RXM196661:RXM196674 SHI196661:SHI196674 SRE196661:SRE196674 TBA196661:TBA196674 TKW196661:TKW196674 TUS196661:TUS196674 UEO196661:UEO196674 UOK196661:UOK196674 UYG196661:UYG196674 VIC196661:VIC196674 VRY196661:VRY196674 WBU196661:WBU196674 WLQ196661:WLQ196674 WVM196661:WVM196674 D262178:D262191 JA262197:JA262210 SW262197:SW262210 ACS262197:ACS262210 AMO262197:AMO262210 AWK262197:AWK262210 BGG262197:BGG262210 BQC262197:BQC262210 BZY262197:BZY262210 CJU262197:CJU262210 CTQ262197:CTQ262210 DDM262197:DDM262210 DNI262197:DNI262210 DXE262197:DXE262210 EHA262197:EHA262210 EQW262197:EQW262210 FAS262197:FAS262210 FKO262197:FKO262210 FUK262197:FUK262210 GEG262197:GEG262210 GOC262197:GOC262210 GXY262197:GXY262210 HHU262197:HHU262210 HRQ262197:HRQ262210 IBM262197:IBM262210 ILI262197:ILI262210 IVE262197:IVE262210 JFA262197:JFA262210 JOW262197:JOW262210 JYS262197:JYS262210 KIO262197:KIO262210 KSK262197:KSK262210 LCG262197:LCG262210 LMC262197:LMC262210 LVY262197:LVY262210 MFU262197:MFU262210 MPQ262197:MPQ262210 MZM262197:MZM262210 NJI262197:NJI262210 NTE262197:NTE262210 ODA262197:ODA262210 OMW262197:OMW262210 OWS262197:OWS262210 PGO262197:PGO262210 PQK262197:PQK262210 QAG262197:QAG262210 QKC262197:QKC262210 QTY262197:QTY262210 RDU262197:RDU262210 RNQ262197:RNQ262210 RXM262197:RXM262210 SHI262197:SHI262210 SRE262197:SRE262210 TBA262197:TBA262210 TKW262197:TKW262210 TUS262197:TUS262210 UEO262197:UEO262210 UOK262197:UOK262210 UYG262197:UYG262210 VIC262197:VIC262210 VRY262197:VRY262210 WBU262197:WBU262210 WLQ262197:WLQ262210 WVM262197:WVM262210 D327714:D327727 JA327733:JA327746 SW327733:SW327746 ACS327733:ACS327746 AMO327733:AMO327746 AWK327733:AWK327746 BGG327733:BGG327746 BQC327733:BQC327746 BZY327733:BZY327746 CJU327733:CJU327746 CTQ327733:CTQ327746 DDM327733:DDM327746 DNI327733:DNI327746 DXE327733:DXE327746 EHA327733:EHA327746 EQW327733:EQW327746 FAS327733:FAS327746 FKO327733:FKO327746 FUK327733:FUK327746 GEG327733:GEG327746 GOC327733:GOC327746 GXY327733:GXY327746 HHU327733:HHU327746 HRQ327733:HRQ327746 IBM327733:IBM327746 ILI327733:ILI327746 IVE327733:IVE327746 JFA327733:JFA327746 JOW327733:JOW327746 JYS327733:JYS327746 KIO327733:KIO327746 KSK327733:KSK327746 LCG327733:LCG327746 LMC327733:LMC327746 LVY327733:LVY327746 MFU327733:MFU327746 MPQ327733:MPQ327746 MZM327733:MZM327746 NJI327733:NJI327746 NTE327733:NTE327746 ODA327733:ODA327746 OMW327733:OMW327746 OWS327733:OWS327746 PGO327733:PGO327746 PQK327733:PQK327746 QAG327733:QAG327746 QKC327733:QKC327746 QTY327733:QTY327746 RDU327733:RDU327746 RNQ327733:RNQ327746 RXM327733:RXM327746 SHI327733:SHI327746 SRE327733:SRE327746 TBA327733:TBA327746 TKW327733:TKW327746 TUS327733:TUS327746 UEO327733:UEO327746 UOK327733:UOK327746 UYG327733:UYG327746 VIC327733:VIC327746 VRY327733:VRY327746 WBU327733:WBU327746 WLQ327733:WLQ327746 WVM327733:WVM327746 D393250:D393263 JA393269:JA393282 SW393269:SW393282 ACS393269:ACS393282 AMO393269:AMO393282 AWK393269:AWK393282 BGG393269:BGG393282 BQC393269:BQC393282 BZY393269:BZY393282 CJU393269:CJU393282 CTQ393269:CTQ393282 DDM393269:DDM393282 DNI393269:DNI393282 DXE393269:DXE393282 EHA393269:EHA393282 EQW393269:EQW393282 FAS393269:FAS393282 FKO393269:FKO393282 FUK393269:FUK393282 GEG393269:GEG393282 GOC393269:GOC393282 GXY393269:GXY393282 HHU393269:HHU393282 HRQ393269:HRQ393282 IBM393269:IBM393282 ILI393269:ILI393282 IVE393269:IVE393282 JFA393269:JFA393282 JOW393269:JOW393282 JYS393269:JYS393282 KIO393269:KIO393282 KSK393269:KSK393282 LCG393269:LCG393282 LMC393269:LMC393282 LVY393269:LVY393282 MFU393269:MFU393282 MPQ393269:MPQ393282 MZM393269:MZM393282 NJI393269:NJI393282 NTE393269:NTE393282 ODA393269:ODA393282 OMW393269:OMW393282 OWS393269:OWS393282 PGO393269:PGO393282 PQK393269:PQK393282 QAG393269:QAG393282 QKC393269:QKC393282 QTY393269:QTY393282 RDU393269:RDU393282 RNQ393269:RNQ393282 RXM393269:RXM393282 SHI393269:SHI393282 SRE393269:SRE393282 TBA393269:TBA393282 TKW393269:TKW393282 TUS393269:TUS393282 UEO393269:UEO393282 UOK393269:UOK393282 UYG393269:UYG393282 VIC393269:VIC393282 VRY393269:VRY393282 WBU393269:WBU393282 WLQ393269:WLQ393282 WVM393269:WVM393282 D458786:D458799 JA458805:JA458818 SW458805:SW458818 ACS458805:ACS458818 AMO458805:AMO458818 AWK458805:AWK458818 BGG458805:BGG458818 BQC458805:BQC458818 BZY458805:BZY458818 CJU458805:CJU458818 CTQ458805:CTQ458818 DDM458805:DDM458818 DNI458805:DNI458818 DXE458805:DXE458818 EHA458805:EHA458818 EQW458805:EQW458818 FAS458805:FAS458818 FKO458805:FKO458818 FUK458805:FUK458818 GEG458805:GEG458818 GOC458805:GOC458818 GXY458805:GXY458818 HHU458805:HHU458818 HRQ458805:HRQ458818 IBM458805:IBM458818 ILI458805:ILI458818 IVE458805:IVE458818 JFA458805:JFA458818 JOW458805:JOW458818 JYS458805:JYS458818 KIO458805:KIO458818 KSK458805:KSK458818 LCG458805:LCG458818 LMC458805:LMC458818 LVY458805:LVY458818 MFU458805:MFU458818 MPQ458805:MPQ458818 MZM458805:MZM458818 NJI458805:NJI458818 NTE458805:NTE458818 ODA458805:ODA458818 OMW458805:OMW458818 OWS458805:OWS458818 PGO458805:PGO458818 PQK458805:PQK458818 QAG458805:QAG458818 QKC458805:QKC458818 QTY458805:QTY458818 RDU458805:RDU458818 RNQ458805:RNQ458818 RXM458805:RXM458818 SHI458805:SHI458818 SRE458805:SRE458818 TBA458805:TBA458818 TKW458805:TKW458818 TUS458805:TUS458818 UEO458805:UEO458818 UOK458805:UOK458818 UYG458805:UYG458818 VIC458805:VIC458818 VRY458805:VRY458818 WBU458805:WBU458818 WLQ458805:WLQ458818 WVM458805:WVM458818 D524322:D524335 JA524341:JA524354 SW524341:SW524354 ACS524341:ACS524354 AMO524341:AMO524354 AWK524341:AWK524354 BGG524341:BGG524354 BQC524341:BQC524354 BZY524341:BZY524354 CJU524341:CJU524354 CTQ524341:CTQ524354 DDM524341:DDM524354 DNI524341:DNI524354 DXE524341:DXE524354 EHA524341:EHA524354 EQW524341:EQW524354 FAS524341:FAS524354 FKO524341:FKO524354 FUK524341:FUK524354 GEG524341:GEG524354 GOC524341:GOC524354 GXY524341:GXY524354 HHU524341:HHU524354 HRQ524341:HRQ524354 IBM524341:IBM524354 ILI524341:ILI524354 IVE524341:IVE524354 JFA524341:JFA524354 JOW524341:JOW524354 JYS524341:JYS524354 KIO524341:KIO524354 KSK524341:KSK524354 LCG524341:LCG524354 LMC524341:LMC524354 LVY524341:LVY524354 MFU524341:MFU524354 MPQ524341:MPQ524354 MZM524341:MZM524354 NJI524341:NJI524354 NTE524341:NTE524354 ODA524341:ODA524354 OMW524341:OMW524354 OWS524341:OWS524354 PGO524341:PGO524354 PQK524341:PQK524354 QAG524341:QAG524354 QKC524341:QKC524354 QTY524341:QTY524354 RDU524341:RDU524354 RNQ524341:RNQ524354 RXM524341:RXM524354 SHI524341:SHI524354 SRE524341:SRE524354 TBA524341:TBA524354 TKW524341:TKW524354 TUS524341:TUS524354 UEO524341:UEO524354 UOK524341:UOK524354 UYG524341:UYG524354 VIC524341:VIC524354 VRY524341:VRY524354 WBU524341:WBU524354 WLQ524341:WLQ524354 WVM524341:WVM524354 D589858:D589871 JA589877:JA589890 SW589877:SW589890 ACS589877:ACS589890 AMO589877:AMO589890 AWK589877:AWK589890 BGG589877:BGG589890 BQC589877:BQC589890 BZY589877:BZY589890 CJU589877:CJU589890 CTQ589877:CTQ589890 DDM589877:DDM589890 DNI589877:DNI589890 DXE589877:DXE589890 EHA589877:EHA589890 EQW589877:EQW589890 FAS589877:FAS589890 FKO589877:FKO589890 FUK589877:FUK589890 GEG589877:GEG589890 GOC589877:GOC589890 GXY589877:GXY589890 HHU589877:HHU589890 HRQ589877:HRQ589890 IBM589877:IBM589890 ILI589877:ILI589890 IVE589877:IVE589890 JFA589877:JFA589890 JOW589877:JOW589890 JYS589877:JYS589890 KIO589877:KIO589890 KSK589877:KSK589890 LCG589877:LCG589890 LMC589877:LMC589890 LVY589877:LVY589890 MFU589877:MFU589890 MPQ589877:MPQ589890 MZM589877:MZM589890 NJI589877:NJI589890 NTE589877:NTE589890 ODA589877:ODA589890 OMW589877:OMW589890 OWS589877:OWS589890 PGO589877:PGO589890 PQK589877:PQK589890 QAG589877:QAG589890 QKC589877:QKC589890 QTY589877:QTY589890 RDU589877:RDU589890 RNQ589877:RNQ589890 RXM589877:RXM589890 SHI589877:SHI589890 SRE589877:SRE589890 TBA589877:TBA589890 TKW589877:TKW589890 TUS589877:TUS589890 UEO589877:UEO589890 UOK589877:UOK589890 UYG589877:UYG589890 VIC589877:VIC589890 VRY589877:VRY589890 WBU589877:WBU589890 WLQ589877:WLQ589890 WVM589877:WVM589890 D655394:D655407 JA655413:JA655426 SW655413:SW655426 ACS655413:ACS655426 AMO655413:AMO655426 AWK655413:AWK655426 BGG655413:BGG655426 BQC655413:BQC655426 BZY655413:BZY655426 CJU655413:CJU655426 CTQ655413:CTQ655426 DDM655413:DDM655426 DNI655413:DNI655426 DXE655413:DXE655426 EHA655413:EHA655426 EQW655413:EQW655426 FAS655413:FAS655426 FKO655413:FKO655426 FUK655413:FUK655426 GEG655413:GEG655426 GOC655413:GOC655426 GXY655413:GXY655426 HHU655413:HHU655426 HRQ655413:HRQ655426 IBM655413:IBM655426 ILI655413:ILI655426 IVE655413:IVE655426 JFA655413:JFA655426 JOW655413:JOW655426 JYS655413:JYS655426 KIO655413:KIO655426 KSK655413:KSK655426 LCG655413:LCG655426 LMC655413:LMC655426 LVY655413:LVY655426 MFU655413:MFU655426 MPQ655413:MPQ655426 MZM655413:MZM655426 NJI655413:NJI655426 NTE655413:NTE655426 ODA655413:ODA655426 OMW655413:OMW655426 OWS655413:OWS655426 PGO655413:PGO655426 PQK655413:PQK655426 QAG655413:QAG655426 QKC655413:QKC655426 QTY655413:QTY655426 RDU655413:RDU655426 RNQ655413:RNQ655426 RXM655413:RXM655426 SHI655413:SHI655426 SRE655413:SRE655426 TBA655413:TBA655426 TKW655413:TKW655426 TUS655413:TUS655426 UEO655413:UEO655426 UOK655413:UOK655426 UYG655413:UYG655426 VIC655413:VIC655426 VRY655413:VRY655426 WBU655413:WBU655426 WLQ655413:WLQ655426 WVM655413:WVM655426 D720930:D720943 JA720949:JA720962 SW720949:SW720962 ACS720949:ACS720962 AMO720949:AMO720962 AWK720949:AWK720962 BGG720949:BGG720962 BQC720949:BQC720962 BZY720949:BZY720962 CJU720949:CJU720962 CTQ720949:CTQ720962 DDM720949:DDM720962 DNI720949:DNI720962 DXE720949:DXE720962 EHA720949:EHA720962 EQW720949:EQW720962 FAS720949:FAS720962 FKO720949:FKO720962 FUK720949:FUK720962 GEG720949:GEG720962 GOC720949:GOC720962 GXY720949:GXY720962 HHU720949:HHU720962 HRQ720949:HRQ720962 IBM720949:IBM720962 ILI720949:ILI720962 IVE720949:IVE720962 JFA720949:JFA720962 JOW720949:JOW720962 JYS720949:JYS720962 KIO720949:KIO720962 KSK720949:KSK720962 LCG720949:LCG720962 LMC720949:LMC720962 LVY720949:LVY720962 MFU720949:MFU720962 MPQ720949:MPQ720962 MZM720949:MZM720962 NJI720949:NJI720962 NTE720949:NTE720962 ODA720949:ODA720962 OMW720949:OMW720962 OWS720949:OWS720962 PGO720949:PGO720962 PQK720949:PQK720962 QAG720949:QAG720962 QKC720949:QKC720962 QTY720949:QTY720962 RDU720949:RDU720962 RNQ720949:RNQ720962 RXM720949:RXM720962 SHI720949:SHI720962 SRE720949:SRE720962 TBA720949:TBA720962 TKW720949:TKW720962 TUS720949:TUS720962 UEO720949:UEO720962 UOK720949:UOK720962 UYG720949:UYG720962 VIC720949:VIC720962 VRY720949:VRY720962 WBU720949:WBU720962 WLQ720949:WLQ720962 WVM720949:WVM720962 D786466:D786479 JA786485:JA786498 SW786485:SW786498 ACS786485:ACS786498 AMO786485:AMO786498 AWK786485:AWK786498 BGG786485:BGG786498 BQC786485:BQC786498 BZY786485:BZY786498 CJU786485:CJU786498 CTQ786485:CTQ786498 DDM786485:DDM786498 DNI786485:DNI786498 DXE786485:DXE786498 EHA786485:EHA786498 EQW786485:EQW786498 FAS786485:FAS786498 FKO786485:FKO786498 FUK786485:FUK786498 GEG786485:GEG786498 GOC786485:GOC786498 GXY786485:GXY786498 HHU786485:HHU786498 HRQ786485:HRQ786498 IBM786485:IBM786498 ILI786485:ILI786498 IVE786485:IVE786498 JFA786485:JFA786498 JOW786485:JOW786498 JYS786485:JYS786498 KIO786485:KIO786498 KSK786485:KSK786498 LCG786485:LCG786498 LMC786485:LMC786498 LVY786485:LVY786498 MFU786485:MFU786498 MPQ786485:MPQ786498 MZM786485:MZM786498 NJI786485:NJI786498 NTE786485:NTE786498 ODA786485:ODA786498 OMW786485:OMW786498 OWS786485:OWS786498 PGO786485:PGO786498 PQK786485:PQK786498 QAG786485:QAG786498 QKC786485:QKC786498 QTY786485:QTY786498 RDU786485:RDU786498 RNQ786485:RNQ786498 RXM786485:RXM786498 SHI786485:SHI786498 SRE786485:SRE786498 TBA786485:TBA786498 TKW786485:TKW786498 TUS786485:TUS786498 UEO786485:UEO786498 UOK786485:UOK786498 UYG786485:UYG786498 VIC786485:VIC786498 VRY786485:VRY786498 WBU786485:WBU786498 WLQ786485:WLQ786498 WVM786485:WVM786498 D852002:D852015 JA852021:JA852034 SW852021:SW852034 ACS852021:ACS852034 AMO852021:AMO852034 AWK852021:AWK852034 BGG852021:BGG852034 BQC852021:BQC852034 BZY852021:BZY852034 CJU852021:CJU852034 CTQ852021:CTQ852034 DDM852021:DDM852034 DNI852021:DNI852034 DXE852021:DXE852034 EHA852021:EHA852034 EQW852021:EQW852034 FAS852021:FAS852034 FKO852021:FKO852034 FUK852021:FUK852034 GEG852021:GEG852034 GOC852021:GOC852034 GXY852021:GXY852034 HHU852021:HHU852034 HRQ852021:HRQ852034 IBM852021:IBM852034 ILI852021:ILI852034 IVE852021:IVE852034 JFA852021:JFA852034 JOW852021:JOW852034 JYS852021:JYS852034 KIO852021:KIO852034 KSK852021:KSK852034 LCG852021:LCG852034 LMC852021:LMC852034 LVY852021:LVY852034 MFU852021:MFU852034 MPQ852021:MPQ852034 MZM852021:MZM852034 NJI852021:NJI852034 NTE852021:NTE852034 ODA852021:ODA852034 OMW852021:OMW852034 OWS852021:OWS852034 PGO852021:PGO852034 PQK852021:PQK852034 QAG852021:QAG852034 QKC852021:QKC852034 QTY852021:QTY852034 RDU852021:RDU852034 RNQ852021:RNQ852034 RXM852021:RXM852034 SHI852021:SHI852034 SRE852021:SRE852034 TBA852021:TBA852034 TKW852021:TKW852034 TUS852021:TUS852034 UEO852021:UEO852034 UOK852021:UOK852034 UYG852021:UYG852034 VIC852021:VIC852034 VRY852021:VRY852034 WBU852021:WBU852034 WLQ852021:WLQ852034 WVM852021:WVM852034 D917538:D917551 JA917557:JA917570 SW917557:SW917570 ACS917557:ACS917570 AMO917557:AMO917570 AWK917557:AWK917570 BGG917557:BGG917570 BQC917557:BQC917570 BZY917557:BZY917570 CJU917557:CJU917570 CTQ917557:CTQ917570 DDM917557:DDM917570 DNI917557:DNI917570 DXE917557:DXE917570 EHA917557:EHA917570 EQW917557:EQW917570 FAS917557:FAS917570 FKO917557:FKO917570 FUK917557:FUK917570 GEG917557:GEG917570 GOC917557:GOC917570 GXY917557:GXY917570 HHU917557:HHU917570 HRQ917557:HRQ917570 IBM917557:IBM917570 ILI917557:ILI917570 IVE917557:IVE917570 JFA917557:JFA917570 JOW917557:JOW917570 JYS917557:JYS917570 KIO917557:KIO917570 KSK917557:KSK917570 LCG917557:LCG917570 LMC917557:LMC917570 LVY917557:LVY917570 MFU917557:MFU917570 MPQ917557:MPQ917570 MZM917557:MZM917570 NJI917557:NJI917570 NTE917557:NTE917570 ODA917557:ODA917570 OMW917557:OMW917570 OWS917557:OWS917570 PGO917557:PGO917570 PQK917557:PQK917570 QAG917557:QAG917570 QKC917557:QKC917570 QTY917557:QTY917570 RDU917557:RDU917570 RNQ917557:RNQ917570 RXM917557:RXM917570 SHI917557:SHI917570 SRE917557:SRE917570 TBA917557:TBA917570 TKW917557:TKW917570 TUS917557:TUS917570 UEO917557:UEO917570 UOK917557:UOK917570 UYG917557:UYG917570 VIC917557:VIC917570 VRY917557:VRY917570 WBU917557:WBU917570 WLQ917557:WLQ917570 WVM917557:WVM917570 D983074:D983087 JA983093:JA983106 SW983093:SW983106 ACS983093:ACS983106 AMO983093:AMO983106 AWK983093:AWK983106 BGG983093:BGG983106 BQC983093:BQC983106 BZY983093:BZY983106 CJU983093:CJU983106 CTQ983093:CTQ983106 DDM983093:DDM983106 DNI983093:DNI983106 DXE983093:DXE983106 EHA983093:EHA983106 EQW983093:EQW983106 FAS983093:FAS983106 FKO983093:FKO983106 FUK983093:FUK983106 GEG983093:GEG983106 GOC983093:GOC983106 GXY983093:GXY983106 HHU983093:HHU983106 HRQ983093:HRQ983106 IBM983093:IBM983106 ILI983093:ILI983106 IVE983093:IVE983106 JFA983093:JFA983106 JOW983093:JOW983106 JYS983093:JYS983106 KIO983093:KIO983106 KSK983093:KSK983106 LCG983093:LCG983106 LMC983093:LMC983106 LVY983093:LVY983106 MFU983093:MFU983106 MPQ983093:MPQ983106 MZM983093:MZM983106 NJI983093:NJI983106 NTE983093:NTE983106 ODA983093:ODA983106 OMW983093:OMW983106 OWS983093:OWS983106 PGO983093:PGO983106 PQK983093:PQK983106 QAG983093:QAG983106 QKC983093:QKC983106 QTY983093:QTY983106 RDU983093:RDU983106 RNQ983093:RNQ983106 RXM983093:RXM983106 SHI983093:SHI983106 SRE983093:SRE983106 TBA983093:TBA983106 TKW983093:TKW983106 TUS983093:TUS983106 UEO983093:UEO983106 UOK983093:UOK983106 UYG983093:UYG983106 VIC983093:VIC983106 VRY983093:VRY983106 WBU983093:WBU983106 WLQ983093:WLQ983106">
@@ -5645,21 +5636,21 @@
     <hyperlink ref="D52" r:id="rId4"/>
     <hyperlink ref="D53" r:id="rId5"/>
     <hyperlink ref="D54" r:id="rId6"/>
-    <hyperlink ref="G10" r:id="rId7"/>
-    <hyperlink ref="G12" r:id="rId8"/>
-    <hyperlink ref="G14" r:id="rId9"/>
-    <hyperlink ref="G17" r:id="rId10"/>
-    <hyperlink ref="G21" r:id="rId11"/>
-    <hyperlink ref="G24" r:id="rId12"/>
-    <hyperlink ref="G26" r:id="rId13"/>
-    <hyperlink ref="G28" r:id="rId14"/>
-    <hyperlink ref="G30" r:id="rId15"/>
-    <hyperlink ref="G32" r:id="rId16"/>
-    <hyperlink ref="G34" r:id="rId17"/>
-    <hyperlink ref="G36" r:id="rId18"/>
-    <hyperlink ref="G38" r:id="rId19"/>
-    <hyperlink ref="G40" r:id="rId20"/>
-    <hyperlink ref="G41" r:id="rId21"/>
+    <hyperlink ref="G10" r:id="rId7" display="Vease en matriz de roles"/>
+    <hyperlink ref="G12" r:id="rId8" display="Vease en matriz de roles"/>
+    <hyperlink ref="G14" r:id="rId9" display="Vease en matriz de roles"/>
+    <hyperlink ref="G17" r:id="rId10" display="Vease en matriz de roles"/>
+    <hyperlink ref="G21" r:id="rId11" display="Vease en matriz de roles"/>
+    <hyperlink ref="G24" r:id="rId12" display="Vease en matriz de roles"/>
+    <hyperlink ref="G26" r:id="rId13" display="Vease en matriz de roles"/>
+    <hyperlink ref="G28" r:id="rId14" display="Vease en matriz de roles"/>
+    <hyperlink ref="G30" r:id="rId15" display="Vease en matriz de roles"/>
+    <hyperlink ref="G32" r:id="rId16" display="Vease en matriz de roles"/>
+    <hyperlink ref="G34" r:id="rId17" display="Vease en matriz de roles"/>
+    <hyperlink ref="G36" r:id="rId18" display="Vease en matriz de roles"/>
+    <hyperlink ref="G38" r:id="rId19" display="Vease en matriz de roles"/>
+    <hyperlink ref="G40" r:id="rId20" display="Vease en matriz de roles"/>
+    <hyperlink ref="G41" r:id="rId21" display="Vease en matriz de roles"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId22"/>
@@ -5680,7 +5671,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6461,7 +6452,7 @@
     <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -6493,56 +6484,56 @@
     <row r="4" spans="1:12" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>211</v>
+        <v>257</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>209</v>
+        <v>258</v>
       </c>
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:12" s="10" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>277</v>
+        <v>223</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>210</v>
+        <v>259</v>
       </c>
       <c r="G5" s="12"/>
       <c r="L5" s="82"/>
     </row>
     <row r="6" spans="1:12" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>274</v>
+        <v>222</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>207</v>
+        <v>255</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>278</v>
+        <v>224</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>279</v>
+        <v>225</v>
       </c>
       <c r="G6" s="12"/>
       <c r="L6" s="82"/>
@@ -6635,9 +6626,9 @@
   <dimension ref="A1:JI112"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="R13" sqref="R13"/>
+      <selection pane="bottomLeft" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7611,7 +7602,7 @@
     <row r="2" spans="1:269" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="132"/>
       <c r="B2" s="133" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2" s="133"/>
       <c r="D2" s="132"/>
@@ -7630,10 +7621,10 @@
       <c r="Q2" s="132"/>
       <c r="R2" s="132"/>
       <c r="S2" s="189" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="JB2" s="160" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="JC2" s="27">
         <v>5</v>
@@ -7657,60 +7648,60 @@
     </row>
     <row r="3" spans="1:269" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>37</v>
-      </c>
       <c r="J3" s="38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K3" s="37"/>
       <c r="L3" s="57" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M3" s="57" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="N3" s="38" t="s">
+        <v>264</v>
+      </c>
+      <c r="O3" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="P3" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="38" t="s">
         <v>59</v>
-      </c>
-      <c r="O3" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="P3" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q3" s="38" t="s">
-        <v>141</v>
       </c>
       <c r="R3" s="38" t="s">
         <v>11</v>
       </c>
       <c r="S3" s="189"/>
       <c r="JB3" s="160" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="JC3" s="27">
         <v>4</v>
@@ -7735,7 +7726,7 @@
     <row r="4" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="165"/>
       <c r="B4" s="164" t="s">
-        <v>219</v>
+        <v>190</v>
       </c>
       <c r="C4" s="164"/>
       <c r="D4" s="166"/>
@@ -7755,7 +7746,7 @@
       <c r="R4" s="169"/>
       <c r="S4" s="189"/>
       <c r="JB4" s="160" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="JC4" s="27">
         <v>3</v>
@@ -7782,19 +7773,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>212</v>
+        <v>265</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>213</v>
+        <v>266</v>
       </c>
       <c r="D5" s="73" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G5" s="141">
         <v>1</v>
@@ -7803,29 +7794,29 @@
         <v>3</v>
       </c>
       <c r="I5" s="138" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="137" t="s">
         <v>39</v>
-      </c>
-      <c r="J5" s="137" t="s">
-        <v>40</v>
       </c>
       <c r="K5" s="35"/>
       <c r="L5" s="54" t="s">
-        <v>236</v>
+        <v>267</v>
       </c>
       <c r="M5" s="175" t="s">
-        <v>237</v>
+        <v>268</v>
       </c>
       <c r="N5" s="175" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="O5" s="52" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
       <c r="P5" s="52" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="Q5" s="52" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="R5" s="42"/>
       <c r="S5" s="189"/>
@@ -7842,19 +7833,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>214</v>
+        <v>269</v>
       </c>
       <c r="D6" s="73" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G6" s="141">
         <v>2</v>
@@ -7863,34 +7854,34 @@
         <v>1</v>
       </c>
       <c r="I6" s="139" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6" s="137" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="K6" s="35"/>
       <c r="L6" s="53" t="s">
-        <v>241</v>
+        <v>207</v>
       </c>
       <c r="M6" s="175" t="s">
-        <v>242</v>
+        <v>270</v>
       </c>
       <c r="N6" s="175" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
       <c r="O6" s="52" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="P6" s="52" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
       <c r="Q6" s="52" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="R6" s="59"/>
       <c r="S6" s="189"/>
       <c r="JB6" s="160" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="JC6" s="27">
         <v>2</v>
@@ -7917,19 +7908,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="53" t="s">
-        <v>215</v>
+        <v>186</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>216</v>
+        <v>187</v>
       </c>
       <c r="D7" s="73" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="G7" s="141">
         <v>2</v>
@@ -7938,34 +7929,34 @@
         <v>1</v>
       </c>
       <c r="I7" s="138" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7" s="137" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" s="35"/>
       <c r="L7" s="53" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="M7" s="175" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="N7" s="175" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="O7" s="52" t="s">
-        <v>250</v>
+        <v>275</v>
       </c>
       <c r="P7" s="52" t="s">
-        <v>251</v>
+        <v>211</v>
       </c>
       <c r="Q7" s="52" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="R7" s="59"/>
       <c r="S7" s="189"/>
       <c r="JB7" s="160" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="JC7" s="27">
         <v>1</v>
@@ -7992,19 +7983,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>217</v>
+        <v>188</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="D8" s="73" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G8" s="141">
         <v>1</v>
@@ -8013,29 +8004,29 @@
         <v>1</v>
       </c>
       <c r="I8" s="139" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J8" s="137" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K8" s="35"/>
       <c r="L8" s="53" t="s">
-        <v>253</v>
+        <v>276</v>
       </c>
       <c r="M8" s="175" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="N8" s="175" t="s">
-        <v>255</v>
+        <v>213</v>
       </c>
       <c r="O8" s="52" t="s">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="P8" s="52" t="s">
-        <v>257</v>
+        <v>214</v>
       </c>
       <c r="Q8" s="52" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="R8" s="59"/>
       <c r="JC8" s="32"/>
@@ -8059,7 +8050,7 @@
     <row r="9" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="171"/>
       <c r="B9" s="172" t="s">
-        <v>220</v>
+        <v>191</v>
       </c>
       <c r="C9" s="164"/>
       <c r="D9" s="166"/>
@@ -8079,19 +8070,19 @@
       <c r="R9" s="174"/>
       <c r="JC9" s="32"/>
       <c r="JD9" s="160" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="JE9" s="160" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="JF9" s="160" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="JG9" s="160" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="JH9" s="160" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="JI9" s="32"/>
     </row>
@@ -8100,19 +8091,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>224</v>
+        <v>279</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="D10" s="73" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G10" s="141">
         <v>1</v>
@@ -8121,35 +8112,35 @@
         <v>1</v>
       </c>
       <c r="I10" s="139" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="137" t="s">
         <v>38</v>
-      </c>
-      <c r="J10" s="137" t="s">
-        <v>39</v>
       </c>
       <c r="K10" s="35"/>
       <c r="L10" s="53" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="M10" s="175" t="s">
-        <v>259</v>
+        <v>281</v>
       </c>
       <c r="N10" s="36" t="s">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="O10" s="52" t="s">
-        <v>261</v>
+        <v>282</v>
       </c>
       <c r="P10" s="52" t="s">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="Q10" s="52" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="R10" s="59"/>
       <c r="JC10" s="32"/>
       <c r="JD10" s="32"/>
       <c r="JE10" s="160" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="JF10" s="34"/>
       <c r="JG10" s="34"/>
@@ -8161,19 +8152,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>223</v>
+        <v>194</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="D11" s="73" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="E11" s="56" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G11" s="141">
         <v>2</v>
@@ -8182,29 +8173,29 @@
         <v>1</v>
       </c>
       <c r="I11" s="138" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="137" t="s">
         <v>39</v>
-      </c>
-      <c r="J11" s="137" t="s">
-        <v>40</v>
       </c>
       <c r="K11" s="35"/>
       <c r="L11" s="53" t="s">
-        <v>262</v>
+        <v>216</v>
       </c>
       <c r="M11" s="175" t="s">
-        <v>263</v>
+        <v>217</v>
       </c>
       <c r="N11" s="175" t="s">
-        <v>243</v>
+        <v>208</v>
       </c>
       <c r="O11" s="52" t="s">
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="P11" s="52" t="s">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="Q11" s="52" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="R11" s="59"/>
       <c r="JC11" s="32"/>
@@ -8220,19 +8211,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="53" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>226</v>
+        <v>284</v>
       </c>
       <c r="D12" s="73" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="G12" s="141">
         <v>3</v>
@@ -8241,34 +8232,34 @@
         <v>1</v>
       </c>
       <c r="I12" s="139" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J12" s="137" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="K12" s="35"/>
       <c r="L12" s="53" t="s">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="M12" s="175" t="s">
-        <v>266</v>
+        <v>218</v>
       </c>
       <c r="N12" s="175" t="s">
-        <v>267</v>
+        <v>286</v>
       </c>
       <c r="O12" s="52" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
       <c r="P12" s="52" t="s">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="Q12" s="52" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="R12" s="59"/>
       <c r="JC12" s="142"/>
       <c r="JD12" s="143" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="JE12" s="129"/>
       <c r="JF12" s="129"/>
@@ -8281,19 +8272,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>227</v>
+        <v>287</v>
       </c>
       <c r="C13" s="91" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="D13" s="73" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G13" s="141">
         <v>1</v>
@@ -8302,36 +8293,36 @@
         <v>3</v>
       </c>
       <c r="I13" s="139" t="s">
+        <v>37</v>
+      </c>
+      <c r="J13" s="137" t="s">
         <v>38</v>
-      </c>
-      <c r="J13" s="137" t="s">
-        <v>39</v>
       </c>
       <c r="K13" s="35"/>
       <c r="L13" s="53" t="s">
-        <v>269</v>
+        <v>288</v>
       </c>
       <c r="M13" s="175" t="s">
-        <v>270</v>
+        <v>289</v>
       </c>
       <c r="N13" s="175" t="s">
-        <v>271</v>
+        <v>220</v>
       </c>
       <c r="O13" s="52" t="s">
-        <v>272</v>
+        <v>221</v>
       </c>
       <c r="P13" s="52" t="s">
-        <v>273</v>
+        <v>290</v>
       </c>
       <c r="Q13" s="52" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="R13" s="59"/>
       <c r="JC13" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="JD13" s="51" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="JE13" s="129"/>
       <c r="JF13" s="130"/>
@@ -8364,11 +8355,11 @@
         <v>1</v>
       </c>
       <c r="JD14" s="47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="JE14" s="129"/>
       <c r="JF14" s="130" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="JG14" s="130"/>
       <c r="JH14" s="128"/>
@@ -8399,11 +8390,11 @@
         <v>2</v>
       </c>
       <c r="JD15" s="48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="JE15" s="130"/>
       <c r="JF15" s="130" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="JG15" s="130"/>
       <c r="JH15" s="127"/>
@@ -8432,11 +8423,11 @@
         <v>3</v>
       </c>
       <c r="JD16" s="47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="JE16" s="130"/>
       <c r="JF16" s="131" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="JG16" s="129"/>
       <c r="JH16" s="127"/>
@@ -8465,11 +8456,11 @@
         <v>4</v>
       </c>
       <c r="JD17" s="47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="JE17" s="130"/>
       <c r="JF17" s="131" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="JG17" s="129"/>
       <c r="JH17" s="127"/>
@@ -8498,11 +8489,11 @@
         <v>5</v>
       </c>
       <c r="JD18" s="47" t="s">
-        <v>50</v>
+        <v>261</v>
       </c>
       <c r="JE18" s="129"/>
       <c r="JF18" s="131" t="s">
-        <v>146</v>
+        <v>262</v>
       </c>
       <c r="JG18" s="129"/>
       <c r="JH18" s="128"/>
@@ -8528,14 +8519,14 @@
       <c r="Q19" s="52"/>
       <c r="R19" s="59"/>
       <c r="JC19" s="50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="JD19" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="JE19" s="129"/>
       <c r="JF19" s="130" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="JG19" s="130"/>
       <c r="JH19" s="128"/>
@@ -8564,11 +8555,11 @@
         <v>1</v>
       </c>
       <c r="JD20" s="46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="JE20" s="129"/>
       <c r="JF20" s="130" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="JG20" s="130"/>
       <c r="JH20" s="128"/>
@@ -8598,7 +8589,7 @@
         <v>2</v>
       </c>
       <c r="JD21" s="49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="JE21" s="130"/>
       <c r="JF21" s="130"/>
@@ -8626,16 +8617,16 @@
       <c r="Q22" s="52"/>
       <c r="R22" s="59"/>
       <c r="AP22" s="37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AQ22" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="JC22" s="43">
         <v>3</v>
       </c>
       <c r="JD22" s="48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="JE22" s="130"/>
       <c r="JF22" s="130"/>
@@ -8657,16 +8648,16 @@
       <c r="K23" s="31"/>
       <c r="L23" s="33"/>
       <c r="AP23" s="35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AQ23" s="35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="JC23" s="43">
         <v>4</v>
       </c>
       <c r="JD23" s="47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="JE23" s="130"/>
       <c r="JF23" s="129"/>
@@ -8691,7 +8682,7 @@
         <v>5</v>
       </c>
       <c r="JD24" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="JE24" s="34"/>
       <c r="JF24" s="32"/>
@@ -8705,10 +8696,10 @@
       <c r="K25" s="31"/>
       <c r="L25" s="33"/>
       <c r="JC25" s="72" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="JD25" s="45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="JE25" s="34"/>
       <c r="JF25" s="32"/>
@@ -8725,7 +8716,7 @@
         <v>1</v>
       </c>
       <c r="JD26" s="43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="JE26" s="32"/>
       <c r="JF26" s="32"/>
@@ -8742,7 +8733,7 @@
         <v>2</v>
       </c>
       <c r="JD27" s="43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="JE27" s="32"/>
       <c r="JF27" s="32"/>
@@ -8759,7 +8750,7 @@
         <v>3</v>
       </c>
       <c r="JD28" s="43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="JE28" s="32"/>
       <c r="JF28" s="32"/>
@@ -8776,7 +8767,7 @@
         <v>4</v>
       </c>
       <c r="JD29" s="43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="JE29" s="32"/>
       <c r="JF29" s="32"/>
@@ -8791,16 +8782,16 @@
       <c r="L30" s="33"/>
       <c r="JC30" s="44"/>
       <c r="JD30" s="44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="JE30" s="121" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="JF30" s="121" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="JG30" s="121" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="JH30" s="32"/>
       <c r="JI30" s="32"/>
@@ -8812,16 +8803,16 @@
       <c r="L31" s="33"/>
       <c r="JC31" s="108"/>
       <c r="JD31" s="111" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="JE31" s="123" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="JF31" s="124" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="JG31" s="124" t="s">
-        <v>138</v>
+        <v>263</v>
       </c>
       <c r="JH31" s="32"/>
       <c r="JI31" s="32"/>
@@ -8833,16 +8824,16 @@
       <c r="L32" s="33"/>
       <c r="JC32" s="109"/>
       <c r="JD32" s="111" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="JE32" s="123" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="JF32" s="123" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="JG32" s="124" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="JH32" s="32"/>
       <c r="JI32" s="32"/>
@@ -8854,16 +8845,16 @@
       <c r="L33" s="33"/>
       <c r="JC33" s="110"/>
       <c r="JD33" s="111" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="JE33" s="123" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="JF33" s="124" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="JG33" s="124" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="JH33" s="32"/>
       <c r="JI33" s="32"/>
@@ -8874,10 +8865,10 @@
       <c r="K34" s="33"/>
       <c r="L34" s="41"/>
       <c r="JC34" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="JD34" s="45" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="JE34" s="32"/>
       <c r="JF34" s="32"/>
@@ -8894,7 +8885,7 @@
         <v>1</v>
       </c>
       <c r="JD35" s="43" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="JE35" s="32"/>
       <c r="JF35" s="32"/>
@@ -8911,7 +8902,7 @@
         <v>2</v>
       </c>
       <c r="JD36" s="43" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="JE36" s="32"/>
       <c r="JF36" s="32"/>
@@ -8928,7 +8919,7 @@
         <v>3</v>
       </c>
       <c r="JD37" s="43" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="JE37" s="32"/>
       <c r="JF37" s="32"/>
@@ -8945,7 +8936,7 @@
         <v>4</v>
       </c>
       <c r="JD38" s="43" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="JE38" s="32"/>
       <c r="JF38" s="32"/>
@@ -9151,10 +9142,10 @@
     <row r="64" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A64" s="32"/>
       <c r="B64" s="122" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C64" s="122" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D64" s="32"/>
       <c r="E64" s="32"/>
@@ -9171,10 +9162,10 @@
     <row r="65" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A65" s="32"/>
       <c r="B65" s="122" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C65" s="122" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D65" s="32"/>
       <c r="E65" s="32"/>
@@ -9191,10 +9182,10 @@
     <row r="66" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A66" s="32"/>
       <c r="B66" s="122" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="C66" s="122" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D66" s="32"/>
       <c r="E66" s="32"/>
@@ -10134,8 +10125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10149,20 +10140,20 @@
     <row r="1" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="92" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="157" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B3" s="157" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="192" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B4" s="193"/>
       <c r="D4" s="93"/>
@@ -10173,37 +10164,37 @@
     </row>
     <row r="5" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="95" t="s">
-        <v>149</v>
+        <v>291</v>
       </c>
       <c r="B5" s="94" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="D5" s="93"/>
       <c r="E5" s="100"/>
       <c r="F5" s="100"/>
       <c r="G5" s="100" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H5" s="100"/>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="97" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="B6" s="94" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="D6" s="93"/>
       <c r="E6" s="100"/>
       <c r="F6" s="100"/>
       <c r="G6" s="100" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H6" s="100"/>
     </row>
     <row r="7" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="194" t="s">
-        <v>152</v>
+        <v>246</v>
       </c>
       <c r="B7" s="195"/>
       <c r="E7" s="100"/>
@@ -10213,23 +10204,23 @@
     </row>
     <row r="8" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="95" t="s">
-        <v>154</v>
+        <v>292</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="E8" s="100" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F8" s="100" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G8" s="100"/>
       <c r="H8" s="100"/>
     </row>
     <row r="9" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="190" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B9" s="191"/>
       <c r="C9" s="100"/>
@@ -10241,10 +10232,10 @@
     </row>
     <row r="10" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="97" t="s">
-        <v>155</v>
+        <v>293</v>
       </c>
       <c r="B10" s="94" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="C10" s="100"/>
       <c r="D10" s="100"/>
@@ -10255,7 +10246,7 @@
     </row>
     <row r="11" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="190" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B11" s="191"/>
       <c r="C11" s="100"/>
@@ -10267,10 +10258,10 @@
     </row>
     <row r="12" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="97" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="B12" s="94" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="C12" s="100"/>
       <c r="D12" s="100"/>
@@ -10281,10 +10272,10 @@
     </row>
     <row r="13" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="99" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="B13" s="94" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
@@ -10295,17 +10286,17 @@
     </row>
     <row r="14" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="99" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="B14" s="94" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="C14" s="100"/>
       <c r="D14" s="100" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E14" s="100" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F14" s="100"/>
       <c r="G14" s="100"/>
@@ -10313,7 +10304,7 @@
     </row>
     <row r="15" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="190" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="B15" s="191"/>
       <c r="C15" s="100"/>
@@ -10325,10 +10316,10 @@
     </row>
     <row r="16" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="97" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="B16" s="94" t="s">
-        <v>252</v>
+        <v>212</v>
       </c>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
@@ -10392,10 +10383,10 @@
       <c r="B22" s="98"/>
       <c r="C22" s="100"/>
       <c r="D22" s="100" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E22" s="100" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F22" s="100"/>
       <c r="G22" s="100"/>
@@ -10443,10 +10434,10 @@
       <c r="B27" s="98"/>
       <c r="C27" s="100"/>
       <c r="D27" s="100" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E27" s="100" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F27" s="100"/>
       <c r="G27" s="100"/>
@@ -10483,10 +10474,10 @@
       <c r="B31" s="94"/>
       <c r="C31" s="100"/>
       <c r="D31" s="100" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E31" s="100" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F31" s="100"/>
       <c r="G31" s="100"/>
@@ -10514,10 +10505,10 @@
       <c r="B34" s="94"/>
       <c r="C34" s="100"/>
       <c r="D34" s="100" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E34" s="100" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F34" s="100"/>
       <c r="G34" s="100"/>
@@ -10596,8 +10587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10614,92 +10605,92 @@
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="157" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B3" s="158" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C3" s="113"/>
     </row>
     <row r="4" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="125" t="s">
-        <v>287</v>
+        <v>230</v>
       </c>
       <c r="B4" s="114" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="C4" s="113"/>
       <c r="D4" s="100"/>
       <c r="E4" s="100"/>
       <c r="F4" s="100"/>
       <c r="G4" s="100" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H4" s="100"/>
     </row>
     <row r="5" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="126" t="s">
-        <v>289</v>
+        <v>231</v>
       </c>
       <c r="B5" s="114" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C5" s="113"/>
       <c r="D5" s="100"/>
       <c r="E5" s="100"/>
       <c r="F5" s="100"/>
       <c r="G5" s="100" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H5" s="100"/>
     </row>
     <row r="6" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="126" t="s">
-        <v>291</v>
+        <v>232</v>
       </c>
       <c r="B6" s="114" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="C6" s="113"/>
       <c r="D6" s="100"/>
       <c r="E6" s="100"/>
       <c r="F6" s="100"/>
       <c r="G6" s="100" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="H6" s="100" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="157" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B7" s="157" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C7" s="159" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A8" s="125" t="s">
-        <v>293</v>
+        <v>233</v>
       </c>
       <c r="B8" s="101" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C8" s="94" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E8" s="100" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F8" s="100" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G8" s="100" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H8" s="100"/>
       <c r="I8" s="100"/>
@@ -10707,13 +10698,13 @@
     </row>
     <row r="9" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="126" t="s">
-        <v>294</v>
+        <v>234</v>
       </c>
       <c r="B9" s="102" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C9" s="94" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
@@ -10724,13 +10715,13 @@
     </row>
     <row r="10" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="176" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="B10" s="103" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C10" s="94" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E10" s="100"/>
       <c r="F10" s="100"/>
@@ -10739,13 +10730,13 @@
     </row>
     <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="126" t="s">
-        <v>298</v>
+        <v>235</v>
       </c>
       <c r="B11" s="102" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C11" s="94" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E11" s="100"/>
       <c r="F11" s="100"/>
@@ -10754,13 +10745,13 @@
     </row>
     <row r="12" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="126" t="s">
-        <v>300</v>
+        <v>236</v>
       </c>
       <c r="B12" s="102" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C12" s="94" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D12" s="100"/>
       <c r="E12" s="100"/>
@@ -10770,13 +10761,13 @@
     </row>
     <row r="13" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="126" t="s">
-        <v>302</v>
+        <v>237</v>
       </c>
       <c r="B13" s="104" t="s">
-        <v>303</v>
+        <v>238</v>
       </c>
       <c r="C13" s="94" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D13" s="100"/>
       <c r="E13" s="100"/>
@@ -10786,13 +10777,13 @@
     </row>
     <row r="14" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="126" t="s">
-        <v>304</v>
+        <v>239</v>
       </c>
       <c r="B14" s="104" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C14" s="94" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
@@ -10802,13 +10793,13 @@
     </row>
     <row r="15" spans="1:10" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="126" t="s">
-        <v>306</v>
+        <v>240</v>
       </c>
       <c r="B15" s="101" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C15" s="94" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D15" s="100"/>
       <c r="E15" s="100"/>
@@ -10818,13 +10809,13 @@
     </row>
     <row r="16" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="126" t="s">
-        <v>308</v>
+        <v>241</v>
       </c>
       <c r="B16" s="102" t="s">
-        <v>309</v>
+        <v>242</v>
       </c>
       <c r="C16" s="94" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D16" s="100"/>
       <c r="E16" s="100"/>
@@ -10984,7 +10975,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11762,7 +11753,7 @@
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -11773,36 +11764,36 @@
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G3" s="116"/>
       <c r="H3" s="116" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I3" s="116" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="67" t="s">
-        <v>280</v>
+        <v>226</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="116"/>
       <c r="H4" s="116" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I4" s="116" t="s">
         <v>9</v>
@@ -11811,13 +11802,13 @@
     <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="67" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G5" s="116"/>
       <c r="H5" s="116"/>
@@ -11825,109 +11816,109 @@
     </row>
     <row r="6" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="62" t="s">
-        <v>281</v>
+        <v>227</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G6" s="117"/>
       <c r="H6" s="117"/>
       <c r="I6" s="116" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" s="62" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G7" s="117"/>
       <c r="H7" s="117"/>
       <c r="I7" s="116" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
-        <v>174</v>
+        <v>247</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G8" s="117"/>
       <c r="H8" s="117"/>
       <c r="I8" s="118" t="s">
-        <v>119</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="62" t="s">
-        <v>282</v>
+        <v>305</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G9" s="117"/>
       <c r="H9" s="117"/>
       <c r="I9" s="118" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B10" s="62" t="s">
-        <v>177</v>
+        <v>160</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G10" s="117"/>
       <c r="H10" s="117"/>
       <c r="I10" s="118" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B11" s="62" t="s">
-        <v>178</v>
+        <v>249</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G11" s="117"/>
       <c r="H11" s="117"/>
       <c r="I11" s="118" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B12" s="62" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G12" s="117"/>
       <c r="H12" s="117"/>
@@ -11935,13 +11926,13 @@
     </row>
     <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="G13" s="116"/>
       <c r="H13" s="116"/>
@@ -11986,8 +11977,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:D5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12765,7 +12756,7 @@
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -12776,28 +12767,28 @@
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="197" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C3" s="197"/>
       <c r="D3" s="197"/>
       <c r="G3" s="116"/>
       <c r="H3" s="116" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I3" s="116" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="196" t="s">
-        <v>285</v>
+        <v>307</v>
       </c>
       <c r="C4" s="196"/>
       <c r="D4" s="196"/>
       <c r="G4" s="116"/>
       <c r="H4" s="116" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I4" s="116" t="s">
         <v>9</v>
@@ -12805,19 +12796,19 @@
     </row>
     <row r="5" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="196" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="C5" s="196"/>
       <c r="D5" s="196"/>
       <c r="G5" s="117"/>
       <c r="H5" s="117"/>
       <c r="I5" s="116" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="196" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C6" s="196"/>
       <c r="D6" s="196"/>
@@ -12827,7 +12818,7 @@
     </row>
     <row r="7" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="196" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C7" s="196"/>
       <c r="D7" s="196"/>
@@ -12837,7 +12828,7 @@
     </row>
     <row r="8" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="196" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C8" s="196"/>
       <c r="D8" s="196"/>
@@ -12847,7 +12838,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="196" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C9" s="196"/>
       <c r="D9" s="196"/>
@@ -12868,7 +12859,7 @@
     <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="148"/>
       <c r="B12" s="149" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C12" s="148"/>
       <c r="D12" s="148"/>
@@ -12879,28 +12870,28 @@
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="197" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C13" s="197"/>
       <c r="D13" s="197"/>
       <c r="G13" s="116"/>
       <c r="H13" s="116" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I13" s="116" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="196" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="C14" s="196"/>
       <c r="D14" s="196"/>
       <c r="G14" s="116"/>
       <c r="H14" s="116" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I14" s="116" t="s">
         <v>9</v>
@@ -12908,19 +12899,19 @@
     </row>
     <row r="15" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="196" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="C15" s="196"/>
       <c r="D15" s="196"/>
       <c r="G15" s="117"/>
       <c r="H15" s="117"/>
       <c r="I15" s="116" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="196" t="s">
-        <v>283</v>
+        <v>228</v>
       </c>
       <c r="C16" s="196"/>
       <c r="D16" s="196"/>
@@ -12930,7 +12921,7 @@
     </row>
     <row r="17" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="196" t="s">
-        <v>284</v>
+        <v>229</v>
       </c>
       <c r="C17" s="196"/>
       <c r="D17" s="196"/>
@@ -12940,7 +12931,7 @@
     </row>
     <row r="18" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="196" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C18" s="196"/>
       <c r="D18" s="196"/>
@@ -12950,7 +12941,7 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="196" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C19" s="196"/>
       <c r="D19" s="196"/>
@@ -12960,6 +12951,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B3:D3"/>
@@ -12967,13 +12965,6 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="IS65533:IS65542 SO65533:SO65542 ACK65533:ACK65542 AMG65533:AMG65542 AWC65533:AWC65542 BFY65533:BFY65542 BPU65533:BPU65542 BZQ65533:BZQ65542 CJM65533:CJM65542 CTI65533:CTI65542 DDE65533:DDE65542 DNA65533:DNA65542 DWW65533:DWW65542 EGS65533:EGS65542 EQO65533:EQO65542 FAK65533:FAK65542 FKG65533:FKG65542 FUC65533:FUC65542 GDY65533:GDY65542 GNU65533:GNU65542 GXQ65533:GXQ65542 HHM65533:HHM65542 HRI65533:HRI65542 IBE65533:IBE65542 ILA65533:ILA65542 IUW65533:IUW65542 JES65533:JES65542 JOO65533:JOO65542 JYK65533:JYK65542 KIG65533:KIG65542 KSC65533:KSC65542 LBY65533:LBY65542 LLU65533:LLU65542 LVQ65533:LVQ65542 MFM65533:MFM65542 MPI65533:MPI65542 MZE65533:MZE65542 NJA65533:NJA65542 NSW65533:NSW65542 OCS65533:OCS65542 OMO65533:OMO65542 OWK65533:OWK65542 PGG65533:PGG65542 PQC65533:PQC65542 PZY65533:PZY65542 QJU65533:QJU65542 QTQ65533:QTQ65542 RDM65533:RDM65542 RNI65533:RNI65542 RXE65533:RXE65542 SHA65533:SHA65542 SQW65533:SQW65542 TAS65533:TAS65542 TKO65533:TKO65542 TUK65533:TUK65542 UEG65533:UEG65542 UOC65533:UOC65542 UXY65533:UXY65542 VHU65533:VHU65542 VRQ65533:VRQ65542 WBM65533:WBM65542 WLI65533:WLI65542 WVE65533:WVE65542 IS131069:IS131078 SO131069:SO131078 ACK131069:ACK131078 AMG131069:AMG131078 AWC131069:AWC131078 BFY131069:BFY131078 BPU131069:BPU131078 BZQ131069:BZQ131078 CJM131069:CJM131078 CTI131069:CTI131078 DDE131069:DDE131078 DNA131069:DNA131078 DWW131069:DWW131078 EGS131069:EGS131078 EQO131069:EQO131078 FAK131069:FAK131078 FKG131069:FKG131078 FUC131069:FUC131078 GDY131069:GDY131078 GNU131069:GNU131078 GXQ131069:GXQ131078 HHM131069:HHM131078 HRI131069:HRI131078 IBE131069:IBE131078 ILA131069:ILA131078 IUW131069:IUW131078 JES131069:JES131078 JOO131069:JOO131078 JYK131069:JYK131078 KIG131069:KIG131078 KSC131069:KSC131078 LBY131069:LBY131078 LLU131069:LLU131078 LVQ131069:LVQ131078 MFM131069:MFM131078 MPI131069:MPI131078 MZE131069:MZE131078 NJA131069:NJA131078 NSW131069:NSW131078 OCS131069:OCS131078 OMO131069:OMO131078 OWK131069:OWK131078 PGG131069:PGG131078 PQC131069:PQC131078 PZY131069:PZY131078 QJU131069:QJU131078 QTQ131069:QTQ131078 RDM131069:RDM131078 RNI131069:RNI131078 RXE131069:RXE131078 SHA131069:SHA131078 SQW131069:SQW131078 TAS131069:TAS131078 TKO131069:TKO131078 TUK131069:TUK131078 UEG131069:UEG131078 UOC131069:UOC131078 UXY131069:UXY131078 VHU131069:VHU131078 VRQ131069:VRQ131078 WBM131069:WBM131078 WLI131069:WLI131078 WVE131069:WVE131078 IS196605:IS196614 SO196605:SO196614 ACK196605:ACK196614 AMG196605:AMG196614 AWC196605:AWC196614 BFY196605:BFY196614 BPU196605:BPU196614 BZQ196605:BZQ196614 CJM196605:CJM196614 CTI196605:CTI196614 DDE196605:DDE196614 DNA196605:DNA196614 DWW196605:DWW196614 EGS196605:EGS196614 EQO196605:EQO196614 FAK196605:FAK196614 FKG196605:FKG196614 FUC196605:FUC196614 GDY196605:GDY196614 GNU196605:GNU196614 GXQ196605:GXQ196614 HHM196605:HHM196614 HRI196605:HRI196614 IBE196605:IBE196614 ILA196605:ILA196614 IUW196605:IUW196614 JES196605:JES196614 JOO196605:JOO196614 JYK196605:JYK196614 KIG196605:KIG196614 KSC196605:KSC196614 LBY196605:LBY196614 LLU196605:LLU196614 LVQ196605:LVQ196614 MFM196605:MFM196614 MPI196605:MPI196614 MZE196605:MZE196614 NJA196605:NJA196614 NSW196605:NSW196614 OCS196605:OCS196614 OMO196605:OMO196614 OWK196605:OWK196614 PGG196605:PGG196614 PQC196605:PQC196614 PZY196605:PZY196614 QJU196605:QJU196614 QTQ196605:QTQ196614 RDM196605:RDM196614 RNI196605:RNI196614 RXE196605:RXE196614 SHA196605:SHA196614 SQW196605:SQW196614 TAS196605:TAS196614 TKO196605:TKO196614 TUK196605:TUK196614 UEG196605:UEG196614 UOC196605:UOC196614 UXY196605:UXY196614 VHU196605:VHU196614 VRQ196605:VRQ196614 WBM196605:WBM196614 WLI196605:WLI196614 WVE196605:WVE196614 IS262141:IS262150 SO262141:SO262150 ACK262141:ACK262150 AMG262141:AMG262150 AWC262141:AWC262150 BFY262141:BFY262150 BPU262141:BPU262150 BZQ262141:BZQ262150 CJM262141:CJM262150 CTI262141:CTI262150 DDE262141:DDE262150 DNA262141:DNA262150 DWW262141:DWW262150 EGS262141:EGS262150 EQO262141:EQO262150 FAK262141:FAK262150 FKG262141:FKG262150 FUC262141:FUC262150 GDY262141:GDY262150 GNU262141:GNU262150 GXQ262141:GXQ262150 HHM262141:HHM262150 HRI262141:HRI262150 IBE262141:IBE262150 ILA262141:ILA262150 IUW262141:IUW262150 JES262141:JES262150 JOO262141:JOO262150 JYK262141:JYK262150 KIG262141:KIG262150 KSC262141:KSC262150 LBY262141:LBY262150 LLU262141:LLU262150 LVQ262141:LVQ262150 MFM262141:MFM262150 MPI262141:MPI262150 MZE262141:MZE262150 NJA262141:NJA262150 NSW262141:NSW262150 OCS262141:OCS262150 OMO262141:OMO262150 OWK262141:OWK262150 PGG262141:PGG262150 PQC262141:PQC262150 PZY262141:PZY262150 QJU262141:QJU262150 QTQ262141:QTQ262150 RDM262141:RDM262150 RNI262141:RNI262150 RXE262141:RXE262150 SHA262141:SHA262150 SQW262141:SQW262150 TAS262141:TAS262150 TKO262141:TKO262150 TUK262141:TUK262150 UEG262141:UEG262150 UOC262141:UOC262150 UXY262141:UXY262150 VHU262141:VHU262150 VRQ262141:VRQ262150 WBM262141:WBM262150 WLI262141:WLI262150 WVE262141:WVE262150 IS327677:IS327686 SO327677:SO327686 ACK327677:ACK327686 AMG327677:AMG327686 AWC327677:AWC327686 BFY327677:BFY327686 BPU327677:BPU327686 BZQ327677:BZQ327686 CJM327677:CJM327686 CTI327677:CTI327686 DDE327677:DDE327686 DNA327677:DNA327686 DWW327677:DWW327686 EGS327677:EGS327686 EQO327677:EQO327686 FAK327677:FAK327686 FKG327677:FKG327686 FUC327677:FUC327686 GDY327677:GDY327686 GNU327677:GNU327686 GXQ327677:GXQ327686 HHM327677:HHM327686 HRI327677:HRI327686 IBE327677:IBE327686 ILA327677:ILA327686 IUW327677:IUW327686 JES327677:JES327686 JOO327677:JOO327686 JYK327677:JYK327686 KIG327677:KIG327686 KSC327677:KSC327686 LBY327677:LBY327686 LLU327677:LLU327686 LVQ327677:LVQ327686 MFM327677:MFM327686 MPI327677:MPI327686 MZE327677:MZE327686 NJA327677:NJA327686 NSW327677:NSW327686 OCS327677:OCS327686 OMO327677:OMO327686 OWK327677:OWK327686 PGG327677:PGG327686 PQC327677:PQC327686 PZY327677:PZY327686 QJU327677:QJU327686 QTQ327677:QTQ327686 RDM327677:RDM327686 RNI327677:RNI327686 RXE327677:RXE327686 SHA327677:SHA327686 SQW327677:SQW327686 TAS327677:TAS327686 TKO327677:TKO327686 TUK327677:TUK327686 UEG327677:UEG327686 UOC327677:UOC327686 UXY327677:UXY327686 VHU327677:VHU327686 VRQ327677:VRQ327686 WBM327677:WBM327686 WLI327677:WLI327686 WVE327677:WVE327686 IS393213:IS393222 SO393213:SO393222 ACK393213:ACK393222 AMG393213:AMG393222 AWC393213:AWC393222 BFY393213:BFY393222 BPU393213:BPU393222 BZQ393213:BZQ393222 CJM393213:CJM393222 CTI393213:CTI393222 DDE393213:DDE393222 DNA393213:DNA393222 DWW393213:DWW393222 EGS393213:EGS393222 EQO393213:EQO393222 FAK393213:FAK393222 FKG393213:FKG393222 FUC393213:FUC393222 GDY393213:GDY393222 GNU393213:GNU393222 GXQ393213:GXQ393222 HHM393213:HHM393222 HRI393213:HRI393222 IBE393213:IBE393222 ILA393213:ILA393222 IUW393213:IUW393222 JES393213:JES393222 JOO393213:JOO393222 JYK393213:JYK393222 KIG393213:KIG393222 KSC393213:KSC393222 LBY393213:LBY393222 LLU393213:LLU393222 LVQ393213:LVQ393222 MFM393213:MFM393222 MPI393213:MPI393222 MZE393213:MZE393222 NJA393213:NJA393222 NSW393213:NSW393222 OCS393213:OCS393222 OMO393213:OMO393222 OWK393213:OWK393222 PGG393213:PGG393222 PQC393213:PQC393222 PZY393213:PZY393222 QJU393213:QJU393222 QTQ393213:QTQ393222 RDM393213:RDM393222 RNI393213:RNI393222 RXE393213:RXE393222 SHA393213:SHA393222 SQW393213:SQW393222 TAS393213:TAS393222 TKO393213:TKO393222 TUK393213:TUK393222 UEG393213:UEG393222 UOC393213:UOC393222 UXY393213:UXY393222 VHU393213:VHU393222 VRQ393213:VRQ393222 WBM393213:WBM393222 WLI393213:WLI393222 WVE393213:WVE393222 IS458749:IS458758 SO458749:SO458758 ACK458749:ACK458758 AMG458749:AMG458758 AWC458749:AWC458758 BFY458749:BFY458758 BPU458749:BPU458758 BZQ458749:BZQ458758 CJM458749:CJM458758 CTI458749:CTI458758 DDE458749:DDE458758 DNA458749:DNA458758 DWW458749:DWW458758 EGS458749:EGS458758 EQO458749:EQO458758 FAK458749:FAK458758 FKG458749:FKG458758 FUC458749:FUC458758 GDY458749:GDY458758 GNU458749:GNU458758 GXQ458749:GXQ458758 HHM458749:HHM458758 HRI458749:HRI458758 IBE458749:IBE458758 ILA458749:ILA458758 IUW458749:IUW458758 JES458749:JES458758 JOO458749:JOO458758 JYK458749:JYK458758 KIG458749:KIG458758 KSC458749:KSC458758 LBY458749:LBY458758 LLU458749:LLU458758 LVQ458749:LVQ458758 MFM458749:MFM458758 MPI458749:MPI458758 MZE458749:MZE458758 NJA458749:NJA458758 NSW458749:NSW458758 OCS458749:OCS458758 OMO458749:OMO458758 OWK458749:OWK458758 PGG458749:PGG458758 PQC458749:PQC458758 PZY458749:PZY458758 QJU458749:QJU458758 QTQ458749:QTQ458758 RDM458749:RDM458758 RNI458749:RNI458758 RXE458749:RXE458758 SHA458749:SHA458758 SQW458749:SQW458758 TAS458749:TAS458758 TKO458749:TKO458758 TUK458749:TUK458758 UEG458749:UEG458758 UOC458749:UOC458758 UXY458749:UXY458758 VHU458749:VHU458758 VRQ458749:VRQ458758 WBM458749:WBM458758 WLI458749:WLI458758 WVE458749:WVE458758 IS524285:IS524294 SO524285:SO524294 ACK524285:ACK524294 AMG524285:AMG524294 AWC524285:AWC524294 BFY524285:BFY524294 BPU524285:BPU524294 BZQ524285:BZQ524294 CJM524285:CJM524294 CTI524285:CTI524294 DDE524285:DDE524294 DNA524285:DNA524294 DWW524285:DWW524294 EGS524285:EGS524294 EQO524285:EQO524294 FAK524285:FAK524294 FKG524285:FKG524294 FUC524285:FUC524294 GDY524285:GDY524294 GNU524285:GNU524294 GXQ524285:GXQ524294 HHM524285:HHM524294 HRI524285:HRI524294 IBE524285:IBE524294 ILA524285:ILA524294 IUW524285:IUW524294 JES524285:JES524294 JOO524285:JOO524294 JYK524285:JYK524294 KIG524285:KIG524294 KSC524285:KSC524294 LBY524285:LBY524294 LLU524285:LLU524294 LVQ524285:LVQ524294 MFM524285:MFM524294 MPI524285:MPI524294 MZE524285:MZE524294 NJA524285:NJA524294 NSW524285:NSW524294 OCS524285:OCS524294 OMO524285:OMO524294 OWK524285:OWK524294 PGG524285:PGG524294 PQC524285:PQC524294 PZY524285:PZY524294 QJU524285:QJU524294 QTQ524285:QTQ524294 RDM524285:RDM524294 RNI524285:RNI524294 RXE524285:RXE524294 SHA524285:SHA524294 SQW524285:SQW524294 TAS524285:TAS524294 TKO524285:TKO524294 TUK524285:TUK524294 UEG524285:UEG524294 UOC524285:UOC524294 UXY524285:UXY524294 VHU524285:VHU524294 VRQ524285:VRQ524294 WBM524285:WBM524294 WLI524285:WLI524294 WVE524285:WVE524294 IS589821:IS589830 SO589821:SO589830 ACK589821:ACK589830 AMG589821:AMG589830 AWC589821:AWC589830 BFY589821:BFY589830 BPU589821:BPU589830 BZQ589821:BZQ589830 CJM589821:CJM589830 CTI589821:CTI589830 DDE589821:DDE589830 DNA589821:DNA589830 DWW589821:DWW589830 EGS589821:EGS589830 EQO589821:EQO589830 FAK589821:FAK589830 FKG589821:FKG589830 FUC589821:FUC589830 GDY589821:GDY589830 GNU589821:GNU589830 GXQ589821:GXQ589830 HHM589821:HHM589830 HRI589821:HRI589830 IBE589821:IBE589830 ILA589821:ILA589830 IUW589821:IUW589830 JES589821:JES589830 JOO589821:JOO589830 JYK589821:JYK589830 KIG589821:KIG589830 KSC589821:KSC589830 LBY589821:LBY589830 LLU589821:LLU589830 LVQ589821:LVQ589830 MFM589821:MFM589830 MPI589821:MPI589830 MZE589821:MZE589830 NJA589821:NJA589830 NSW589821:NSW589830 OCS589821:OCS589830 OMO589821:OMO589830 OWK589821:OWK589830 PGG589821:PGG589830 PQC589821:PQC589830 PZY589821:PZY589830 QJU589821:QJU589830 QTQ589821:QTQ589830 RDM589821:RDM589830 RNI589821:RNI589830 RXE589821:RXE589830 SHA589821:SHA589830 SQW589821:SQW589830 TAS589821:TAS589830 TKO589821:TKO589830 TUK589821:TUK589830 UEG589821:UEG589830 UOC589821:UOC589830 UXY589821:UXY589830 VHU589821:VHU589830 VRQ589821:VRQ589830 WBM589821:WBM589830 WLI589821:WLI589830 WVE589821:WVE589830 IS655357:IS655366 SO655357:SO655366 ACK655357:ACK655366 AMG655357:AMG655366 AWC655357:AWC655366 BFY655357:BFY655366 BPU655357:BPU655366 BZQ655357:BZQ655366 CJM655357:CJM655366 CTI655357:CTI655366 DDE655357:DDE655366 DNA655357:DNA655366 DWW655357:DWW655366 EGS655357:EGS655366 EQO655357:EQO655366 FAK655357:FAK655366 FKG655357:FKG655366 FUC655357:FUC655366 GDY655357:GDY655366 GNU655357:GNU655366 GXQ655357:GXQ655366 HHM655357:HHM655366 HRI655357:HRI655366 IBE655357:IBE655366 ILA655357:ILA655366 IUW655357:IUW655366 JES655357:JES655366 JOO655357:JOO655366 JYK655357:JYK655366 KIG655357:KIG655366 KSC655357:KSC655366 LBY655357:LBY655366 LLU655357:LLU655366 LVQ655357:LVQ655366 MFM655357:MFM655366 MPI655357:MPI655366 MZE655357:MZE655366 NJA655357:NJA655366 NSW655357:NSW655366 OCS655357:OCS655366 OMO655357:OMO655366 OWK655357:OWK655366 PGG655357:PGG655366 PQC655357:PQC655366 PZY655357:PZY655366 QJU655357:QJU655366 QTQ655357:QTQ655366 RDM655357:RDM655366 RNI655357:RNI655366 RXE655357:RXE655366 SHA655357:SHA655366 SQW655357:SQW655366 TAS655357:TAS655366 TKO655357:TKO655366 TUK655357:TUK655366 UEG655357:UEG655366 UOC655357:UOC655366 UXY655357:UXY655366 VHU655357:VHU655366 VRQ655357:VRQ655366 WBM655357:WBM655366 WLI655357:WLI655366 WVE655357:WVE655366 IS720893:IS720902 SO720893:SO720902 ACK720893:ACK720902 AMG720893:AMG720902 AWC720893:AWC720902 BFY720893:BFY720902 BPU720893:BPU720902 BZQ720893:BZQ720902 CJM720893:CJM720902 CTI720893:CTI720902 DDE720893:DDE720902 DNA720893:DNA720902 DWW720893:DWW720902 EGS720893:EGS720902 EQO720893:EQO720902 FAK720893:FAK720902 FKG720893:FKG720902 FUC720893:FUC720902 GDY720893:GDY720902 GNU720893:GNU720902 GXQ720893:GXQ720902 HHM720893:HHM720902 HRI720893:HRI720902 IBE720893:IBE720902 ILA720893:ILA720902 IUW720893:IUW720902 JES720893:JES720902 JOO720893:JOO720902 JYK720893:JYK720902 KIG720893:KIG720902 KSC720893:KSC720902 LBY720893:LBY720902 LLU720893:LLU720902 LVQ720893:LVQ720902 MFM720893:MFM720902 MPI720893:MPI720902 MZE720893:MZE720902 NJA720893:NJA720902 NSW720893:NSW720902 OCS720893:OCS720902 OMO720893:OMO720902 OWK720893:OWK720902 PGG720893:PGG720902 PQC720893:PQC720902 PZY720893:PZY720902 QJU720893:QJU720902 QTQ720893:QTQ720902 RDM720893:RDM720902 RNI720893:RNI720902 RXE720893:RXE720902 SHA720893:SHA720902 SQW720893:SQW720902 TAS720893:TAS720902 TKO720893:TKO720902 TUK720893:TUK720902 UEG720893:UEG720902 UOC720893:UOC720902 UXY720893:UXY720902 VHU720893:VHU720902 VRQ720893:VRQ720902 WBM720893:WBM720902 WLI720893:WLI720902 WVE720893:WVE720902 IS786429:IS786438 SO786429:SO786438 ACK786429:ACK786438 AMG786429:AMG786438 AWC786429:AWC786438 BFY786429:BFY786438 BPU786429:BPU786438 BZQ786429:BZQ786438 CJM786429:CJM786438 CTI786429:CTI786438 DDE786429:DDE786438 DNA786429:DNA786438 DWW786429:DWW786438 EGS786429:EGS786438 EQO786429:EQO786438 FAK786429:FAK786438 FKG786429:FKG786438 FUC786429:FUC786438 GDY786429:GDY786438 GNU786429:GNU786438 GXQ786429:GXQ786438 HHM786429:HHM786438 HRI786429:HRI786438 IBE786429:IBE786438 ILA786429:ILA786438 IUW786429:IUW786438 JES786429:JES786438 JOO786429:JOO786438 JYK786429:JYK786438 KIG786429:KIG786438 KSC786429:KSC786438 LBY786429:LBY786438 LLU786429:LLU786438 LVQ786429:LVQ786438 MFM786429:MFM786438 MPI786429:MPI786438 MZE786429:MZE786438 NJA786429:NJA786438 NSW786429:NSW786438 OCS786429:OCS786438 OMO786429:OMO786438 OWK786429:OWK786438 PGG786429:PGG786438 PQC786429:PQC786438 PZY786429:PZY786438 QJU786429:QJU786438 QTQ786429:QTQ786438 RDM786429:RDM786438 RNI786429:RNI786438 RXE786429:RXE786438 SHA786429:SHA786438 SQW786429:SQW786438 TAS786429:TAS786438 TKO786429:TKO786438 TUK786429:TUK786438 UEG786429:UEG786438 UOC786429:UOC786438 UXY786429:UXY786438 VHU786429:VHU786438 VRQ786429:VRQ786438 WBM786429:WBM786438 WLI786429:WLI786438 WVE786429:WVE786438 IS851965:IS851974 SO851965:SO851974 ACK851965:ACK851974 AMG851965:AMG851974 AWC851965:AWC851974 BFY851965:BFY851974 BPU851965:BPU851974 BZQ851965:BZQ851974 CJM851965:CJM851974 CTI851965:CTI851974 DDE851965:DDE851974 DNA851965:DNA851974 DWW851965:DWW851974 EGS851965:EGS851974 EQO851965:EQO851974 FAK851965:FAK851974 FKG851965:FKG851974 FUC851965:FUC851974 GDY851965:GDY851974 GNU851965:GNU851974 GXQ851965:GXQ851974 HHM851965:HHM851974 HRI851965:HRI851974 IBE851965:IBE851974 ILA851965:ILA851974 IUW851965:IUW851974 JES851965:JES851974 JOO851965:JOO851974 JYK851965:JYK851974 KIG851965:KIG851974 KSC851965:KSC851974 LBY851965:LBY851974 LLU851965:LLU851974 LVQ851965:LVQ851974 MFM851965:MFM851974 MPI851965:MPI851974 MZE851965:MZE851974 NJA851965:NJA851974 NSW851965:NSW851974 OCS851965:OCS851974 OMO851965:OMO851974 OWK851965:OWK851974 PGG851965:PGG851974 PQC851965:PQC851974 PZY851965:PZY851974 QJU851965:QJU851974 QTQ851965:QTQ851974 RDM851965:RDM851974 RNI851965:RNI851974 RXE851965:RXE851974 SHA851965:SHA851974 SQW851965:SQW851974 TAS851965:TAS851974 TKO851965:TKO851974 TUK851965:TUK851974 UEG851965:UEG851974 UOC851965:UOC851974 UXY851965:UXY851974 VHU851965:VHU851974 VRQ851965:VRQ851974 WBM851965:WBM851974 WLI851965:WLI851974 WVE851965:WVE851974 IS917501:IS917510 SO917501:SO917510 ACK917501:ACK917510 AMG917501:AMG917510 AWC917501:AWC917510 BFY917501:BFY917510 BPU917501:BPU917510 BZQ917501:BZQ917510 CJM917501:CJM917510 CTI917501:CTI917510 DDE917501:DDE917510 DNA917501:DNA917510 DWW917501:DWW917510 EGS917501:EGS917510 EQO917501:EQO917510 FAK917501:FAK917510 FKG917501:FKG917510 FUC917501:FUC917510 GDY917501:GDY917510 GNU917501:GNU917510 GXQ917501:GXQ917510 HHM917501:HHM917510 HRI917501:HRI917510 IBE917501:IBE917510 ILA917501:ILA917510 IUW917501:IUW917510 JES917501:JES917510 JOO917501:JOO917510 JYK917501:JYK917510 KIG917501:KIG917510 KSC917501:KSC917510 LBY917501:LBY917510 LLU917501:LLU917510 LVQ917501:LVQ917510 MFM917501:MFM917510 MPI917501:MPI917510 MZE917501:MZE917510 NJA917501:NJA917510 NSW917501:NSW917510 OCS917501:OCS917510 OMO917501:OMO917510 OWK917501:OWK917510 PGG917501:PGG917510 PQC917501:PQC917510 PZY917501:PZY917510 QJU917501:QJU917510 QTQ917501:QTQ917510 RDM917501:RDM917510 RNI917501:RNI917510 RXE917501:RXE917510 SHA917501:SHA917510 SQW917501:SQW917510 TAS917501:TAS917510 TKO917501:TKO917510 TUK917501:TUK917510 UEG917501:UEG917510 UOC917501:UOC917510 UXY917501:UXY917510 VHU917501:VHU917510 VRQ917501:VRQ917510 WBM917501:WBM917510 WLI917501:WLI917510 WVE917501:WVE917510 IS983037:IS983046 SO983037:SO983046 ACK983037:ACK983046 AMG983037:AMG983046 AWC983037:AWC983046 BFY983037:BFY983046 BPU983037:BPU983046 BZQ983037:BZQ983046 CJM983037:CJM983046 CTI983037:CTI983046 DDE983037:DDE983046 DNA983037:DNA983046 DWW983037:DWW983046 EGS983037:EGS983046 EQO983037:EQO983046 FAK983037:FAK983046 FKG983037:FKG983046 FUC983037:FUC983046 GDY983037:GDY983046 GNU983037:GNU983046 GXQ983037:GXQ983046 HHM983037:HHM983046 HRI983037:HRI983046 IBE983037:IBE983046 ILA983037:ILA983046 IUW983037:IUW983046 JES983037:JES983046 JOO983037:JOO983046 JYK983037:JYK983046 KIG983037:KIG983046 KSC983037:KSC983046 LBY983037:LBY983046 LLU983037:LLU983046 LVQ983037:LVQ983046 MFM983037:MFM983046 MPI983037:MPI983046 MZE983037:MZE983046 NJA983037:NJA983046 NSW983037:NSW983046 OCS983037:OCS983046 OMO983037:OMO983046 OWK983037:OWK983046 PGG983037:PGG983046 PQC983037:PQC983046 PZY983037:PZY983046 QJU983037:QJU983046 QTQ983037:QTQ983046 RDM983037:RDM983046 RNI983037:RNI983046 RXE983037:RXE983046 SHA983037:SHA983046 SQW983037:SQW983046 TAS983037:TAS983046 TKO983037:TKO983046 TUK983037:TUK983046 UEG983037:UEG983046 UOC983037:UOC983046 UXY983037:UXY983046 VHU983037:VHU983046 VRQ983037:VRQ983046 WBM983037:WBM983046 WLI983037:WLI983046 WVE983037:WVE983046 SO5:SO8 ACK5:ACK8 AMG5:AMG8 AWC5:AWC8 BFY5:BFY8 BPU5:BPU8 BZQ5:BZQ8 CJM5:CJM8 CTI5:CTI8 DDE5:DDE8 DNA5:DNA8 DWW5:DWW8 EGS5:EGS8 EQO5:EQO8 FAK5:FAK8 FKG5:FKG8 FUC5:FUC8 GDY5:GDY8 GNU5:GNU8 GXQ5:GXQ8 HHM5:HHM8 HRI5:HRI8 IBE5:IBE8 ILA5:ILA8 IUW5:IUW8 JES5:JES8 JOO5:JOO8 JYK5:JYK8 KIG5:KIG8 KSC5:KSC8 LBY5:LBY8 LLU5:LLU8 LVQ5:LVQ8 MFM5:MFM8 MPI5:MPI8 MZE5:MZE8 NJA5:NJA8 NSW5:NSW8 OCS5:OCS8 OMO5:OMO8 OWK5:OWK8 PGG5:PGG8 PQC5:PQC8 PZY5:PZY8 QJU5:QJU8 QTQ5:QTQ8 RDM5:RDM8 RNI5:RNI8 RXE5:RXE8 SHA5:SHA8 SQW5:SQW8 TAS5:TAS8 TKO5:TKO8 TUK5:TUK8 UEG5:UEG8 UOC5:UOC8 UXY5:UXY8 VHU5:VHU8 VRQ5:VRQ8 WBM5:WBM8 WLI5:WLI8 WVE5:WVE8 IS5:IS8 SO15:SO18 ACK15:ACK18 AMG15:AMG18 AWC15:AWC18 BFY15:BFY18 BPU15:BPU18 BZQ15:BZQ18 CJM15:CJM18 CTI15:CTI18 DDE15:DDE18 DNA15:DNA18 DWW15:DWW18 EGS15:EGS18 EQO15:EQO18 FAK15:FAK18 FKG15:FKG18 FUC15:FUC18 GDY15:GDY18 GNU15:GNU18 GXQ15:GXQ18 HHM15:HHM18 HRI15:HRI18 IBE15:IBE18 ILA15:ILA18 IUW15:IUW18 JES15:JES18 JOO15:JOO18 JYK15:JYK18 KIG15:KIG18 KSC15:KSC18 LBY15:LBY18 LLU15:LLU18 LVQ15:LVQ18 MFM15:MFM18 MPI15:MPI18 MZE15:MZE18 NJA15:NJA18 NSW15:NSW18 OCS15:OCS18 OMO15:OMO18 OWK15:OWK18 PGG15:PGG18 PQC15:PQC18 PZY15:PZY18 QJU15:QJU18 QTQ15:QTQ18 RDM15:RDM18 RNI15:RNI18 RXE15:RXE18 SHA15:SHA18 SQW15:SQW18 TAS15:TAS18 TKO15:TKO18 TUK15:TUK18 UEG15:UEG18 UOC15:UOC18 UXY15:UXY18 VHU15:VHU18 VRQ15:VRQ18 WBM15:WBM18 WLI15:WLI18 WVE15:WVE18 IS15:IS18">

</xml_diff>

<commit_message>
Viaticos_q_Plan de proyectos actualizado
</commit_message>
<xml_diff>
--- a/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/2. Plantillas planeacion/Viaticos_q_Plan_Proyecto.xlsx
+++ b/Proyectos/Activos/Viaticos_q/2. Estimacion y planeacion/2. Plantillas planeacion/Viaticos_q_Plan_Proyecto.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="875" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="875" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Generales" sheetId="23" r:id="rId1"/>
@@ -538,7 +538,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="307">
   <si>
     <t>Nombre</t>
   </si>
@@ -753,9 +753,6 @@
   </si>
   <si>
     <t>Calendario del Proyecto</t>
-  </si>
-  <si>
-    <t>Definirlas en el calendario del proyecto Dotproject</t>
   </si>
   <si>
     <t>Analistas</t>
@@ -2475,7 +2472,7 @@
     </xf>
     <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="45" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2929,21 +2926,21 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="12" xfId="52" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="27" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="46" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2970,6 +2967,9 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="24" borderId="0" xfId="54" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="56">
@@ -3807,8 +3807,8 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -4098,7 +4098,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" s="80"/>
       <c r="E4" s="80"/>
@@ -4118,7 +4118,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D6" s="76"/>
       <c r="E6" s="76"/>
@@ -4148,13 +4148,13 @@
         <v>22</v>
       </c>
       <c r="C9" s="98" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E9" s="115" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F9" s="115" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="12.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4170,7 +4170,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -4194,76 +4194,76 @@
     </row>
     <row r="15" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B15" s="181" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B16" s="182"/>
       <c r="C16" s="67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B17" s="183" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C17" s="62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B18" s="182"/>
       <c r="C18" s="62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B19" s="183" t="s">
+        <v>245</v>
+      </c>
+      <c r="C19" s="62" t="s">
         <v>246</v>
-      </c>
-      <c r="C19" s="62" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B20" s="181"/>
       <c r="C20" s="62" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B21" s="181"/>
       <c r="C21" s="62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B22" s="181"/>
       <c r="C22" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B23" s="182"/>
       <c r="C23" s="62" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B24" s="183" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:3" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B25" s="182"/>
       <c r="C25" s="62" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -4279,20 +4279,20 @@
     </row>
     <row r="28" spans="1:3" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="179" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C28" s="180"/>
     </row>
     <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="147"/>
       <c r="B29" s="144" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C29" s="147"/>
     </row>
     <row r="30" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="179" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C30" s="179"/>
     </row>
@@ -4330,8 +4330,8 @@
   </sheetPr>
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -4790,7 +4790,7 @@
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -4801,7 +4801,7 @@
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="155"/>
       <c r="B3" s="156" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C3" s="155"/>
       <c r="D3" s="155"/>
@@ -4833,22 +4833,22 @@
     <row r="5" spans="1:7" ht="38.25" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
       <c r="B5" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E5" s="162" t="s">
+        <v>167</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="E5" s="162" t="s">
-        <v>168</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>167</v>
-      </c>
       <c r="G5" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4876,14 +4876,14 @@
       <c r="B8" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="187" t="s">
+      <c r="C8" s="185" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="187"/>
-      <c r="E8" s="188" t="s">
+      <c r="D8" s="185"/>
+      <c r="E8" s="186" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="188"/>
+      <c r="F8" s="186"/>
       <c r="G8" s="25"/>
     </row>
     <row r="9" spans="1:7" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -4900,26 +4900,26 @@
     <row r="10" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" s="185" t="str">
+        <v>179</v>
+      </c>
+      <c r="C10" s="184" t="str">
         <f>VLOOKUP(B10,$B$50:$D$66,2,0)</f>
         <v>33 1605 3573</v>
       </c>
-      <c r="D10" s="185"/>
-      <c r="E10" s="185" t="str">
+      <c r="D10" s="184"/>
+      <c r="E10" s="184" t="str">
         <f>VLOOKUP(B10,$B$50:$D$66,3,0)</f>
         <v>felipelozanopadilla@gmail.com</v>
       </c>
-      <c r="F10" s="185"/>
+      <c r="F10" s="184"/>
       <c r="G10" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="153"/>
       <c r="B11" s="154" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="154"/>
       <c r="D11" s="154"/>
@@ -4930,26 +4930,26 @@
     <row r="12" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C12" s="185" t="str">
+        <v>169</v>
+      </c>
+      <c r="C12" s="184" t="str">
         <f>VLOOKUP(B12,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D12" s="185"/>
-      <c r="E12" s="185" t="str">
+      <c r="D12" s="184"/>
+      <c r="E12" s="184" t="str">
         <f>VLOOKUP(B12,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F12" s="185"/>
+      <c r="F12" s="184"/>
       <c r="G12" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="153"/>
       <c r="B13" s="154" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="154"/>
       <c r="D13" s="154"/>
@@ -4960,43 +4960,43 @@
     <row r="14" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="185" t="str">
+        <v>164</v>
+      </c>
+      <c r="C14" s="184" t="str">
         <f>VLOOKUP(B14,$B$50:$D$66,2,0)</f>
         <v>33 1862 1719</v>
       </c>
-      <c r="D14" s="185"/>
-      <c r="E14" s="185" t="str">
+      <c r="D14" s="184"/>
+      <c r="E14" s="184" t="str">
         <f>VLOOKUP(B14,$B$50:$D$66,3,0)</f>
         <v>rpulido@qualtop.com</v>
       </c>
-      <c r="F14" s="185"/>
+      <c r="F14" s="184"/>
       <c r="G14" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" s="185" t="e">
+        <v>75</v>
+      </c>
+      <c r="C15" s="184" t="e">
         <f>VLOOKUP(B15,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D15" s="185"/>
-      <c r="E15" s="185" t="e">
+      <c r="D15" s="184"/>
+      <c r="E15" s="184" t="e">
         <f>VLOOKUP(B15,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F15" s="185"/>
+      <c r="F15" s="184"/>
       <c r="G15" s="23"/>
     </row>
     <row r="16" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="153"/>
       <c r="B16" s="154" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="154"/>
       <c r="D16" s="154"/>
@@ -5007,54 +5007,54 @@
     <row r="17" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="C17" s="185" t="str">
+        <v>171</v>
+      </c>
+      <c r="C17" s="184" t="str">
         <f>VLOOKUP(B17,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D17" s="185"/>
-      <c r="E17" s="185" t="str">
+      <c r="D17" s="184"/>
+      <c r="E17" s="184" t="str">
         <f>VLOOKUP(B17,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F17" s="185"/>
+      <c r="F17" s="184"/>
       <c r="G17" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C18" s="185" t="e">
+        <v>75</v>
+      </c>
+      <c r="C18" s="184" t="e">
         <f>VLOOKUP(B18,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D18" s="185"/>
-      <c r="E18" s="185" t="e">
+      <c r="D18" s="184"/>
+      <c r="E18" s="184" t="e">
         <f>VLOOKUP(B18,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F18" s="185"/>
+      <c r="F18" s="184"/>
       <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="185" t="e">
+        <v>75</v>
+      </c>
+      <c r="C19" s="184" t="e">
         <f>VLOOKUP(B19,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D19" s="185"/>
-      <c r="E19" s="185" t="e">
+      <c r="D19" s="184"/>
+      <c r="E19" s="184" t="e">
         <f>VLOOKUP(B19,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F19" s="185"/>
+      <c r="F19" s="184"/>
       <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -5071,37 +5071,37 @@
     <row r="21" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C21" s="185" t="str">
+        <v>169</v>
+      </c>
+      <c r="C21" s="184" t="str">
         <f>VLOOKUP(B21,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D21" s="185"/>
-      <c r="E21" s="185" t="str">
+      <c r="D21" s="184"/>
+      <c r="E21" s="184" t="str">
         <f>VLOOKUP(B21,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F21" s="185"/>
+      <c r="F21" s="184"/>
       <c r="G21" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C22" s="185" t="e">
+        <v>75</v>
+      </c>
+      <c r="C22" s="184" t="e">
         <f>VLOOKUP(B22,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D22" s="185"/>
-      <c r="E22" s="185" t="e">
+      <c r="D22" s="184"/>
+      <c r="E22" s="184" t="e">
         <f>VLOOKUP(B22,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F22" s="185"/>
+      <c r="F22" s="184"/>
       <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -5118,20 +5118,20 @@
     <row r="24" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="C24" s="185" t="str">
+        <v>171</v>
+      </c>
+      <c r="C24" s="184" t="str">
         <f>VLOOKUP(B24,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D24" s="185"/>
-      <c r="E24" s="185" t="str">
+      <c r="D24" s="184"/>
+      <c r="E24" s="184" t="str">
         <f>VLOOKUP(B24,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F24" s="185"/>
+      <c r="F24" s="184"/>
       <c r="G24" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
@@ -5148,26 +5148,26 @@
     <row r="26" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="C26" s="185" t="str">
+        <v>171</v>
+      </c>
+      <c r="C26" s="184" t="str">
         <f>VLOOKUP(B26,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D26" s="185"/>
-      <c r="E26" s="185" t="str">
+      <c r="D26" s="184"/>
+      <c r="E26" s="184" t="str">
         <f>VLOOKUP(B26,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F26" s="185"/>
+      <c r="F26" s="184"/>
       <c r="G26" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="153"/>
       <c r="B27" s="154" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C27" s="154"/>
       <c r="D27" s="154"/>
@@ -5178,26 +5178,26 @@
     <row r="28" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="C28" s="185" t="str">
+        <v>172</v>
+      </c>
+      <c r="C28" s="184" t="str">
         <f>VLOOKUP(B28,$B$50:$D$66,2,0)</f>
         <v>33 3807 6830</v>
       </c>
-      <c r="D28" s="185"/>
-      <c r="E28" s="185" t="str">
+      <c r="D28" s="184"/>
+      <c r="E28" s="184" t="str">
         <f>VLOOKUP(B28,$B$50:$D$66,3,0)</f>
         <v>asosa@qualtop.com</v>
       </c>
-      <c r="F28" s="185"/>
+      <c r="F28" s="184"/>
       <c r="G28" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="153"/>
       <c r="B29" s="154" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" s="154"/>
       <c r="D29" s="154"/>
@@ -5208,26 +5208,26 @@
     <row r="30" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="26"/>
       <c r="B30" s="21" t="s">
-        <v>173</v>
-      </c>
-      <c r="C30" s="185" t="str">
+        <v>172</v>
+      </c>
+      <c r="C30" s="184" t="str">
         <f>VLOOKUP(B30,$B$50:$D$66,2,0)</f>
         <v>33 3807 6830</v>
       </c>
-      <c r="D30" s="185"/>
-      <c r="E30" s="185" t="str">
+      <c r="D30" s="184"/>
+      <c r="E30" s="184" t="str">
         <f>VLOOKUP(B30,$B$50:$D$66,3,0)</f>
         <v>asosa@qualtop.com</v>
       </c>
-      <c r="F30" s="185"/>
+      <c r="F30" s="184"/>
       <c r="G30" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="153"/>
       <c r="B31" s="154" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C31" s="154"/>
       <c r="D31" s="154"/>
@@ -5238,26 +5238,26 @@
     <row r="32" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="26"/>
       <c r="B32" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C32" s="185" t="str">
+        <v>169</v>
+      </c>
+      <c r="C32" s="184" t="str">
         <f>VLOOKUP(B32,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D32" s="185"/>
-      <c r="E32" s="185" t="str">
+      <c r="D32" s="184"/>
+      <c r="E32" s="184" t="str">
         <f>VLOOKUP(B32,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F32" s="185"/>
+      <c r="F32" s="184"/>
       <c r="G32" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="153"/>
       <c r="B33" s="154" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C33" s="154"/>
       <c r="D33" s="154"/>
@@ -5268,26 +5268,26 @@
     <row r="34" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="26"/>
       <c r="B34" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="C34" s="186" t="str">
+        <v>171</v>
+      </c>
+      <c r="C34" s="187" t="str">
         <f>VLOOKUP(B34,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D34" s="186"/>
-      <c r="E34" s="186" t="str">
+      <c r="D34" s="187"/>
+      <c r="E34" s="187" t="str">
         <f>VLOOKUP(B34,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F34" s="186"/>
+      <c r="F34" s="187"/>
       <c r="G34" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="153"/>
       <c r="B35" s="154" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C35" s="154"/>
       <c r="D35" s="154"/>
@@ -5298,26 +5298,26 @@
     <row r="36" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26"/>
       <c r="B36" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C36" s="186" t="str">
+        <v>169</v>
+      </c>
+      <c r="C36" s="187" t="str">
         <f>VLOOKUP(B36,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D36" s="186"/>
-      <c r="E36" s="186" t="str">
+      <c r="D36" s="187"/>
+      <c r="E36" s="187" t="str">
         <f>VLOOKUP(B36,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F36" s="186"/>
+      <c r="F36" s="187"/>
       <c r="G36" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A37" s="153"/>
       <c r="B37" s="154" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C37" s="154"/>
       <c r="D37" s="154"/>
@@ -5328,26 +5328,26 @@
     <row r="38" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26"/>
       <c r="B38" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="C38" s="185" t="str">
+        <v>171</v>
+      </c>
+      <c r="C38" s="184" t="str">
         <f>VLOOKUP(B38,$B$50:$D$66,2,0)</f>
         <v>22 2752 8219</v>
       </c>
-      <c r="D38" s="185"/>
-      <c r="E38" s="185" t="str">
+      <c r="D38" s="184"/>
+      <c r="E38" s="184" t="str">
         <f>VLOOKUP(B38,$B$50:$D$66,3,0)</f>
         <v>jzepeda@qualtop.com</v>
       </c>
-      <c r="F38" s="185"/>
+      <c r="F38" s="184"/>
       <c r="G38" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="24.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="153"/>
       <c r="B39" s="154" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C39" s="154"/>
       <c r="D39" s="154"/>
@@ -5358,56 +5358,56 @@
     <row r="40" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26"/>
       <c r="B40" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="C40" s="185" t="str">
+        <v>164</v>
+      </c>
+      <c r="C40" s="184" t="str">
         <f>VLOOKUP(B40,$B$50:$D$66,2,0)</f>
         <v>33 1862 1719</v>
       </c>
-      <c r="D40" s="185"/>
-      <c r="E40" s="185" t="str">
+      <c r="D40" s="184"/>
+      <c r="E40" s="184" t="str">
         <f>VLOOKUP(B40,$B$50:$D$66,3,0)</f>
         <v>rpulido@qualtop.com</v>
       </c>
-      <c r="F40" s="185"/>
+      <c r="F40" s="184"/>
       <c r="G40" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="26"/>
       <c r="B41" s="21" t="s">
-        <v>170</v>
-      </c>
-      <c r="C41" s="185" t="str">
+        <v>169</v>
+      </c>
+      <c r="C41" s="184" t="str">
         <f>VLOOKUP(B41,$B$50:$D$66,2,0)</f>
         <v>33 3504 5902</v>
       </c>
-      <c r="D41" s="185"/>
-      <c r="E41" s="185" t="str">
+      <c r="D41" s="184"/>
+      <c r="E41" s="184" t="str">
         <f>VLOOKUP(B41,$B$50:$D$66,3,0)</f>
         <v>charles.gonher@gmail.com</v>
       </c>
-      <c r="F41" s="185"/>
+      <c r="F41" s="184"/>
       <c r="G41" s="163" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26"/>
       <c r="B42" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="185" t="e">
+        <v>75</v>
+      </c>
+      <c r="C42" s="184" t="e">
         <f>VLOOKUP(B42,$B$50:$D$66,2,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="D42" s="185"/>
-      <c r="E42" s="185" t="e">
+      <c r="D42" s="184"/>
+      <c r="E42" s="184" t="e">
         <f>VLOOKUP(B42,$B$50:$D$66,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F42" s="185"/>
+      <c r="F42" s="184"/>
       <c r="G42" s="23"/>
     </row>
     <row r="43" spans="1:7" ht="18.75" outlineLevel="1" x14ac:dyDescent="0.3">
@@ -5423,21 +5423,21 @@
     </row>
     <row r="44" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5"/>
-      <c r="B44" s="184" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" s="184"/>
-      <c r="D44" s="184"/>
-      <c r="E44" s="184"/>
-      <c r="F44" s="184"/>
+      <c r="B44" s="198" t="s">
+        <v>242</v>
+      </c>
+      <c r="C44" s="188"/>
+      <c r="D44" s="188"/>
+      <c r="E44" s="188"/>
+      <c r="F44" s="188"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="184"/>
-      <c r="C45" s="184"/>
-      <c r="D45" s="184"/>
-      <c r="E45" s="184"/>
-      <c r="F45" s="184"/>
+      <c r="B45" s="188"/>
+      <c r="C45" s="188"/>
+      <c r="D45" s="188"/>
+      <c r="E45" s="188"/>
+      <c r="F45" s="188"/>
       <c r="G45" s="81"/>
     </row>
     <row r="46" spans="1:7" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -5458,57 +5458,57 @@
     </row>
     <row r="50" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B50" s="84" t="s">
+        <v>169</v>
+      </c>
+      <c r="C50" s="85" t="s">
+        <v>174</v>
+      </c>
+      <c r="D50" s="82" t="s">
         <v>170</v>
-      </c>
-      <c r="C50" s="85" t="s">
-        <v>175</v>
-      </c>
-      <c r="D50" s="82" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B51" s="84" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C51" s="85" t="s">
+        <v>175</v>
+      </c>
+      <c r="D51" s="82" t="s">
         <v>176</v>
-      </c>
-      <c r="D51" s="82" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B52" s="84" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C52" s="85" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D52" s="82" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B53" s="84" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C53" s="85" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" s="82" t="s">
         <v>178</v>
-      </c>
-      <c r="D53" s="82" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B54" s="84" t="s">
+        <v>179</v>
+      </c>
+      <c r="C54" s="85" t="s">
         <v>180</v>
       </c>
-      <c r="C54" s="85" t="s">
+      <c r="D54" s="82" t="s">
         <v>181</v>
-      </c>
-      <c r="D54" s="82" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.2">
@@ -5574,6 +5574,33 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="43">
+    <mergeCell ref="B44:F45"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E15:F15"/>
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C8:D8"/>
@@ -5590,33 +5617,6 @@
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B44:F45"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C42:D42"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WVM983093:WVM983106 JA50:JA66 SW50:SW66 ACS50:ACS66 AMO50:AMO66 AWK50:AWK66 BGG50:BGG66 BQC50:BQC66 BZY50:BZY66 CJU50:CJU66 CTQ50:CTQ66 DDM50:DDM66 DNI50:DNI66 DXE50:DXE66 EHA50:EHA66 EQW50:EQW66 FAS50:FAS66 FKO50:FKO66 FUK50:FUK66 GEG50:GEG66 GOC50:GOC66 GXY50:GXY66 HHU50:HHU66 HRQ50:HRQ66 IBM50:IBM66 ILI50:ILI66 IVE50:IVE66 JFA50:JFA66 JOW50:JOW66 JYS50:JYS66 KIO50:KIO66 KSK50:KSK66 LCG50:LCG66 LMC50:LMC66 LVY50:LVY66 MFU50:MFU66 MPQ50:MPQ66 MZM50:MZM66 NJI50:NJI66 NTE50:NTE66 ODA50:ODA66 OMW50:OMW66 OWS50:OWS66 PGO50:PGO66 PQK50:PQK66 QAG50:QAG66 QKC50:QKC66 QTY50:QTY66 RDU50:RDU66 RNQ50:RNQ66 RXM50:RXM66 SHI50:SHI66 SRE50:SRE66 TBA50:TBA66 TKW50:TKW66 TUS50:TUS66 UEO50:UEO66 UOK50:UOK66 UYG50:UYG66 VIC50:VIC66 VRY50:VRY66 WBU50:WBU66 WLQ50:WLQ66 WVM50:WVM66 D65570:D65583 JA65589:JA65602 SW65589:SW65602 ACS65589:ACS65602 AMO65589:AMO65602 AWK65589:AWK65602 BGG65589:BGG65602 BQC65589:BQC65602 BZY65589:BZY65602 CJU65589:CJU65602 CTQ65589:CTQ65602 DDM65589:DDM65602 DNI65589:DNI65602 DXE65589:DXE65602 EHA65589:EHA65602 EQW65589:EQW65602 FAS65589:FAS65602 FKO65589:FKO65602 FUK65589:FUK65602 GEG65589:GEG65602 GOC65589:GOC65602 GXY65589:GXY65602 HHU65589:HHU65602 HRQ65589:HRQ65602 IBM65589:IBM65602 ILI65589:ILI65602 IVE65589:IVE65602 JFA65589:JFA65602 JOW65589:JOW65602 JYS65589:JYS65602 KIO65589:KIO65602 KSK65589:KSK65602 LCG65589:LCG65602 LMC65589:LMC65602 LVY65589:LVY65602 MFU65589:MFU65602 MPQ65589:MPQ65602 MZM65589:MZM65602 NJI65589:NJI65602 NTE65589:NTE65602 ODA65589:ODA65602 OMW65589:OMW65602 OWS65589:OWS65602 PGO65589:PGO65602 PQK65589:PQK65602 QAG65589:QAG65602 QKC65589:QKC65602 QTY65589:QTY65602 RDU65589:RDU65602 RNQ65589:RNQ65602 RXM65589:RXM65602 SHI65589:SHI65602 SRE65589:SRE65602 TBA65589:TBA65602 TKW65589:TKW65602 TUS65589:TUS65602 UEO65589:UEO65602 UOK65589:UOK65602 UYG65589:UYG65602 VIC65589:VIC65602 VRY65589:VRY65602 WBU65589:WBU65602 WLQ65589:WLQ65602 WVM65589:WVM65602 D131106:D131119 JA131125:JA131138 SW131125:SW131138 ACS131125:ACS131138 AMO131125:AMO131138 AWK131125:AWK131138 BGG131125:BGG131138 BQC131125:BQC131138 BZY131125:BZY131138 CJU131125:CJU131138 CTQ131125:CTQ131138 DDM131125:DDM131138 DNI131125:DNI131138 DXE131125:DXE131138 EHA131125:EHA131138 EQW131125:EQW131138 FAS131125:FAS131138 FKO131125:FKO131138 FUK131125:FUK131138 GEG131125:GEG131138 GOC131125:GOC131138 GXY131125:GXY131138 HHU131125:HHU131138 HRQ131125:HRQ131138 IBM131125:IBM131138 ILI131125:ILI131138 IVE131125:IVE131138 JFA131125:JFA131138 JOW131125:JOW131138 JYS131125:JYS131138 KIO131125:KIO131138 KSK131125:KSK131138 LCG131125:LCG131138 LMC131125:LMC131138 LVY131125:LVY131138 MFU131125:MFU131138 MPQ131125:MPQ131138 MZM131125:MZM131138 NJI131125:NJI131138 NTE131125:NTE131138 ODA131125:ODA131138 OMW131125:OMW131138 OWS131125:OWS131138 PGO131125:PGO131138 PQK131125:PQK131138 QAG131125:QAG131138 QKC131125:QKC131138 QTY131125:QTY131138 RDU131125:RDU131138 RNQ131125:RNQ131138 RXM131125:RXM131138 SHI131125:SHI131138 SRE131125:SRE131138 TBA131125:TBA131138 TKW131125:TKW131138 TUS131125:TUS131138 UEO131125:UEO131138 UOK131125:UOK131138 UYG131125:UYG131138 VIC131125:VIC131138 VRY131125:VRY131138 WBU131125:WBU131138 WLQ131125:WLQ131138 WVM131125:WVM131138 D196642:D196655 JA196661:JA196674 SW196661:SW196674 ACS196661:ACS196674 AMO196661:AMO196674 AWK196661:AWK196674 BGG196661:BGG196674 BQC196661:BQC196674 BZY196661:BZY196674 CJU196661:CJU196674 CTQ196661:CTQ196674 DDM196661:DDM196674 DNI196661:DNI196674 DXE196661:DXE196674 EHA196661:EHA196674 EQW196661:EQW196674 FAS196661:FAS196674 FKO196661:FKO196674 FUK196661:FUK196674 GEG196661:GEG196674 GOC196661:GOC196674 GXY196661:GXY196674 HHU196661:HHU196674 HRQ196661:HRQ196674 IBM196661:IBM196674 ILI196661:ILI196674 IVE196661:IVE196674 JFA196661:JFA196674 JOW196661:JOW196674 JYS196661:JYS196674 KIO196661:KIO196674 KSK196661:KSK196674 LCG196661:LCG196674 LMC196661:LMC196674 LVY196661:LVY196674 MFU196661:MFU196674 MPQ196661:MPQ196674 MZM196661:MZM196674 NJI196661:NJI196674 NTE196661:NTE196674 ODA196661:ODA196674 OMW196661:OMW196674 OWS196661:OWS196674 PGO196661:PGO196674 PQK196661:PQK196674 QAG196661:QAG196674 QKC196661:QKC196674 QTY196661:QTY196674 RDU196661:RDU196674 RNQ196661:RNQ196674 RXM196661:RXM196674 SHI196661:SHI196674 SRE196661:SRE196674 TBA196661:TBA196674 TKW196661:TKW196674 TUS196661:TUS196674 UEO196661:UEO196674 UOK196661:UOK196674 UYG196661:UYG196674 VIC196661:VIC196674 VRY196661:VRY196674 WBU196661:WBU196674 WLQ196661:WLQ196674 WVM196661:WVM196674 D262178:D262191 JA262197:JA262210 SW262197:SW262210 ACS262197:ACS262210 AMO262197:AMO262210 AWK262197:AWK262210 BGG262197:BGG262210 BQC262197:BQC262210 BZY262197:BZY262210 CJU262197:CJU262210 CTQ262197:CTQ262210 DDM262197:DDM262210 DNI262197:DNI262210 DXE262197:DXE262210 EHA262197:EHA262210 EQW262197:EQW262210 FAS262197:FAS262210 FKO262197:FKO262210 FUK262197:FUK262210 GEG262197:GEG262210 GOC262197:GOC262210 GXY262197:GXY262210 HHU262197:HHU262210 HRQ262197:HRQ262210 IBM262197:IBM262210 ILI262197:ILI262210 IVE262197:IVE262210 JFA262197:JFA262210 JOW262197:JOW262210 JYS262197:JYS262210 KIO262197:KIO262210 KSK262197:KSK262210 LCG262197:LCG262210 LMC262197:LMC262210 LVY262197:LVY262210 MFU262197:MFU262210 MPQ262197:MPQ262210 MZM262197:MZM262210 NJI262197:NJI262210 NTE262197:NTE262210 ODA262197:ODA262210 OMW262197:OMW262210 OWS262197:OWS262210 PGO262197:PGO262210 PQK262197:PQK262210 QAG262197:QAG262210 QKC262197:QKC262210 QTY262197:QTY262210 RDU262197:RDU262210 RNQ262197:RNQ262210 RXM262197:RXM262210 SHI262197:SHI262210 SRE262197:SRE262210 TBA262197:TBA262210 TKW262197:TKW262210 TUS262197:TUS262210 UEO262197:UEO262210 UOK262197:UOK262210 UYG262197:UYG262210 VIC262197:VIC262210 VRY262197:VRY262210 WBU262197:WBU262210 WLQ262197:WLQ262210 WVM262197:WVM262210 D327714:D327727 JA327733:JA327746 SW327733:SW327746 ACS327733:ACS327746 AMO327733:AMO327746 AWK327733:AWK327746 BGG327733:BGG327746 BQC327733:BQC327746 BZY327733:BZY327746 CJU327733:CJU327746 CTQ327733:CTQ327746 DDM327733:DDM327746 DNI327733:DNI327746 DXE327733:DXE327746 EHA327733:EHA327746 EQW327733:EQW327746 FAS327733:FAS327746 FKO327733:FKO327746 FUK327733:FUK327746 GEG327733:GEG327746 GOC327733:GOC327746 GXY327733:GXY327746 HHU327733:HHU327746 HRQ327733:HRQ327746 IBM327733:IBM327746 ILI327733:ILI327746 IVE327733:IVE327746 JFA327733:JFA327746 JOW327733:JOW327746 JYS327733:JYS327746 KIO327733:KIO327746 KSK327733:KSK327746 LCG327733:LCG327746 LMC327733:LMC327746 LVY327733:LVY327746 MFU327733:MFU327746 MPQ327733:MPQ327746 MZM327733:MZM327746 NJI327733:NJI327746 NTE327733:NTE327746 ODA327733:ODA327746 OMW327733:OMW327746 OWS327733:OWS327746 PGO327733:PGO327746 PQK327733:PQK327746 QAG327733:QAG327746 QKC327733:QKC327746 QTY327733:QTY327746 RDU327733:RDU327746 RNQ327733:RNQ327746 RXM327733:RXM327746 SHI327733:SHI327746 SRE327733:SRE327746 TBA327733:TBA327746 TKW327733:TKW327746 TUS327733:TUS327746 UEO327733:UEO327746 UOK327733:UOK327746 UYG327733:UYG327746 VIC327733:VIC327746 VRY327733:VRY327746 WBU327733:WBU327746 WLQ327733:WLQ327746 WVM327733:WVM327746 D393250:D393263 JA393269:JA393282 SW393269:SW393282 ACS393269:ACS393282 AMO393269:AMO393282 AWK393269:AWK393282 BGG393269:BGG393282 BQC393269:BQC393282 BZY393269:BZY393282 CJU393269:CJU393282 CTQ393269:CTQ393282 DDM393269:DDM393282 DNI393269:DNI393282 DXE393269:DXE393282 EHA393269:EHA393282 EQW393269:EQW393282 FAS393269:FAS393282 FKO393269:FKO393282 FUK393269:FUK393282 GEG393269:GEG393282 GOC393269:GOC393282 GXY393269:GXY393282 HHU393269:HHU393282 HRQ393269:HRQ393282 IBM393269:IBM393282 ILI393269:ILI393282 IVE393269:IVE393282 JFA393269:JFA393282 JOW393269:JOW393282 JYS393269:JYS393282 KIO393269:KIO393282 KSK393269:KSK393282 LCG393269:LCG393282 LMC393269:LMC393282 LVY393269:LVY393282 MFU393269:MFU393282 MPQ393269:MPQ393282 MZM393269:MZM393282 NJI393269:NJI393282 NTE393269:NTE393282 ODA393269:ODA393282 OMW393269:OMW393282 OWS393269:OWS393282 PGO393269:PGO393282 PQK393269:PQK393282 QAG393269:QAG393282 QKC393269:QKC393282 QTY393269:QTY393282 RDU393269:RDU393282 RNQ393269:RNQ393282 RXM393269:RXM393282 SHI393269:SHI393282 SRE393269:SRE393282 TBA393269:TBA393282 TKW393269:TKW393282 TUS393269:TUS393282 UEO393269:UEO393282 UOK393269:UOK393282 UYG393269:UYG393282 VIC393269:VIC393282 VRY393269:VRY393282 WBU393269:WBU393282 WLQ393269:WLQ393282 WVM393269:WVM393282 D458786:D458799 JA458805:JA458818 SW458805:SW458818 ACS458805:ACS458818 AMO458805:AMO458818 AWK458805:AWK458818 BGG458805:BGG458818 BQC458805:BQC458818 BZY458805:BZY458818 CJU458805:CJU458818 CTQ458805:CTQ458818 DDM458805:DDM458818 DNI458805:DNI458818 DXE458805:DXE458818 EHA458805:EHA458818 EQW458805:EQW458818 FAS458805:FAS458818 FKO458805:FKO458818 FUK458805:FUK458818 GEG458805:GEG458818 GOC458805:GOC458818 GXY458805:GXY458818 HHU458805:HHU458818 HRQ458805:HRQ458818 IBM458805:IBM458818 ILI458805:ILI458818 IVE458805:IVE458818 JFA458805:JFA458818 JOW458805:JOW458818 JYS458805:JYS458818 KIO458805:KIO458818 KSK458805:KSK458818 LCG458805:LCG458818 LMC458805:LMC458818 LVY458805:LVY458818 MFU458805:MFU458818 MPQ458805:MPQ458818 MZM458805:MZM458818 NJI458805:NJI458818 NTE458805:NTE458818 ODA458805:ODA458818 OMW458805:OMW458818 OWS458805:OWS458818 PGO458805:PGO458818 PQK458805:PQK458818 QAG458805:QAG458818 QKC458805:QKC458818 QTY458805:QTY458818 RDU458805:RDU458818 RNQ458805:RNQ458818 RXM458805:RXM458818 SHI458805:SHI458818 SRE458805:SRE458818 TBA458805:TBA458818 TKW458805:TKW458818 TUS458805:TUS458818 UEO458805:UEO458818 UOK458805:UOK458818 UYG458805:UYG458818 VIC458805:VIC458818 VRY458805:VRY458818 WBU458805:WBU458818 WLQ458805:WLQ458818 WVM458805:WVM458818 D524322:D524335 JA524341:JA524354 SW524341:SW524354 ACS524341:ACS524354 AMO524341:AMO524354 AWK524341:AWK524354 BGG524341:BGG524354 BQC524341:BQC524354 BZY524341:BZY524354 CJU524341:CJU524354 CTQ524341:CTQ524354 DDM524341:DDM524354 DNI524341:DNI524354 DXE524341:DXE524354 EHA524341:EHA524354 EQW524341:EQW524354 FAS524341:FAS524354 FKO524341:FKO524354 FUK524341:FUK524354 GEG524341:GEG524354 GOC524341:GOC524354 GXY524341:GXY524354 HHU524341:HHU524354 HRQ524341:HRQ524354 IBM524341:IBM524354 ILI524341:ILI524354 IVE524341:IVE524354 JFA524341:JFA524354 JOW524341:JOW524354 JYS524341:JYS524354 KIO524341:KIO524354 KSK524341:KSK524354 LCG524341:LCG524354 LMC524341:LMC524354 LVY524341:LVY524354 MFU524341:MFU524354 MPQ524341:MPQ524354 MZM524341:MZM524354 NJI524341:NJI524354 NTE524341:NTE524354 ODA524341:ODA524354 OMW524341:OMW524354 OWS524341:OWS524354 PGO524341:PGO524354 PQK524341:PQK524354 QAG524341:QAG524354 QKC524341:QKC524354 QTY524341:QTY524354 RDU524341:RDU524354 RNQ524341:RNQ524354 RXM524341:RXM524354 SHI524341:SHI524354 SRE524341:SRE524354 TBA524341:TBA524354 TKW524341:TKW524354 TUS524341:TUS524354 UEO524341:UEO524354 UOK524341:UOK524354 UYG524341:UYG524354 VIC524341:VIC524354 VRY524341:VRY524354 WBU524341:WBU524354 WLQ524341:WLQ524354 WVM524341:WVM524354 D589858:D589871 JA589877:JA589890 SW589877:SW589890 ACS589877:ACS589890 AMO589877:AMO589890 AWK589877:AWK589890 BGG589877:BGG589890 BQC589877:BQC589890 BZY589877:BZY589890 CJU589877:CJU589890 CTQ589877:CTQ589890 DDM589877:DDM589890 DNI589877:DNI589890 DXE589877:DXE589890 EHA589877:EHA589890 EQW589877:EQW589890 FAS589877:FAS589890 FKO589877:FKO589890 FUK589877:FUK589890 GEG589877:GEG589890 GOC589877:GOC589890 GXY589877:GXY589890 HHU589877:HHU589890 HRQ589877:HRQ589890 IBM589877:IBM589890 ILI589877:ILI589890 IVE589877:IVE589890 JFA589877:JFA589890 JOW589877:JOW589890 JYS589877:JYS589890 KIO589877:KIO589890 KSK589877:KSK589890 LCG589877:LCG589890 LMC589877:LMC589890 LVY589877:LVY589890 MFU589877:MFU589890 MPQ589877:MPQ589890 MZM589877:MZM589890 NJI589877:NJI589890 NTE589877:NTE589890 ODA589877:ODA589890 OMW589877:OMW589890 OWS589877:OWS589890 PGO589877:PGO589890 PQK589877:PQK589890 QAG589877:QAG589890 QKC589877:QKC589890 QTY589877:QTY589890 RDU589877:RDU589890 RNQ589877:RNQ589890 RXM589877:RXM589890 SHI589877:SHI589890 SRE589877:SRE589890 TBA589877:TBA589890 TKW589877:TKW589890 TUS589877:TUS589890 UEO589877:UEO589890 UOK589877:UOK589890 UYG589877:UYG589890 VIC589877:VIC589890 VRY589877:VRY589890 WBU589877:WBU589890 WLQ589877:WLQ589890 WVM589877:WVM589890 D655394:D655407 JA655413:JA655426 SW655413:SW655426 ACS655413:ACS655426 AMO655413:AMO655426 AWK655413:AWK655426 BGG655413:BGG655426 BQC655413:BQC655426 BZY655413:BZY655426 CJU655413:CJU655426 CTQ655413:CTQ655426 DDM655413:DDM655426 DNI655413:DNI655426 DXE655413:DXE655426 EHA655413:EHA655426 EQW655413:EQW655426 FAS655413:FAS655426 FKO655413:FKO655426 FUK655413:FUK655426 GEG655413:GEG655426 GOC655413:GOC655426 GXY655413:GXY655426 HHU655413:HHU655426 HRQ655413:HRQ655426 IBM655413:IBM655426 ILI655413:ILI655426 IVE655413:IVE655426 JFA655413:JFA655426 JOW655413:JOW655426 JYS655413:JYS655426 KIO655413:KIO655426 KSK655413:KSK655426 LCG655413:LCG655426 LMC655413:LMC655426 LVY655413:LVY655426 MFU655413:MFU655426 MPQ655413:MPQ655426 MZM655413:MZM655426 NJI655413:NJI655426 NTE655413:NTE655426 ODA655413:ODA655426 OMW655413:OMW655426 OWS655413:OWS655426 PGO655413:PGO655426 PQK655413:PQK655426 QAG655413:QAG655426 QKC655413:QKC655426 QTY655413:QTY655426 RDU655413:RDU655426 RNQ655413:RNQ655426 RXM655413:RXM655426 SHI655413:SHI655426 SRE655413:SRE655426 TBA655413:TBA655426 TKW655413:TKW655426 TUS655413:TUS655426 UEO655413:UEO655426 UOK655413:UOK655426 UYG655413:UYG655426 VIC655413:VIC655426 VRY655413:VRY655426 WBU655413:WBU655426 WLQ655413:WLQ655426 WVM655413:WVM655426 D720930:D720943 JA720949:JA720962 SW720949:SW720962 ACS720949:ACS720962 AMO720949:AMO720962 AWK720949:AWK720962 BGG720949:BGG720962 BQC720949:BQC720962 BZY720949:BZY720962 CJU720949:CJU720962 CTQ720949:CTQ720962 DDM720949:DDM720962 DNI720949:DNI720962 DXE720949:DXE720962 EHA720949:EHA720962 EQW720949:EQW720962 FAS720949:FAS720962 FKO720949:FKO720962 FUK720949:FUK720962 GEG720949:GEG720962 GOC720949:GOC720962 GXY720949:GXY720962 HHU720949:HHU720962 HRQ720949:HRQ720962 IBM720949:IBM720962 ILI720949:ILI720962 IVE720949:IVE720962 JFA720949:JFA720962 JOW720949:JOW720962 JYS720949:JYS720962 KIO720949:KIO720962 KSK720949:KSK720962 LCG720949:LCG720962 LMC720949:LMC720962 LVY720949:LVY720962 MFU720949:MFU720962 MPQ720949:MPQ720962 MZM720949:MZM720962 NJI720949:NJI720962 NTE720949:NTE720962 ODA720949:ODA720962 OMW720949:OMW720962 OWS720949:OWS720962 PGO720949:PGO720962 PQK720949:PQK720962 QAG720949:QAG720962 QKC720949:QKC720962 QTY720949:QTY720962 RDU720949:RDU720962 RNQ720949:RNQ720962 RXM720949:RXM720962 SHI720949:SHI720962 SRE720949:SRE720962 TBA720949:TBA720962 TKW720949:TKW720962 TUS720949:TUS720962 UEO720949:UEO720962 UOK720949:UOK720962 UYG720949:UYG720962 VIC720949:VIC720962 VRY720949:VRY720962 WBU720949:WBU720962 WLQ720949:WLQ720962 WVM720949:WVM720962 D786466:D786479 JA786485:JA786498 SW786485:SW786498 ACS786485:ACS786498 AMO786485:AMO786498 AWK786485:AWK786498 BGG786485:BGG786498 BQC786485:BQC786498 BZY786485:BZY786498 CJU786485:CJU786498 CTQ786485:CTQ786498 DDM786485:DDM786498 DNI786485:DNI786498 DXE786485:DXE786498 EHA786485:EHA786498 EQW786485:EQW786498 FAS786485:FAS786498 FKO786485:FKO786498 FUK786485:FUK786498 GEG786485:GEG786498 GOC786485:GOC786498 GXY786485:GXY786498 HHU786485:HHU786498 HRQ786485:HRQ786498 IBM786485:IBM786498 ILI786485:ILI786498 IVE786485:IVE786498 JFA786485:JFA786498 JOW786485:JOW786498 JYS786485:JYS786498 KIO786485:KIO786498 KSK786485:KSK786498 LCG786485:LCG786498 LMC786485:LMC786498 LVY786485:LVY786498 MFU786485:MFU786498 MPQ786485:MPQ786498 MZM786485:MZM786498 NJI786485:NJI786498 NTE786485:NTE786498 ODA786485:ODA786498 OMW786485:OMW786498 OWS786485:OWS786498 PGO786485:PGO786498 PQK786485:PQK786498 QAG786485:QAG786498 QKC786485:QKC786498 QTY786485:QTY786498 RDU786485:RDU786498 RNQ786485:RNQ786498 RXM786485:RXM786498 SHI786485:SHI786498 SRE786485:SRE786498 TBA786485:TBA786498 TKW786485:TKW786498 TUS786485:TUS786498 UEO786485:UEO786498 UOK786485:UOK786498 UYG786485:UYG786498 VIC786485:VIC786498 VRY786485:VRY786498 WBU786485:WBU786498 WLQ786485:WLQ786498 WVM786485:WVM786498 D852002:D852015 JA852021:JA852034 SW852021:SW852034 ACS852021:ACS852034 AMO852021:AMO852034 AWK852021:AWK852034 BGG852021:BGG852034 BQC852021:BQC852034 BZY852021:BZY852034 CJU852021:CJU852034 CTQ852021:CTQ852034 DDM852021:DDM852034 DNI852021:DNI852034 DXE852021:DXE852034 EHA852021:EHA852034 EQW852021:EQW852034 FAS852021:FAS852034 FKO852021:FKO852034 FUK852021:FUK852034 GEG852021:GEG852034 GOC852021:GOC852034 GXY852021:GXY852034 HHU852021:HHU852034 HRQ852021:HRQ852034 IBM852021:IBM852034 ILI852021:ILI852034 IVE852021:IVE852034 JFA852021:JFA852034 JOW852021:JOW852034 JYS852021:JYS852034 KIO852021:KIO852034 KSK852021:KSK852034 LCG852021:LCG852034 LMC852021:LMC852034 LVY852021:LVY852034 MFU852021:MFU852034 MPQ852021:MPQ852034 MZM852021:MZM852034 NJI852021:NJI852034 NTE852021:NTE852034 ODA852021:ODA852034 OMW852021:OMW852034 OWS852021:OWS852034 PGO852021:PGO852034 PQK852021:PQK852034 QAG852021:QAG852034 QKC852021:QKC852034 QTY852021:QTY852034 RDU852021:RDU852034 RNQ852021:RNQ852034 RXM852021:RXM852034 SHI852021:SHI852034 SRE852021:SRE852034 TBA852021:TBA852034 TKW852021:TKW852034 TUS852021:TUS852034 UEO852021:UEO852034 UOK852021:UOK852034 UYG852021:UYG852034 VIC852021:VIC852034 VRY852021:VRY852034 WBU852021:WBU852034 WLQ852021:WLQ852034 WVM852021:WVM852034 D917538:D917551 JA917557:JA917570 SW917557:SW917570 ACS917557:ACS917570 AMO917557:AMO917570 AWK917557:AWK917570 BGG917557:BGG917570 BQC917557:BQC917570 BZY917557:BZY917570 CJU917557:CJU917570 CTQ917557:CTQ917570 DDM917557:DDM917570 DNI917557:DNI917570 DXE917557:DXE917570 EHA917557:EHA917570 EQW917557:EQW917570 FAS917557:FAS917570 FKO917557:FKO917570 FUK917557:FUK917570 GEG917557:GEG917570 GOC917557:GOC917570 GXY917557:GXY917570 HHU917557:HHU917570 HRQ917557:HRQ917570 IBM917557:IBM917570 ILI917557:ILI917570 IVE917557:IVE917570 JFA917557:JFA917570 JOW917557:JOW917570 JYS917557:JYS917570 KIO917557:KIO917570 KSK917557:KSK917570 LCG917557:LCG917570 LMC917557:LMC917570 LVY917557:LVY917570 MFU917557:MFU917570 MPQ917557:MPQ917570 MZM917557:MZM917570 NJI917557:NJI917570 NTE917557:NTE917570 ODA917557:ODA917570 OMW917557:OMW917570 OWS917557:OWS917570 PGO917557:PGO917570 PQK917557:PQK917570 QAG917557:QAG917570 QKC917557:QKC917570 QTY917557:QTY917570 RDU917557:RDU917570 RNQ917557:RNQ917570 RXM917557:RXM917570 SHI917557:SHI917570 SRE917557:SRE917570 TBA917557:TBA917570 TKW917557:TKW917570 TUS917557:TUS917570 UEO917557:UEO917570 UOK917557:UOK917570 UYG917557:UYG917570 VIC917557:VIC917570 VRY917557:VRY917570 WBU917557:WBU917570 WLQ917557:WLQ917570 WVM917557:WVM917570 D983074:D983087 JA983093:JA983106 SW983093:SW983106 ACS983093:ACS983106 AMO983093:AMO983106 AWK983093:AWK983106 BGG983093:BGG983106 BQC983093:BQC983106 BZY983093:BZY983106 CJU983093:CJU983106 CTQ983093:CTQ983106 DDM983093:DDM983106 DNI983093:DNI983106 DXE983093:DXE983106 EHA983093:EHA983106 EQW983093:EQW983106 FAS983093:FAS983106 FKO983093:FKO983106 FUK983093:FUK983106 GEG983093:GEG983106 GOC983093:GOC983106 GXY983093:GXY983106 HHU983093:HHU983106 HRQ983093:HRQ983106 IBM983093:IBM983106 ILI983093:ILI983106 IVE983093:IVE983106 JFA983093:JFA983106 JOW983093:JOW983106 JYS983093:JYS983106 KIO983093:KIO983106 KSK983093:KSK983106 LCG983093:LCG983106 LMC983093:LMC983106 LVY983093:LVY983106 MFU983093:MFU983106 MPQ983093:MPQ983106 MZM983093:MZM983106 NJI983093:NJI983106 NTE983093:NTE983106 ODA983093:ODA983106 OMW983093:OMW983106 OWS983093:OWS983106 PGO983093:PGO983106 PQK983093:PQK983106 QAG983093:QAG983106 QKC983093:QKC983106 QTY983093:QTY983106 RDU983093:RDU983106 RNQ983093:RNQ983106 RXM983093:RXM983106 SHI983093:SHI983106 SRE983093:SRE983106 TBA983093:TBA983106 TKW983093:TKW983106 TUS983093:TUS983106 UEO983093:UEO983106 UOK983093:UOK983106 UYG983093:UYG983106 VIC983093:VIC983106 VRY983093:VRY983106 WBU983093:WBU983106 WLQ983093:WLQ983106">
@@ -5651,15 +5651,16 @@
     <hyperlink ref="G38" r:id="rId19" display="Vease en matriz de roles"/>
     <hyperlink ref="G40" r:id="rId20" display="Vease en matriz de roles"/>
     <hyperlink ref="G41" r:id="rId21" display="Vease en matriz de roles"/>
+    <hyperlink ref="B44" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
     <ignoredError sqref="C10" evalError="1"/>
   </ignoredErrors>
-  <drawing r:id="rId23"/>
-  <legacyDrawing r:id="rId24"/>
+  <drawing r:id="rId24"/>
+  <legacyDrawing r:id="rId25"/>
 </worksheet>
 </file>
 
@@ -6452,7 +6453,7 @@
     <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -6484,56 +6485,56 @@
     <row r="4" spans="1:12" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>257</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>258</v>
       </c>
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:12" s="10" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B5" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>185</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G5" s="12"/>
       <c r="L5" s="82"/>
     </row>
     <row r="6" spans="1:12" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B6" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E6" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>225</v>
       </c>
       <c r="G6" s="12"/>
       <c r="L6" s="82"/>
@@ -7624,7 +7625,7 @@
         <v>47</v>
       </c>
       <c r="JB2" s="160" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="JC2" s="27">
         <v>5</v>
@@ -7663,7 +7664,7 @@
         <v>59</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G3" s="38" t="s">
         <v>53</v>
@@ -7685,7 +7686,7 @@
         <v>57</v>
       </c>
       <c r="N3" s="38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O3" s="38" t="s">
         <v>56</v>
@@ -7701,7 +7702,7 @@
       </c>
       <c r="S3" s="189"/>
       <c r="JB3" s="160" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="JC3" s="27">
         <v>4</v>
@@ -7726,7 +7727,7 @@
     <row r="4" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="165"/>
       <c r="B4" s="164" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="164"/>
       <c r="D4" s="166"/>
@@ -7746,7 +7747,7 @@
       <c r="R4" s="169"/>
       <c r="S4" s="189"/>
       <c r="JB4" s="160" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="JC4" s="27">
         <v>3</v>
@@ -7773,19 +7774,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="54" t="s">
+        <v>264</v>
+      </c>
+      <c r="C5" s="54" t="s">
         <v>265</v>
-      </c>
-      <c r="C5" s="54" t="s">
-        <v>266</v>
       </c>
       <c r="D5" s="73" t="s">
         <v>64</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G5" s="141">
         <v>1</v>
@@ -7801,22 +7802,22 @@
       </c>
       <c r="K5" s="35"/>
       <c r="L5" s="54" t="s">
+        <v>266</v>
+      </c>
+      <c r="M5" s="175" t="s">
         <v>267</v>
       </c>
-      <c r="M5" s="175" t="s">
-        <v>268</v>
-      </c>
       <c r="N5" s="175" t="s">
+        <v>203</v>
+      </c>
+      <c r="O5" s="52" t="s">
         <v>204</v>
       </c>
-      <c r="O5" s="52" t="s">
+      <c r="P5" s="52" t="s">
         <v>205</v>
       </c>
-      <c r="P5" s="52" t="s">
-        <v>206</v>
-      </c>
       <c r="Q5" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R5" s="42"/>
       <c r="S5" s="189"/>
@@ -7833,19 +7834,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D6" s="73" t="s">
         <v>64</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G6" s="141">
         <v>2</v>
@@ -7857,31 +7858,31 @@
         <v>37</v>
       </c>
       <c r="J6" s="137" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K6" s="35"/>
       <c r="L6" s="53" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M6" s="175" t="s">
+        <v>269</v>
+      </c>
+      <c r="N6" s="175" t="s">
         <v>270</v>
       </c>
-      <c r="N6" s="175" t="s">
-        <v>271</v>
-      </c>
       <c r="O6" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="P6" s="52" t="s">
         <v>209</v>
       </c>
-      <c r="P6" s="52" t="s">
-        <v>210</v>
-      </c>
       <c r="Q6" s="52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R6" s="59"/>
       <c r="S6" s="189"/>
       <c r="JB6" s="160" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="JC6" s="27">
         <v>2</v>
@@ -7908,19 +7909,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="53" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="54" t="s">
         <v>186</v>
       </c>
-      <c r="C7" s="54" t="s">
-        <v>187</v>
-      </c>
       <c r="D7" s="73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G7" s="141">
         <v>2</v>
@@ -7936,27 +7937,27 @@
       </c>
       <c r="K7" s="35"/>
       <c r="L7" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="M7" s="175" t="s">
         <v>272</v>
       </c>
-      <c r="M7" s="175" t="s">
+      <c r="N7" s="175" t="s">
         <v>273</v>
       </c>
-      <c r="N7" s="175" t="s">
+      <c r="O7" s="52" t="s">
         <v>274</v>
       </c>
-      <c r="O7" s="52" t="s">
-        <v>275</v>
-      </c>
       <c r="P7" s="52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="Q7" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R7" s="59"/>
       <c r="S7" s="189"/>
       <c r="JB7" s="160" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="JC7" s="27">
         <v>1</v>
@@ -7983,19 +7984,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="53" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="54" t="s">
         <v>188</v>
-      </c>
-      <c r="C8" s="54" t="s">
-        <v>189</v>
       </c>
       <c r="D8" s="73" t="s">
         <v>64</v>
       </c>
       <c r="E8" s="56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G8" s="141">
         <v>1</v>
@@ -8011,22 +8012,22 @@
       </c>
       <c r="K8" s="35"/>
       <c r="L8" s="53" t="s">
+        <v>275</v>
+      </c>
+      <c r="M8" s="175" t="s">
         <v>276</v>
       </c>
-      <c r="M8" s="175" t="s">
+      <c r="N8" s="175" t="s">
+        <v>212</v>
+      </c>
+      <c r="O8" s="52" t="s">
         <v>277</v>
       </c>
-      <c r="N8" s="175" t="s">
+      <c r="P8" s="52" t="s">
         <v>213</v>
       </c>
-      <c r="O8" s="52" t="s">
-        <v>278</v>
-      </c>
-      <c r="P8" s="52" t="s">
-        <v>214</v>
-      </c>
       <c r="Q8" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R8" s="59"/>
       <c r="JC8" s="32"/>
@@ -8050,7 +8051,7 @@
     <row r="9" spans="1:269" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="171"/>
       <c r="B9" s="172" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C9" s="164"/>
       <c r="D9" s="166"/>
@@ -8070,19 +8071,19 @@
       <c r="R9" s="174"/>
       <c r="JC9" s="32"/>
       <c r="JD9" s="160" t="s">
+        <v>148</v>
+      </c>
+      <c r="JE9" s="160" t="s">
         <v>149</v>
       </c>
-      <c r="JE9" s="160" t="s">
+      <c r="JF9" s="160" t="s">
         <v>150</v>
       </c>
-      <c r="JF9" s="160" t="s">
-        <v>151</v>
-      </c>
       <c r="JG9" s="160" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="JH9" s="160" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="JI9" s="32"/>
     </row>
@@ -8091,19 +8092,19 @@
         <v>1</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D10" s="73" t="s">
         <v>64</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G10" s="141">
         <v>1</v>
@@ -8119,22 +8120,22 @@
       </c>
       <c r="K10" s="35"/>
       <c r="L10" s="53" t="s">
+        <v>279</v>
+      </c>
+      <c r="M10" s="175" t="s">
         <v>280</v>
       </c>
-      <c r="M10" s="175" t="s">
+      <c r="N10" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="O10" s="52" t="s">
         <v>281</v>
       </c>
-      <c r="N10" s="36" t="s">
-        <v>215</v>
-      </c>
-      <c r="O10" s="52" t="s">
-        <v>282</v>
-      </c>
       <c r="P10" s="52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q10" s="52" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R10" s="59"/>
       <c r="JC10" s="32"/>
@@ -8152,19 +8153,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="54" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" s="73" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E11" s="56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G11" s="141">
         <v>2</v>
@@ -8180,22 +8181,22 @@
       </c>
       <c r="K11" s="35"/>
       <c r="L11" s="53" t="s">
+        <v>215</v>
+      </c>
+      <c r="M11" s="175" t="s">
         <v>216</v>
       </c>
-      <c r="M11" s="175" t="s">
-        <v>217</v>
-      </c>
       <c r="N11" s="175" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O11" s="52" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="P11" s="52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q11" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R11" s="59"/>
       <c r="JC11" s="32"/>
@@ -8211,19 +8212,19 @@
         <v>3</v>
       </c>
       <c r="B12" s="53" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D12" s="73" t="s">
         <v>64</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G12" s="141">
         <v>3</v>
@@ -8235,26 +8236,26 @@
         <v>39</v>
       </c>
       <c r="J12" s="137" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K12" s="35"/>
       <c r="L12" s="53" t="s">
+        <v>284</v>
+      </c>
+      <c r="M12" s="175" t="s">
+        <v>217</v>
+      </c>
+      <c r="N12" s="175" t="s">
         <v>285</v>
       </c>
-      <c r="M12" s="175" t="s">
+      <c r="O12" s="52" t="s">
         <v>218</v>
       </c>
-      <c r="N12" s="175" t="s">
-        <v>286</v>
-      </c>
-      <c r="O12" s="52" t="s">
-        <v>219</v>
-      </c>
       <c r="P12" s="52" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="Q12" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R12" s="59"/>
       <c r="JC12" s="142"/>
@@ -8272,19 +8273,19 @@
         <v>4</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C13" s="91" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D13" s="73" t="s">
         <v>64</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G13" s="141">
         <v>1</v>
@@ -8300,22 +8301,22 @@
       </c>
       <c r="K13" s="35"/>
       <c r="L13" s="53" t="s">
+        <v>287</v>
+      </c>
+      <c r="M13" s="175" t="s">
         <v>288</v>
       </c>
-      <c r="M13" s="175" t="s">
+      <c r="N13" s="175" t="s">
+        <v>219</v>
+      </c>
+      <c r="O13" s="52" t="s">
+        <v>220</v>
+      </c>
+      <c r="P13" s="52" t="s">
         <v>289</v>
       </c>
-      <c r="N13" s="175" t="s">
-        <v>220</v>
-      </c>
-      <c r="O13" s="52" t="s">
-        <v>221</v>
-      </c>
-      <c r="P13" s="52" t="s">
-        <v>290</v>
-      </c>
       <c r="Q13" s="52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="R13" s="59"/>
       <c r="JC13" s="50" t="s">
@@ -8359,7 +8360,7 @@
       </c>
       <c r="JE14" s="129"/>
       <c r="JF14" s="130" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="JG14" s="130"/>
       <c r="JH14" s="128"/>
@@ -8394,7 +8395,7 @@
       </c>
       <c r="JE15" s="130"/>
       <c r="JF15" s="130" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="JG15" s="130"/>
       <c r="JH15" s="127"/>
@@ -8427,7 +8428,7 @@
       </c>
       <c r="JE16" s="130"/>
       <c r="JF16" s="131" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="JG16" s="129"/>
       <c r="JH16" s="127"/>
@@ -8460,7 +8461,7 @@
       </c>
       <c r="JE17" s="130"/>
       <c r="JF17" s="131" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="JG17" s="129"/>
       <c r="JH17" s="127"/>
@@ -8489,11 +8490,11 @@
         <v>5</v>
       </c>
       <c r="JD18" s="47" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="JE18" s="129"/>
       <c r="JF18" s="131" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="JG18" s="129"/>
       <c r="JH18" s="128"/>
@@ -8526,7 +8527,7 @@
       </c>
       <c r="JE19" s="129"/>
       <c r="JF19" s="130" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="JG19" s="130"/>
       <c r="JH19" s="128"/>
@@ -8559,7 +8560,7 @@
       </c>
       <c r="JE20" s="129"/>
       <c r="JF20" s="130" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="JG20" s="130"/>
       <c r="JH20" s="128"/>
@@ -8791,7 +8792,7 @@
         <v>55</v>
       </c>
       <c r="JG30" s="121" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="JH30" s="32"/>
       <c r="JI30" s="32"/>
@@ -8806,13 +8807,13 @@
         <v>39</v>
       </c>
       <c r="JE31" s="123" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="JF31" s="124" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="JG31" s="124" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="JH31" s="32"/>
       <c r="JI31" s="32"/>
@@ -8827,13 +8828,13 @@
         <v>38</v>
       </c>
       <c r="JE32" s="123" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="JF32" s="123" t="s">
+        <v>128</v>
+      </c>
+      <c r="JG32" s="124" t="s">
         <v>129</v>
-      </c>
-      <c r="JG32" s="124" t="s">
-        <v>130</v>
       </c>
       <c r="JH32" s="32"/>
       <c r="JI32" s="32"/>
@@ -8848,13 +8849,13 @@
         <v>37</v>
       </c>
       <c r="JE33" s="123" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="JF33" s="124" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="JG33" s="124" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="JH33" s="32"/>
       <c r="JI33" s="32"/>
@@ -9142,10 +9143,10 @@
     <row r="64" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A64" s="32"/>
       <c r="B64" s="122" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="122" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D64" s="32"/>
       <c r="E64" s="32"/>
@@ -9162,10 +9163,10 @@
     <row r="65" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A65" s="32"/>
       <c r="B65" s="122" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C65" s="122" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D65" s="32"/>
       <c r="E65" s="32"/>
@@ -9182,10 +9183,10 @@
     <row r="66" spans="1:17" s="31" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
       <c r="A66" s="32"/>
       <c r="B66" s="122" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C66" s="122" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D66" s="32"/>
       <c r="E66" s="32"/>
@@ -10140,20 +10141,20 @@
     <row r="1" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="92" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="157" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="157" t="s">
         <v>84</v>
-      </c>
-      <c r="B3" s="157" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="192" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B4" s="193"/>
       <c r="D4" s="93"/>
@@ -10164,37 +10165,37 @@
     </row>
     <row r="5" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="95" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B5" s="94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D5" s="93"/>
       <c r="E5" s="100"/>
       <c r="F5" s="100"/>
       <c r="G5" s="100" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H5" s="100"/>
     </row>
     <row r="6" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="97" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6" s="94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D6" s="93"/>
       <c r="E6" s="100"/>
       <c r="F6" s="100"/>
       <c r="G6" s="100" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H6" s="100"/>
     </row>
     <row r="7" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="194" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B7" s="195"/>
       <c r="E7" s="100"/>
@@ -10204,23 +10205,23 @@
     </row>
     <row r="8" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="95" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E8" s="100" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="100" t="s">
         <v>91</v>
-      </c>
-      <c r="F8" s="100" t="s">
-        <v>92</v>
       </c>
       <c r="G8" s="100"/>
       <c r="H8" s="100"/>
     </row>
     <row r="9" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="190" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" s="191"/>
       <c r="C9" s="100"/>
@@ -10232,10 +10233,10 @@
     </row>
     <row r="10" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="97" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B10" s="94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C10" s="100"/>
       <c r="D10" s="100"/>
@@ -10246,7 +10247,7 @@
     </row>
     <row r="11" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="190" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B11" s="191"/>
       <c r="C11" s="100"/>
@@ -10258,10 +10259,10 @@
     </row>
     <row r="12" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="97" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12" s="94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C12" s="100"/>
       <c r="D12" s="100"/>
@@ -10272,10 +10273,10 @@
     </row>
     <row r="13" spans="1:8" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="99" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" s="94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C13" s="100"/>
       <c r="D13" s="100"/>
@@ -10286,17 +10287,17 @@
     </row>
     <row r="14" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="99" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14" s="94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C14" s="100"/>
       <c r="D14" s="100" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="100" t="s">
         <v>93</v>
-      </c>
-      <c r="E14" s="100" t="s">
-        <v>94</v>
       </c>
       <c r="F14" s="100"/>
       <c r="G14" s="100"/>
@@ -10304,7 +10305,7 @@
     </row>
     <row r="15" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="190" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B15" s="191"/>
       <c r="C15" s="100"/>
@@ -10316,10 +10317,10 @@
     </row>
     <row r="16" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="97" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B16" s="94" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C16" s="100"/>
       <c r="D16" s="100"/>
@@ -10383,10 +10384,10 @@
       <c r="B22" s="98"/>
       <c r="C22" s="100"/>
       <c r="D22" s="100" t="s">
+        <v>94</v>
+      </c>
+      <c r="E22" s="100" t="s">
         <v>95</v>
-      </c>
-      <c r="E22" s="100" t="s">
-        <v>96</v>
       </c>
       <c r="F22" s="100"/>
       <c r="G22" s="100"/>
@@ -10434,10 +10435,10 @@
       <c r="B27" s="98"/>
       <c r="C27" s="100"/>
       <c r="D27" s="100" t="s">
+        <v>96</v>
+      </c>
+      <c r="E27" s="100" t="s">
         <v>97</v>
-      </c>
-      <c r="E27" s="100" t="s">
-        <v>98</v>
       </c>
       <c r="F27" s="100"/>
       <c r="G27" s="100"/>
@@ -10474,10 +10475,10 @@
       <c r="B31" s="94"/>
       <c r="C31" s="100"/>
       <c r="D31" s="100" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="100" t="s">
         <v>97</v>
-      </c>
-      <c r="E31" s="100" t="s">
-        <v>98</v>
       </c>
       <c r="F31" s="100"/>
       <c r="G31" s="100"/>
@@ -10505,10 +10506,10 @@
       <c r="B34" s="94"/>
       <c r="C34" s="100"/>
       <c r="D34" s="100" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="100" t="s">
         <v>97</v>
-      </c>
-      <c r="E34" s="100" t="s">
-        <v>98</v>
       </c>
       <c r="F34" s="100"/>
       <c r="G34" s="100"/>
@@ -10605,92 +10606,92 @@
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="157" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" s="158" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" s="113"/>
     </row>
     <row r="4" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="125" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B4" s="114" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C4" s="113"/>
       <c r="D4" s="100"/>
       <c r="E4" s="100"/>
       <c r="F4" s="100"/>
       <c r="G4" s="100" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H4" s="100"/>
     </row>
     <row r="5" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="126" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B5" s="114" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C5" s="113"/>
       <c r="D5" s="100"/>
       <c r="E5" s="100"/>
       <c r="F5" s="100"/>
       <c r="G5" s="100" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H5" s="100"/>
     </row>
     <row r="6" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="126" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B6" s="114" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C6" s="113"/>
       <c r="D6" s="100"/>
       <c r="E6" s="100"/>
       <c r="F6" s="100"/>
       <c r="G6" s="100" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="100" t="s">
         <v>89</v>
-      </c>
-      <c r="H6" s="100" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="157" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="157" t="s">
         <v>100</v>
       </c>
-      <c r="B7" s="157" t="s">
-        <v>101</v>
-      </c>
       <c r="C7" s="159" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A8" s="125" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B8" s="101" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C8" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="100" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="100" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="100" t="s">
         <v>103</v>
-      </c>
-      <c r="E8" s="100" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="100" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" s="100" t="s">
-        <v>104</v>
       </c>
       <c r="H8" s="100"/>
       <c r="I8" s="100"/>
@@ -10698,13 +10699,13 @@
     </row>
     <row r="9" spans="1:10" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="126" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B9" s="102" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C9" s="94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" s="100"/>
       <c r="F9" s="100"/>
@@ -10715,13 +10716,13 @@
     </row>
     <row r="10" spans="1:10" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="176" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10" s="103" t="s">
         <v>299</v>
       </c>
-      <c r="B10" s="103" t="s">
-        <v>300</v>
-      </c>
       <c r="C10" s="94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E10" s="100"/>
       <c r="F10" s="100"/>
@@ -10730,13 +10731,13 @@
     </row>
     <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="126" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B11" s="102" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C11" s="94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E11" s="100"/>
       <c r="F11" s="100"/>
@@ -10745,13 +10746,13 @@
     </row>
     <row r="12" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="126" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B12" s="102" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C12" s="94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="100"/>
       <c r="E12" s="100"/>
@@ -10761,13 +10762,13 @@
     </row>
     <row r="13" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="126" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="104" t="s">
         <v>237</v>
       </c>
-      <c r="B13" s="104" t="s">
-        <v>238</v>
-      </c>
       <c r="C13" s="94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" s="100"/>
       <c r="E13" s="100"/>
@@ -10777,13 +10778,13 @@
     </row>
     <row r="14" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="126" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B14" s="104" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C14" s="94" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D14" s="100"/>
       <c r="E14" s="100"/>
@@ -10793,13 +10794,13 @@
     </row>
     <row r="15" spans="1:10" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="126" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B15" s="101" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C15" s="94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D15" s="100"/>
       <c r="E15" s="100"/>
@@ -10809,13 +10810,13 @@
     </row>
     <row r="16" spans="1:10" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="126" t="s">
+        <v>240</v>
+      </c>
+      <c r="B16" s="102" t="s">
         <v>241</v>
       </c>
-      <c r="B16" s="102" t="s">
-        <v>242</v>
-      </c>
       <c r="C16" s="94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D16" s="100"/>
       <c r="E16" s="100"/>
@@ -11753,7 +11754,7 @@
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -11764,36 +11765,36 @@
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G3" s="116"/>
       <c r="H3" s="116" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I3" s="116" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="67" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="116"/>
       <c r="H4" s="116" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I4" s="116" t="s">
         <v>9</v>
@@ -11802,13 +11803,13 @@
     <row r="5" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="67" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G5" s="116"/>
       <c r="H5" s="116"/>
@@ -11816,109 +11817,109 @@
     </row>
     <row r="6" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B6" s="62" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" s="117"/>
       <c r="H6" s="117"/>
       <c r="I6" s="116" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" s="62" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" s="117"/>
       <c r="H7" s="117"/>
       <c r="I7" s="116" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B8" s="62" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G8" s="117"/>
       <c r="H8" s="117"/>
       <c r="I8" s="118" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="62" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G9" s="117"/>
       <c r="H9" s="117"/>
       <c r="I9" s="118" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B10" s="62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G10" s="117"/>
       <c r="H10" s="117"/>
       <c r="I10" s="118" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B11" s="62" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G11" s="117"/>
       <c r="H11" s="117"/>
       <c r="I11" s="118" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B12" s="62" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G12" s="117"/>
       <c r="H12" s="117"/>
@@ -11926,13 +11927,13 @@
     </row>
     <row r="13" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="62" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G13" s="116"/>
       <c r="H13" s="116"/>
@@ -11977,8 +11978,8 @@
   </sheetPr>
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D4"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12756,7 +12757,7 @@
     <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="148"/>
       <c r="B2" s="149" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="148"/>
       <c r="D2" s="148"/>
@@ -12767,28 +12768,28 @@
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="197" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C3" s="197"/>
       <c r="D3" s="197"/>
       <c r="G3" s="116"/>
       <c r="H3" s="116" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I3" s="116" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="196" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C4" s="196"/>
       <c r="D4" s="196"/>
       <c r="G4" s="116"/>
       <c r="H4" s="116" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I4" s="116" t="s">
         <v>9</v>
@@ -12796,19 +12797,19 @@
     </row>
     <row r="5" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="196" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C5" s="196"/>
       <c r="D5" s="196"/>
       <c r="G5" s="117"/>
       <c r="H5" s="117"/>
       <c r="I5" s="116" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="196" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" s="196"/>
       <c r="D6" s="196"/>
@@ -12818,7 +12819,7 @@
     </row>
     <row r="7" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="196" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="196"/>
       <c r="D7" s="196"/>
@@ -12828,7 +12829,7 @@
     </row>
     <row r="8" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="196" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="196"/>
       <c r="D8" s="196"/>
@@ -12838,7 +12839,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="196" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" s="196"/>
       <c r="D9" s="196"/>
@@ -12859,7 +12860,7 @@
     <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="148"/>
       <c r="B12" s="149" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" s="148"/>
       <c r="D12" s="148"/>
@@ -12870,28 +12871,28 @@
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="197" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="197"/>
       <c r="D13" s="197"/>
       <c r="G13" s="116"/>
       <c r="H13" s="116" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I13" s="116" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="196" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C14" s="196"/>
       <c r="D14" s="196"/>
       <c r="G14" s="116"/>
       <c r="H14" s="116" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I14" s="116" t="s">
         <v>9</v>
@@ -12899,19 +12900,19 @@
     </row>
     <row r="15" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B15" s="196" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C15" s="196"/>
       <c r="D15" s="196"/>
       <c r="G15" s="117"/>
       <c r="H15" s="117"/>
       <c r="I15" s="116" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B16" s="196" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C16" s="196"/>
       <c r="D16" s="196"/>
@@ -12921,7 +12922,7 @@
     </row>
     <row r="17" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="196" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C17" s="196"/>
       <c r="D17" s="196"/>
@@ -12931,7 +12932,7 @@
     </row>
     <row r="18" spans="2:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="196" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="196"/>
       <c r="D18" s="196"/>
@@ -12941,7 +12942,7 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="196" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="196"/>
       <c r="D19" s="196"/>
@@ -12951,6 +12952,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B6:D6"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
@@ -12958,13 +12966,6 @@
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="IS65533:IS65542 SO65533:SO65542 ACK65533:ACK65542 AMG65533:AMG65542 AWC65533:AWC65542 BFY65533:BFY65542 BPU65533:BPU65542 BZQ65533:BZQ65542 CJM65533:CJM65542 CTI65533:CTI65542 DDE65533:DDE65542 DNA65533:DNA65542 DWW65533:DWW65542 EGS65533:EGS65542 EQO65533:EQO65542 FAK65533:FAK65542 FKG65533:FKG65542 FUC65533:FUC65542 GDY65533:GDY65542 GNU65533:GNU65542 GXQ65533:GXQ65542 HHM65533:HHM65542 HRI65533:HRI65542 IBE65533:IBE65542 ILA65533:ILA65542 IUW65533:IUW65542 JES65533:JES65542 JOO65533:JOO65542 JYK65533:JYK65542 KIG65533:KIG65542 KSC65533:KSC65542 LBY65533:LBY65542 LLU65533:LLU65542 LVQ65533:LVQ65542 MFM65533:MFM65542 MPI65533:MPI65542 MZE65533:MZE65542 NJA65533:NJA65542 NSW65533:NSW65542 OCS65533:OCS65542 OMO65533:OMO65542 OWK65533:OWK65542 PGG65533:PGG65542 PQC65533:PQC65542 PZY65533:PZY65542 QJU65533:QJU65542 QTQ65533:QTQ65542 RDM65533:RDM65542 RNI65533:RNI65542 RXE65533:RXE65542 SHA65533:SHA65542 SQW65533:SQW65542 TAS65533:TAS65542 TKO65533:TKO65542 TUK65533:TUK65542 UEG65533:UEG65542 UOC65533:UOC65542 UXY65533:UXY65542 VHU65533:VHU65542 VRQ65533:VRQ65542 WBM65533:WBM65542 WLI65533:WLI65542 WVE65533:WVE65542 IS131069:IS131078 SO131069:SO131078 ACK131069:ACK131078 AMG131069:AMG131078 AWC131069:AWC131078 BFY131069:BFY131078 BPU131069:BPU131078 BZQ131069:BZQ131078 CJM131069:CJM131078 CTI131069:CTI131078 DDE131069:DDE131078 DNA131069:DNA131078 DWW131069:DWW131078 EGS131069:EGS131078 EQO131069:EQO131078 FAK131069:FAK131078 FKG131069:FKG131078 FUC131069:FUC131078 GDY131069:GDY131078 GNU131069:GNU131078 GXQ131069:GXQ131078 HHM131069:HHM131078 HRI131069:HRI131078 IBE131069:IBE131078 ILA131069:ILA131078 IUW131069:IUW131078 JES131069:JES131078 JOO131069:JOO131078 JYK131069:JYK131078 KIG131069:KIG131078 KSC131069:KSC131078 LBY131069:LBY131078 LLU131069:LLU131078 LVQ131069:LVQ131078 MFM131069:MFM131078 MPI131069:MPI131078 MZE131069:MZE131078 NJA131069:NJA131078 NSW131069:NSW131078 OCS131069:OCS131078 OMO131069:OMO131078 OWK131069:OWK131078 PGG131069:PGG131078 PQC131069:PQC131078 PZY131069:PZY131078 QJU131069:QJU131078 QTQ131069:QTQ131078 RDM131069:RDM131078 RNI131069:RNI131078 RXE131069:RXE131078 SHA131069:SHA131078 SQW131069:SQW131078 TAS131069:TAS131078 TKO131069:TKO131078 TUK131069:TUK131078 UEG131069:UEG131078 UOC131069:UOC131078 UXY131069:UXY131078 VHU131069:VHU131078 VRQ131069:VRQ131078 WBM131069:WBM131078 WLI131069:WLI131078 WVE131069:WVE131078 IS196605:IS196614 SO196605:SO196614 ACK196605:ACK196614 AMG196605:AMG196614 AWC196605:AWC196614 BFY196605:BFY196614 BPU196605:BPU196614 BZQ196605:BZQ196614 CJM196605:CJM196614 CTI196605:CTI196614 DDE196605:DDE196614 DNA196605:DNA196614 DWW196605:DWW196614 EGS196605:EGS196614 EQO196605:EQO196614 FAK196605:FAK196614 FKG196605:FKG196614 FUC196605:FUC196614 GDY196605:GDY196614 GNU196605:GNU196614 GXQ196605:GXQ196614 HHM196605:HHM196614 HRI196605:HRI196614 IBE196605:IBE196614 ILA196605:ILA196614 IUW196605:IUW196614 JES196605:JES196614 JOO196605:JOO196614 JYK196605:JYK196614 KIG196605:KIG196614 KSC196605:KSC196614 LBY196605:LBY196614 LLU196605:LLU196614 LVQ196605:LVQ196614 MFM196605:MFM196614 MPI196605:MPI196614 MZE196605:MZE196614 NJA196605:NJA196614 NSW196605:NSW196614 OCS196605:OCS196614 OMO196605:OMO196614 OWK196605:OWK196614 PGG196605:PGG196614 PQC196605:PQC196614 PZY196605:PZY196614 QJU196605:QJU196614 QTQ196605:QTQ196614 RDM196605:RDM196614 RNI196605:RNI196614 RXE196605:RXE196614 SHA196605:SHA196614 SQW196605:SQW196614 TAS196605:TAS196614 TKO196605:TKO196614 TUK196605:TUK196614 UEG196605:UEG196614 UOC196605:UOC196614 UXY196605:UXY196614 VHU196605:VHU196614 VRQ196605:VRQ196614 WBM196605:WBM196614 WLI196605:WLI196614 WVE196605:WVE196614 IS262141:IS262150 SO262141:SO262150 ACK262141:ACK262150 AMG262141:AMG262150 AWC262141:AWC262150 BFY262141:BFY262150 BPU262141:BPU262150 BZQ262141:BZQ262150 CJM262141:CJM262150 CTI262141:CTI262150 DDE262141:DDE262150 DNA262141:DNA262150 DWW262141:DWW262150 EGS262141:EGS262150 EQO262141:EQO262150 FAK262141:FAK262150 FKG262141:FKG262150 FUC262141:FUC262150 GDY262141:GDY262150 GNU262141:GNU262150 GXQ262141:GXQ262150 HHM262141:HHM262150 HRI262141:HRI262150 IBE262141:IBE262150 ILA262141:ILA262150 IUW262141:IUW262150 JES262141:JES262150 JOO262141:JOO262150 JYK262141:JYK262150 KIG262141:KIG262150 KSC262141:KSC262150 LBY262141:LBY262150 LLU262141:LLU262150 LVQ262141:LVQ262150 MFM262141:MFM262150 MPI262141:MPI262150 MZE262141:MZE262150 NJA262141:NJA262150 NSW262141:NSW262150 OCS262141:OCS262150 OMO262141:OMO262150 OWK262141:OWK262150 PGG262141:PGG262150 PQC262141:PQC262150 PZY262141:PZY262150 QJU262141:QJU262150 QTQ262141:QTQ262150 RDM262141:RDM262150 RNI262141:RNI262150 RXE262141:RXE262150 SHA262141:SHA262150 SQW262141:SQW262150 TAS262141:TAS262150 TKO262141:TKO262150 TUK262141:TUK262150 UEG262141:UEG262150 UOC262141:UOC262150 UXY262141:UXY262150 VHU262141:VHU262150 VRQ262141:VRQ262150 WBM262141:WBM262150 WLI262141:WLI262150 WVE262141:WVE262150 IS327677:IS327686 SO327677:SO327686 ACK327677:ACK327686 AMG327677:AMG327686 AWC327677:AWC327686 BFY327677:BFY327686 BPU327677:BPU327686 BZQ327677:BZQ327686 CJM327677:CJM327686 CTI327677:CTI327686 DDE327677:DDE327686 DNA327677:DNA327686 DWW327677:DWW327686 EGS327677:EGS327686 EQO327677:EQO327686 FAK327677:FAK327686 FKG327677:FKG327686 FUC327677:FUC327686 GDY327677:GDY327686 GNU327677:GNU327686 GXQ327677:GXQ327686 HHM327677:HHM327686 HRI327677:HRI327686 IBE327677:IBE327686 ILA327677:ILA327686 IUW327677:IUW327686 JES327677:JES327686 JOO327677:JOO327686 JYK327677:JYK327686 KIG327677:KIG327686 KSC327677:KSC327686 LBY327677:LBY327686 LLU327677:LLU327686 LVQ327677:LVQ327686 MFM327677:MFM327686 MPI327677:MPI327686 MZE327677:MZE327686 NJA327677:NJA327686 NSW327677:NSW327686 OCS327677:OCS327686 OMO327677:OMO327686 OWK327677:OWK327686 PGG327677:PGG327686 PQC327677:PQC327686 PZY327677:PZY327686 QJU327677:QJU327686 QTQ327677:QTQ327686 RDM327677:RDM327686 RNI327677:RNI327686 RXE327677:RXE327686 SHA327677:SHA327686 SQW327677:SQW327686 TAS327677:TAS327686 TKO327677:TKO327686 TUK327677:TUK327686 UEG327677:UEG327686 UOC327677:UOC327686 UXY327677:UXY327686 VHU327677:VHU327686 VRQ327677:VRQ327686 WBM327677:WBM327686 WLI327677:WLI327686 WVE327677:WVE327686 IS393213:IS393222 SO393213:SO393222 ACK393213:ACK393222 AMG393213:AMG393222 AWC393213:AWC393222 BFY393213:BFY393222 BPU393213:BPU393222 BZQ393213:BZQ393222 CJM393213:CJM393222 CTI393213:CTI393222 DDE393213:DDE393222 DNA393213:DNA393222 DWW393213:DWW393222 EGS393213:EGS393222 EQO393213:EQO393222 FAK393213:FAK393222 FKG393213:FKG393222 FUC393213:FUC393222 GDY393213:GDY393222 GNU393213:GNU393222 GXQ393213:GXQ393222 HHM393213:HHM393222 HRI393213:HRI393222 IBE393213:IBE393222 ILA393213:ILA393222 IUW393213:IUW393222 JES393213:JES393222 JOO393213:JOO393222 JYK393213:JYK393222 KIG393213:KIG393222 KSC393213:KSC393222 LBY393213:LBY393222 LLU393213:LLU393222 LVQ393213:LVQ393222 MFM393213:MFM393222 MPI393213:MPI393222 MZE393213:MZE393222 NJA393213:NJA393222 NSW393213:NSW393222 OCS393213:OCS393222 OMO393213:OMO393222 OWK393213:OWK393222 PGG393213:PGG393222 PQC393213:PQC393222 PZY393213:PZY393222 QJU393213:QJU393222 QTQ393213:QTQ393222 RDM393213:RDM393222 RNI393213:RNI393222 RXE393213:RXE393222 SHA393213:SHA393222 SQW393213:SQW393222 TAS393213:TAS393222 TKO393213:TKO393222 TUK393213:TUK393222 UEG393213:UEG393222 UOC393213:UOC393222 UXY393213:UXY393222 VHU393213:VHU393222 VRQ393213:VRQ393222 WBM393213:WBM393222 WLI393213:WLI393222 WVE393213:WVE393222 IS458749:IS458758 SO458749:SO458758 ACK458749:ACK458758 AMG458749:AMG458758 AWC458749:AWC458758 BFY458749:BFY458758 BPU458749:BPU458758 BZQ458749:BZQ458758 CJM458749:CJM458758 CTI458749:CTI458758 DDE458749:DDE458758 DNA458749:DNA458758 DWW458749:DWW458758 EGS458749:EGS458758 EQO458749:EQO458758 FAK458749:FAK458758 FKG458749:FKG458758 FUC458749:FUC458758 GDY458749:GDY458758 GNU458749:GNU458758 GXQ458749:GXQ458758 HHM458749:HHM458758 HRI458749:HRI458758 IBE458749:IBE458758 ILA458749:ILA458758 IUW458749:IUW458758 JES458749:JES458758 JOO458749:JOO458758 JYK458749:JYK458758 KIG458749:KIG458758 KSC458749:KSC458758 LBY458749:LBY458758 LLU458749:LLU458758 LVQ458749:LVQ458758 MFM458749:MFM458758 MPI458749:MPI458758 MZE458749:MZE458758 NJA458749:NJA458758 NSW458749:NSW458758 OCS458749:OCS458758 OMO458749:OMO458758 OWK458749:OWK458758 PGG458749:PGG458758 PQC458749:PQC458758 PZY458749:PZY458758 QJU458749:QJU458758 QTQ458749:QTQ458758 RDM458749:RDM458758 RNI458749:RNI458758 RXE458749:RXE458758 SHA458749:SHA458758 SQW458749:SQW458758 TAS458749:TAS458758 TKO458749:TKO458758 TUK458749:TUK458758 UEG458749:UEG458758 UOC458749:UOC458758 UXY458749:UXY458758 VHU458749:VHU458758 VRQ458749:VRQ458758 WBM458749:WBM458758 WLI458749:WLI458758 WVE458749:WVE458758 IS524285:IS524294 SO524285:SO524294 ACK524285:ACK524294 AMG524285:AMG524294 AWC524285:AWC524294 BFY524285:BFY524294 BPU524285:BPU524294 BZQ524285:BZQ524294 CJM524285:CJM524294 CTI524285:CTI524294 DDE524285:DDE524294 DNA524285:DNA524294 DWW524285:DWW524294 EGS524285:EGS524294 EQO524285:EQO524294 FAK524285:FAK524294 FKG524285:FKG524294 FUC524285:FUC524294 GDY524285:GDY524294 GNU524285:GNU524294 GXQ524285:GXQ524294 HHM524285:HHM524294 HRI524285:HRI524294 IBE524285:IBE524294 ILA524285:ILA524294 IUW524285:IUW524294 JES524285:JES524294 JOO524285:JOO524294 JYK524285:JYK524294 KIG524285:KIG524294 KSC524285:KSC524294 LBY524285:LBY524294 LLU524285:LLU524294 LVQ524285:LVQ524294 MFM524285:MFM524294 MPI524285:MPI524294 MZE524285:MZE524294 NJA524285:NJA524294 NSW524285:NSW524294 OCS524285:OCS524294 OMO524285:OMO524294 OWK524285:OWK524294 PGG524285:PGG524294 PQC524285:PQC524294 PZY524285:PZY524294 QJU524285:QJU524294 QTQ524285:QTQ524294 RDM524285:RDM524294 RNI524285:RNI524294 RXE524285:RXE524294 SHA524285:SHA524294 SQW524285:SQW524294 TAS524285:TAS524294 TKO524285:TKO524294 TUK524285:TUK524294 UEG524285:UEG524294 UOC524285:UOC524294 UXY524285:UXY524294 VHU524285:VHU524294 VRQ524285:VRQ524294 WBM524285:WBM524294 WLI524285:WLI524294 WVE524285:WVE524294 IS589821:IS589830 SO589821:SO589830 ACK589821:ACK589830 AMG589821:AMG589830 AWC589821:AWC589830 BFY589821:BFY589830 BPU589821:BPU589830 BZQ589821:BZQ589830 CJM589821:CJM589830 CTI589821:CTI589830 DDE589821:DDE589830 DNA589821:DNA589830 DWW589821:DWW589830 EGS589821:EGS589830 EQO589821:EQO589830 FAK589821:FAK589830 FKG589821:FKG589830 FUC589821:FUC589830 GDY589821:GDY589830 GNU589821:GNU589830 GXQ589821:GXQ589830 HHM589821:HHM589830 HRI589821:HRI589830 IBE589821:IBE589830 ILA589821:ILA589830 IUW589821:IUW589830 JES589821:JES589830 JOO589821:JOO589830 JYK589821:JYK589830 KIG589821:KIG589830 KSC589821:KSC589830 LBY589821:LBY589830 LLU589821:LLU589830 LVQ589821:LVQ589830 MFM589821:MFM589830 MPI589821:MPI589830 MZE589821:MZE589830 NJA589821:NJA589830 NSW589821:NSW589830 OCS589821:OCS589830 OMO589821:OMO589830 OWK589821:OWK589830 PGG589821:PGG589830 PQC589821:PQC589830 PZY589821:PZY589830 QJU589821:QJU589830 QTQ589821:QTQ589830 RDM589821:RDM589830 RNI589821:RNI589830 RXE589821:RXE589830 SHA589821:SHA589830 SQW589821:SQW589830 TAS589821:TAS589830 TKO589821:TKO589830 TUK589821:TUK589830 UEG589821:UEG589830 UOC589821:UOC589830 UXY589821:UXY589830 VHU589821:VHU589830 VRQ589821:VRQ589830 WBM589821:WBM589830 WLI589821:WLI589830 WVE589821:WVE589830 IS655357:IS655366 SO655357:SO655366 ACK655357:ACK655366 AMG655357:AMG655366 AWC655357:AWC655366 BFY655357:BFY655366 BPU655357:BPU655366 BZQ655357:BZQ655366 CJM655357:CJM655366 CTI655357:CTI655366 DDE655357:DDE655366 DNA655357:DNA655366 DWW655357:DWW655366 EGS655357:EGS655366 EQO655357:EQO655366 FAK655357:FAK655366 FKG655357:FKG655366 FUC655357:FUC655366 GDY655357:GDY655366 GNU655357:GNU655366 GXQ655357:GXQ655366 HHM655357:HHM655366 HRI655357:HRI655366 IBE655357:IBE655366 ILA655357:ILA655366 IUW655357:IUW655366 JES655357:JES655366 JOO655357:JOO655366 JYK655357:JYK655366 KIG655357:KIG655366 KSC655357:KSC655366 LBY655357:LBY655366 LLU655357:LLU655366 LVQ655357:LVQ655366 MFM655357:MFM655366 MPI655357:MPI655366 MZE655357:MZE655366 NJA655357:NJA655366 NSW655357:NSW655366 OCS655357:OCS655366 OMO655357:OMO655366 OWK655357:OWK655366 PGG655357:PGG655366 PQC655357:PQC655366 PZY655357:PZY655366 QJU655357:QJU655366 QTQ655357:QTQ655366 RDM655357:RDM655366 RNI655357:RNI655366 RXE655357:RXE655366 SHA655357:SHA655366 SQW655357:SQW655366 TAS655357:TAS655366 TKO655357:TKO655366 TUK655357:TUK655366 UEG655357:UEG655366 UOC655357:UOC655366 UXY655357:UXY655366 VHU655357:VHU655366 VRQ655357:VRQ655366 WBM655357:WBM655366 WLI655357:WLI655366 WVE655357:WVE655366 IS720893:IS720902 SO720893:SO720902 ACK720893:ACK720902 AMG720893:AMG720902 AWC720893:AWC720902 BFY720893:BFY720902 BPU720893:BPU720902 BZQ720893:BZQ720902 CJM720893:CJM720902 CTI720893:CTI720902 DDE720893:DDE720902 DNA720893:DNA720902 DWW720893:DWW720902 EGS720893:EGS720902 EQO720893:EQO720902 FAK720893:FAK720902 FKG720893:FKG720902 FUC720893:FUC720902 GDY720893:GDY720902 GNU720893:GNU720902 GXQ720893:GXQ720902 HHM720893:HHM720902 HRI720893:HRI720902 IBE720893:IBE720902 ILA720893:ILA720902 IUW720893:IUW720902 JES720893:JES720902 JOO720893:JOO720902 JYK720893:JYK720902 KIG720893:KIG720902 KSC720893:KSC720902 LBY720893:LBY720902 LLU720893:LLU720902 LVQ720893:LVQ720902 MFM720893:MFM720902 MPI720893:MPI720902 MZE720893:MZE720902 NJA720893:NJA720902 NSW720893:NSW720902 OCS720893:OCS720902 OMO720893:OMO720902 OWK720893:OWK720902 PGG720893:PGG720902 PQC720893:PQC720902 PZY720893:PZY720902 QJU720893:QJU720902 QTQ720893:QTQ720902 RDM720893:RDM720902 RNI720893:RNI720902 RXE720893:RXE720902 SHA720893:SHA720902 SQW720893:SQW720902 TAS720893:TAS720902 TKO720893:TKO720902 TUK720893:TUK720902 UEG720893:UEG720902 UOC720893:UOC720902 UXY720893:UXY720902 VHU720893:VHU720902 VRQ720893:VRQ720902 WBM720893:WBM720902 WLI720893:WLI720902 WVE720893:WVE720902 IS786429:IS786438 SO786429:SO786438 ACK786429:ACK786438 AMG786429:AMG786438 AWC786429:AWC786438 BFY786429:BFY786438 BPU786429:BPU786438 BZQ786429:BZQ786438 CJM786429:CJM786438 CTI786429:CTI786438 DDE786429:DDE786438 DNA786429:DNA786438 DWW786429:DWW786438 EGS786429:EGS786438 EQO786429:EQO786438 FAK786429:FAK786438 FKG786429:FKG786438 FUC786429:FUC786438 GDY786429:GDY786438 GNU786429:GNU786438 GXQ786429:GXQ786438 HHM786429:HHM786438 HRI786429:HRI786438 IBE786429:IBE786438 ILA786429:ILA786438 IUW786429:IUW786438 JES786429:JES786438 JOO786429:JOO786438 JYK786429:JYK786438 KIG786429:KIG786438 KSC786429:KSC786438 LBY786429:LBY786438 LLU786429:LLU786438 LVQ786429:LVQ786438 MFM786429:MFM786438 MPI786429:MPI786438 MZE786429:MZE786438 NJA786429:NJA786438 NSW786429:NSW786438 OCS786429:OCS786438 OMO786429:OMO786438 OWK786429:OWK786438 PGG786429:PGG786438 PQC786429:PQC786438 PZY786429:PZY786438 QJU786429:QJU786438 QTQ786429:QTQ786438 RDM786429:RDM786438 RNI786429:RNI786438 RXE786429:RXE786438 SHA786429:SHA786438 SQW786429:SQW786438 TAS786429:TAS786438 TKO786429:TKO786438 TUK786429:TUK786438 UEG786429:UEG786438 UOC786429:UOC786438 UXY786429:UXY786438 VHU786429:VHU786438 VRQ786429:VRQ786438 WBM786429:WBM786438 WLI786429:WLI786438 WVE786429:WVE786438 IS851965:IS851974 SO851965:SO851974 ACK851965:ACK851974 AMG851965:AMG851974 AWC851965:AWC851974 BFY851965:BFY851974 BPU851965:BPU851974 BZQ851965:BZQ851974 CJM851965:CJM851974 CTI851965:CTI851974 DDE851965:DDE851974 DNA851965:DNA851974 DWW851965:DWW851974 EGS851965:EGS851974 EQO851965:EQO851974 FAK851965:FAK851974 FKG851965:FKG851974 FUC851965:FUC851974 GDY851965:GDY851974 GNU851965:GNU851974 GXQ851965:GXQ851974 HHM851965:HHM851974 HRI851965:HRI851974 IBE851965:IBE851974 ILA851965:ILA851974 IUW851965:IUW851974 JES851965:JES851974 JOO851965:JOO851974 JYK851965:JYK851974 KIG851965:KIG851974 KSC851965:KSC851974 LBY851965:LBY851974 LLU851965:LLU851974 LVQ851965:LVQ851974 MFM851965:MFM851974 MPI851965:MPI851974 MZE851965:MZE851974 NJA851965:NJA851974 NSW851965:NSW851974 OCS851965:OCS851974 OMO851965:OMO851974 OWK851965:OWK851974 PGG851965:PGG851974 PQC851965:PQC851974 PZY851965:PZY851974 QJU851965:QJU851974 QTQ851965:QTQ851974 RDM851965:RDM851974 RNI851965:RNI851974 RXE851965:RXE851974 SHA851965:SHA851974 SQW851965:SQW851974 TAS851965:TAS851974 TKO851965:TKO851974 TUK851965:TUK851974 UEG851965:UEG851974 UOC851965:UOC851974 UXY851965:UXY851974 VHU851965:VHU851974 VRQ851965:VRQ851974 WBM851965:WBM851974 WLI851965:WLI851974 WVE851965:WVE851974 IS917501:IS917510 SO917501:SO917510 ACK917501:ACK917510 AMG917501:AMG917510 AWC917501:AWC917510 BFY917501:BFY917510 BPU917501:BPU917510 BZQ917501:BZQ917510 CJM917501:CJM917510 CTI917501:CTI917510 DDE917501:DDE917510 DNA917501:DNA917510 DWW917501:DWW917510 EGS917501:EGS917510 EQO917501:EQO917510 FAK917501:FAK917510 FKG917501:FKG917510 FUC917501:FUC917510 GDY917501:GDY917510 GNU917501:GNU917510 GXQ917501:GXQ917510 HHM917501:HHM917510 HRI917501:HRI917510 IBE917501:IBE917510 ILA917501:ILA917510 IUW917501:IUW917510 JES917501:JES917510 JOO917501:JOO917510 JYK917501:JYK917510 KIG917501:KIG917510 KSC917501:KSC917510 LBY917501:LBY917510 LLU917501:LLU917510 LVQ917501:LVQ917510 MFM917501:MFM917510 MPI917501:MPI917510 MZE917501:MZE917510 NJA917501:NJA917510 NSW917501:NSW917510 OCS917501:OCS917510 OMO917501:OMO917510 OWK917501:OWK917510 PGG917501:PGG917510 PQC917501:PQC917510 PZY917501:PZY917510 QJU917501:QJU917510 QTQ917501:QTQ917510 RDM917501:RDM917510 RNI917501:RNI917510 RXE917501:RXE917510 SHA917501:SHA917510 SQW917501:SQW917510 TAS917501:TAS917510 TKO917501:TKO917510 TUK917501:TUK917510 UEG917501:UEG917510 UOC917501:UOC917510 UXY917501:UXY917510 VHU917501:VHU917510 VRQ917501:VRQ917510 WBM917501:WBM917510 WLI917501:WLI917510 WVE917501:WVE917510 IS983037:IS983046 SO983037:SO983046 ACK983037:ACK983046 AMG983037:AMG983046 AWC983037:AWC983046 BFY983037:BFY983046 BPU983037:BPU983046 BZQ983037:BZQ983046 CJM983037:CJM983046 CTI983037:CTI983046 DDE983037:DDE983046 DNA983037:DNA983046 DWW983037:DWW983046 EGS983037:EGS983046 EQO983037:EQO983046 FAK983037:FAK983046 FKG983037:FKG983046 FUC983037:FUC983046 GDY983037:GDY983046 GNU983037:GNU983046 GXQ983037:GXQ983046 HHM983037:HHM983046 HRI983037:HRI983046 IBE983037:IBE983046 ILA983037:ILA983046 IUW983037:IUW983046 JES983037:JES983046 JOO983037:JOO983046 JYK983037:JYK983046 KIG983037:KIG983046 KSC983037:KSC983046 LBY983037:LBY983046 LLU983037:LLU983046 LVQ983037:LVQ983046 MFM983037:MFM983046 MPI983037:MPI983046 MZE983037:MZE983046 NJA983037:NJA983046 NSW983037:NSW983046 OCS983037:OCS983046 OMO983037:OMO983046 OWK983037:OWK983046 PGG983037:PGG983046 PQC983037:PQC983046 PZY983037:PZY983046 QJU983037:QJU983046 QTQ983037:QTQ983046 RDM983037:RDM983046 RNI983037:RNI983046 RXE983037:RXE983046 SHA983037:SHA983046 SQW983037:SQW983046 TAS983037:TAS983046 TKO983037:TKO983046 TUK983037:TUK983046 UEG983037:UEG983046 UOC983037:UOC983046 UXY983037:UXY983046 VHU983037:VHU983046 VRQ983037:VRQ983046 WBM983037:WBM983046 WLI983037:WLI983046 WVE983037:WVE983046 SO5:SO8 ACK5:ACK8 AMG5:AMG8 AWC5:AWC8 BFY5:BFY8 BPU5:BPU8 BZQ5:BZQ8 CJM5:CJM8 CTI5:CTI8 DDE5:DDE8 DNA5:DNA8 DWW5:DWW8 EGS5:EGS8 EQO5:EQO8 FAK5:FAK8 FKG5:FKG8 FUC5:FUC8 GDY5:GDY8 GNU5:GNU8 GXQ5:GXQ8 HHM5:HHM8 HRI5:HRI8 IBE5:IBE8 ILA5:ILA8 IUW5:IUW8 JES5:JES8 JOO5:JOO8 JYK5:JYK8 KIG5:KIG8 KSC5:KSC8 LBY5:LBY8 LLU5:LLU8 LVQ5:LVQ8 MFM5:MFM8 MPI5:MPI8 MZE5:MZE8 NJA5:NJA8 NSW5:NSW8 OCS5:OCS8 OMO5:OMO8 OWK5:OWK8 PGG5:PGG8 PQC5:PQC8 PZY5:PZY8 QJU5:QJU8 QTQ5:QTQ8 RDM5:RDM8 RNI5:RNI8 RXE5:RXE8 SHA5:SHA8 SQW5:SQW8 TAS5:TAS8 TKO5:TKO8 TUK5:TUK8 UEG5:UEG8 UOC5:UOC8 UXY5:UXY8 VHU5:VHU8 VRQ5:VRQ8 WBM5:WBM8 WLI5:WLI8 WVE5:WVE8 IS5:IS8 SO15:SO18 ACK15:ACK18 AMG15:AMG18 AWC15:AWC18 BFY15:BFY18 BPU15:BPU18 BZQ15:BZQ18 CJM15:CJM18 CTI15:CTI18 DDE15:DDE18 DNA15:DNA18 DWW15:DWW18 EGS15:EGS18 EQO15:EQO18 FAK15:FAK18 FKG15:FKG18 FUC15:FUC18 GDY15:GDY18 GNU15:GNU18 GXQ15:GXQ18 HHM15:HHM18 HRI15:HRI18 IBE15:IBE18 ILA15:ILA18 IUW15:IUW18 JES15:JES18 JOO15:JOO18 JYK15:JYK18 KIG15:KIG18 KSC15:KSC18 LBY15:LBY18 LLU15:LLU18 LVQ15:LVQ18 MFM15:MFM18 MPI15:MPI18 MZE15:MZE18 NJA15:NJA18 NSW15:NSW18 OCS15:OCS18 OMO15:OMO18 OWK15:OWK18 PGG15:PGG18 PQC15:PQC18 PZY15:PZY18 QJU15:QJU18 QTQ15:QTQ18 RDM15:RDM18 RNI15:RNI18 RXE15:RXE18 SHA15:SHA18 SQW15:SQW18 TAS15:TAS18 TKO15:TKO18 TUK15:TUK18 UEG15:UEG18 UOC15:UOC18 UXY15:UXY18 VHU15:VHU18 VRQ15:VRQ18 WBM15:WBM18 WLI15:WLI18 WVE15:WVE18 IS15:IS18">

</xml_diff>